<commit_message>
Missing fuel supplies for power added to SUP
</commit_message>
<xml_diff>
--- a/VT_REGION1_SUP.xlsx
+++ b/VT_REGION1_SUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EB40BB-56E7-453D-8DD5-51179F1F2240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A8038F-7128-4D70-91CD-CB2F4C624EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="12" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="12" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -223,6 +223,7 @@
     <author>tc={54934D05-AB8B-43EA-94D5-DA4230739148}</author>
     <author>tc={2D025629-877F-4A51-97DF-4B63BC17F90B}</author>
     <author>tc={00B9291C-0286-423F-9703-F64CCB57F70F}</author>
+    <author>tc={87179AE4-EC17-4370-98D7-F32C73BD771A}</author>
     <author>tc={6A82080C-3A46-4F98-A8BB-1FF2F957BEF2}</author>
     <author>tc={E56230BC-BD11-4915-915B-9473750B9EC2}</author>
   </authors>
@@ -669,7 +670,15 @@
         </r>
       </text>
     </comment>
-    <comment ref="K89" authorId="9" shapeId="0" xr:uid="{6A82080C-3A46-4F98-A8BB-1FF2F957BEF2}">
+    <comment ref="F83" authorId="9" shapeId="0" xr:uid="{87179AE4-EC17-4370-98D7-F32C73BD771A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    IRP 2019 costs adjusted to 2022</t>
+      </text>
+    </comment>
+    <comment ref="K89" authorId="10" shapeId="0" xr:uid="{6A82080C-3A46-4F98-A8BB-1FF2F957BEF2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -677,7 +686,7 @@
     .56 added to avoid zzs</t>
       </text>
     </comment>
-    <comment ref="F95" authorId="10" shapeId="0" xr:uid="{E56230BC-BD11-4915-915B-9473750B9EC2}">
+    <comment ref="F95" authorId="11" shapeId="0" xr:uid="{E56230BC-BD11-4915-915B-9473750B9EC2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1587,7 +1596,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2626" uniqueCount="1116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2668" uniqueCount="1116">
   <si>
     <t>Agriculture</t>
   </si>
@@ -6570,7 +6579,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="172" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6605,6 +6614,7 @@
     <xf numFmtId="183" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="452">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -7378,6 +7388,57 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7417,57 +7478,6 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7484,7 +7494,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="27">
     <cellStyle name="Accent2" xfId="10" builtinId="33"/>
     <cellStyle name="Accent4" xfId="11" builtinId="41"/>
     <cellStyle name="Bad" xfId="6" builtinId="27"/>
@@ -7509,6 +7519,7 @@
     <cellStyle name="Normal 13" xfId="20" xr:uid="{E2592950-4ED9-41AE-B126-E7C61CACE4FB}"/>
     <cellStyle name="Normal 2" xfId="12" xr:uid="{07540C44-1236-4F52-ADF2-28F7197333C4}"/>
     <cellStyle name="Normal 2 2" xfId="19" xr:uid="{9E14FE11-A3BB-42F9-9021-8042EAB56468}"/>
+    <cellStyle name="Normal 7" xfId="26" xr:uid="{ABB2DBC2-F744-4899-96E1-16AACB0FB8DE}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="17" xr:uid="{DEC93E5C-1EDF-4DE0-98A7-4B3BFAC40E98}"/>
   </cellStyles>
@@ -24799,6 +24810,9 @@
   <threadedComment ref="F70" dT="2023-08-14T09:42:24.18" personId="{8B1FB5F6-C05B-4C45-A9FE-3B209CC95A5D}" id="{00B9291C-0286-423F-9703-F64CCB57F70F}">
     <text>Parity with coal in R/GJ assumed</text>
   </threadedComment>
+  <threadedComment ref="F83" dT="2023-09-07T10:07:04.92" personId="{8B1FB5F6-C05B-4C45-A9FE-3B209CC95A5D}" id="{87179AE4-EC17-4370-98D7-F32C73BD771A}">
+    <text>IRP 2019 costs adjusted to 2022</text>
+  </threadedComment>
   <threadedComment ref="K89" dT="2021-07-26T15:05:55.74" personId="{E500B1BD-2FF0-4DFA-88F6-72D20CDE0583}" id="{6A82080C-3A46-4F98-A8BB-1FF2F957BEF2}">
     <text>.56 added to avoid zzs</text>
   </threadedComment>
@@ -27995,25 +28009,25 @@
       <c r="W6" s="177" t="s">
         <v>373</v>
       </c>
-      <c r="AC6" s="418" t="s">
+      <c r="AC6" s="435" t="s">
         <v>374</v>
       </c>
-      <c r="AD6" s="418"/>
-      <c r="AE6" s="418"/>
+      <c r="AD6" s="435"/>
+      <c r="AE6" s="435"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="419" t="s">
+      <c r="A7" s="436" t="s">
         <v>375</v>
       </c>
-      <c r="B7" s="421" t="s">
+      <c r="B7" s="438" t="s">
         <v>376</v>
       </c>
-      <c r="C7" s="423" t="s">
+      <c r="C7" s="440" t="s">
         <v>377</v>
       </c>
-      <c r="D7" s="424"/>
-      <c r="E7" s="425"/>
-      <c r="F7" s="428" t="s">
+      <c r="D7" s="441"/>
+      <c r="E7" s="442"/>
+      <c r="F7" s="445" t="s">
         <v>378</v>
       </c>
       <c r="G7" s="178"/>
@@ -28041,12 +28055,12 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="420"/>
-      <c r="B8" s="422"/>
-      <c r="C8" s="426"/>
-      <c r="D8" s="427"/>
-      <c r="E8" s="427"/>
-      <c r="F8" s="429"/>
+      <c r="A8" s="437"/>
+      <c r="B8" s="439"/>
+      <c r="C8" s="443"/>
+      <c r="D8" s="444"/>
+      <c r="E8" s="444"/>
+      <c r="F8" s="446"/>
       <c r="G8" s="178"/>
       <c r="H8" s="178"/>
       <c r="I8" s="178"/>
@@ -28912,11 +28926,11 @@
       <c r="I25" s="57"/>
       <c r="J25" s="57"/>
       <c r="V25" s="219"/>
-      <c r="AC25" s="417" t="s">
+      <c r="AC25" s="434" t="s">
         <v>444</v>
       </c>
-      <c r="AD25" s="417"/>
-      <c r="AE25" s="417"/>
+      <c r="AD25" s="434"/>
+      <c r="AE25" s="434"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C26" s="57"/>
@@ -28995,8 +29009,8 @@
       <c r="D30" s="57"/>
     </row>
     <row r="31" spans="1:31" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H31" s="437"/>
-      <c r="I31" s="437"/>
+      <c r="H31" s="430"/>
+      <c r="I31" s="430"/>
       <c r="R31" t="s">
         <v>382</v>
       </c>
@@ -29017,10 +29031,10 @@
       </c>
     </row>
     <row r="32" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L32" s="430" t="s">
+      <c r="L32" s="422" t="s">
         <v>448</v>
       </c>
-      <c r="M32" s="438" t="s">
+      <c r="M32" s="431" t="s">
         <v>449</v>
       </c>
       <c r="N32" s="222" t="s">
@@ -29035,22 +29049,22 @@
       <c r="Q32" s="225" t="s">
         <v>451</v>
       </c>
-      <c r="R32" s="430" t="s">
+      <c r="R32" s="422" t="s">
         <v>401</v>
       </c>
-      <c r="S32" s="430" t="s">
+      <c r="S32" s="422" t="s">
         <v>405</v>
       </c>
-      <c r="T32" s="430" t="s">
+      <c r="T32" s="422" t="s">
         <v>452</v>
       </c>
-      <c r="U32" s="430" t="s">
+      <c r="U32" s="422" t="s">
         <v>401</v>
       </c>
-      <c r="V32" s="430" t="s">
+      <c r="V32" s="422" t="s">
         <v>405</v>
       </c>
-      <c r="W32" s="430" t="s">
+      <c r="W32" s="422" t="s">
         <v>452</v>
       </c>
     </row>
@@ -29073,28 +29087,28 @@
       <c r="G33" s="142" t="s">
         <v>456</v>
       </c>
-      <c r="H33" s="433" t="s">
+      <c r="H33" s="429" t="s">
         <v>457</v>
       </c>
-      <c r="I33" s="433"/>
+      <c r="I33" s="429"/>
       <c r="J33" s="142" t="s">
         <v>455</v>
       </c>
       <c r="K33" t="s">
         <v>456</v>
       </c>
-      <c r="L33" s="431"/>
-      <c r="M33" s="439"/>
+      <c r="L33" s="423"/>
+      <c r="M33" s="432"/>
       <c r="N33" s="16"/>
       <c r="O33" s="73"/>
       <c r="P33" s="73"/>
       <c r="Q33" s="226"/>
-      <c r="R33" s="431"/>
-      <c r="S33" s="431"/>
-      <c r="T33" s="431"/>
-      <c r="U33" s="431"/>
-      <c r="V33" s="431"/>
-      <c r="W33" s="431"/>
+      <c r="R33" s="423"/>
+      <c r="S33" s="423"/>
+      <c r="T33" s="423"/>
+      <c r="U33" s="423"/>
+      <c r="V33" s="423"/>
+      <c r="W33" s="423"/>
     </row>
     <row r="34" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -29114,8 +29128,8 @@
       <c r="K34" t="s">
         <v>459</v>
       </c>
-      <c r="L34" s="432"/>
-      <c r="M34" s="440"/>
+      <c r="L34" s="424"/>
+      <c r="M34" s="433"/>
       <c r="N34" s="227" t="s">
         <v>461</v>
       </c>
@@ -29128,12 +29142,12 @@
       <c r="Q34" s="229" t="s">
         <v>461</v>
       </c>
-      <c r="R34" s="432"/>
-      <c r="S34" s="432"/>
-      <c r="T34" s="432"/>
-      <c r="U34" s="432"/>
-      <c r="V34" s="432"/>
-      <c r="W34" s="432"/>
+      <c r="R34" s="424"/>
+      <c r="S34" s="424"/>
+      <c r="T34" s="424"/>
+      <c r="U34" s="424"/>
+      <c r="V34" s="424"/>
+      <c r="W34" s="424"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="230" t="s">
@@ -29199,7 +29213,7 @@
         <v>2.9</v>
       </c>
       <c r="I36" s="239"/>
-      <c r="L36" s="434" t="str">
+      <c r="L36" s="425" t="str">
         <f>A36</f>
         <v>Well completion</v>
       </c>
@@ -29279,7 +29293,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="I37" s="239"/>
-      <c r="L37" s="435"/>
+      <c r="L37" s="426"/>
       <c r="M37" t="str">
         <f t="shared" ref="M37:M45" si="5">B37</f>
         <v>Jiang et al. (2011)</v>
@@ -29350,7 +29364,7 @@
         <v>7.8</v>
       </c>
       <c r="I38" s="239"/>
-      <c r="L38" s="435"/>
+      <c r="L38" s="426"/>
       <c r="M38" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -29425,7 +29439,7 @@
       </c>
       <c r="I39" s="239"/>
       <c r="K39" s="239"/>
-      <c r="L39" s="435"/>
+      <c r="L39" s="426"/>
       <c r="M39" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -29496,7 +29510,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="I40" s="239"/>
-      <c r="L40" s="435"/>
+      <c r="L40" s="426"/>
       <c r="M40" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -29570,7 +29584,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="I41" s="239"/>
-      <c r="L41" s="436"/>
+      <c r="L41" s="427"/>
       <c r="M41" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Broderick et al. (2011)</v>
@@ -29644,7 +29658,7 @@
         <v>4.2</v>
       </c>
       <c r="I42" s="239"/>
-      <c r="L42" s="434" t="s">
+      <c r="L42" s="425" t="s">
         <v>425</v>
       </c>
       <c r="M42" s="224" t="str">
@@ -29717,7 +29731,7 @@
         <v>3.5</v>
       </c>
       <c r="I43" s="239"/>
-      <c r="L43" s="435"/>
+      <c r="L43" s="426"/>
       <c r="M43" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -29793,7 +29807,7 @@
       </c>
       <c r="I44" s="239"/>
       <c r="K44" s="239"/>
-      <c r="L44" s="435"/>
+      <c r="L44" s="426"/>
       <c r="M44" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -29865,7 +29879,7 @@
         <v>8.9</v>
       </c>
       <c r="I45" s="239"/>
-      <c r="L45" s="436"/>
+      <c r="L45" s="427"/>
       <c r="M45" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -29934,7 +29948,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="239"/>
-      <c r="L46" s="434" t="str">
+      <c r="L46" s="425" t="str">
         <f>A47</f>
         <v>Transport, storage and distribution</v>
       </c>
@@ -30010,7 +30024,7 @@
         <v>1.9</v>
       </c>
       <c r="I47" s="239"/>
-      <c r="L47" s="435"/>
+      <c r="L47" s="426"/>
       <c r="M47" t="str">
         <f>B48</f>
         <v>Skone et al. (2011)</v>
@@ -30081,7 +30095,7 @@
         <v>2.7</v>
       </c>
       <c r="I48" s="239"/>
-      <c r="L48" s="436"/>
+      <c r="L48" s="427"/>
       <c r="M48" s="95" t="str">
         <f>B49</f>
         <v>Howarth et al. (2011)</v>
@@ -30450,10 +30464,10 @@
       <c r="C79" s="8" t="s">
         <v>509</v>
       </c>
-      <c r="D79" s="446" t="s">
+      <c r="D79" s="428" t="s">
         <v>510</v>
       </c>
-      <c r="E79" s="446"/>
+      <c r="E79" s="428"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
@@ -30555,13 +30569,13 @@
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="441" t="s">
+      <c r="A103" s="417" t="s">
         <v>520</v>
       </c>
       <c r="B103" s="268" t="s">
         <v>521</v>
       </c>
-      <c r="C103" s="443" t="s">
+      <c r="C103" s="419" t="s">
         <v>522</v>
       </c>
       <c r="D103" s="268">
@@ -30572,11 +30586,11 @@
       </c>
     </row>
     <row r="104" spans="1:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="442"/>
+      <c r="A104" s="418"/>
       <c r="B104" s="268" t="s">
         <v>523</v>
       </c>
-      <c r="C104" s="444"/>
+      <c r="C104" s="420"/>
       <c r="D104" s="268">
         <v>0.18</v>
       </c>
@@ -30589,13 +30603,13 @@
       </c>
     </row>
     <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="441" t="s">
+      <c r="A105" s="417" t="s">
         <v>524</v>
       </c>
       <c r="B105" s="268" t="s">
         <v>525</v>
       </c>
-      <c r="C105" s="444"/>
+      <c r="C105" s="420"/>
       <c r="D105" s="268">
         <v>0</v>
       </c>
@@ -30604,11 +30618,11 @@
       </c>
     </row>
     <row r="106" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="442"/>
+      <c r="A106" s="418"/>
       <c r="B106" s="268" t="s">
         <v>526</v>
       </c>
-      <c r="C106" s="445"/>
+      <c r="C106" s="421"/>
       <c r="D106" s="268">
         <v>0</v>
       </c>
@@ -30617,13 +30631,13 @@
       </c>
     </row>
     <row r="107" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="441" t="s">
+      <c r="A107" s="417" t="s">
         <v>520</v>
       </c>
       <c r="B107" s="268" t="s">
         <v>525</v>
       </c>
-      <c r="C107" s="443" t="s">
+      <c r="C107" s="419" t="s">
         <v>527</v>
       </c>
       <c r="D107" s="268">
@@ -30634,11 +30648,11 @@
       </c>
     </row>
     <row r="108" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="442"/>
+      <c r="A108" s="418"/>
       <c r="B108" s="268" t="s">
         <v>526</v>
       </c>
-      <c r="C108" s="444"/>
+      <c r="C108" s="420"/>
       <c r="D108" s="268">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -30647,13 +30661,13 @@
       </c>
     </row>
     <row r="109" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="441" t="s">
+      <c r="A109" s="417" t="s">
         <v>524</v>
       </c>
       <c r="B109" s="268" t="s">
         <v>525</v>
       </c>
-      <c r="C109" s="444"/>
+      <c r="C109" s="420"/>
       <c r="D109" s="268">
         <v>0</v>
       </c>
@@ -30662,11 +30676,11 @@
       </c>
     </row>
     <row r="110" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="442"/>
+      <c r="A110" s="418"/>
       <c r="B110" s="268" t="s">
         <v>526</v>
       </c>
-      <c r="C110" s="445"/>
+      <c r="C110" s="421"/>
       <c r="D110" s="268">
         <v>0</v>
       </c>
@@ -32129,6 +32143,22 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="AC25:AE25"/>
+    <mergeCell ref="AC6:AE6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="W32:W34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="L36:L41"/>
+    <mergeCell ref="L42:L45"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="L32:L34"/>
+    <mergeCell ref="M32:M34"/>
+    <mergeCell ref="R32:R34"/>
+    <mergeCell ref="S32:S34"/>
+    <mergeCell ref="T32:T34"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="C107:C110"/>
     <mergeCell ref="A109:A110"/>
@@ -32139,22 +32169,6 @@
     <mergeCell ref="A103:A104"/>
     <mergeCell ref="C103:C106"/>
     <mergeCell ref="A105:A106"/>
-    <mergeCell ref="W32:W34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="L36:L41"/>
-    <mergeCell ref="L42:L45"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="L32:L34"/>
-    <mergeCell ref="M32:M34"/>
-    <mergeCell ref="R32:R34"/>
-    <mergeCell ref="S32:S34"/>
-    <mergeCell ref="T32:T34"/>
-    <mergeCell ref="AC25:AE25"/>
-    <mergeCell ref="AC6:AE6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -32905,8 +32919,8 @@
   </sheetPr>
   <dimension ref="A1:AE114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -36818,22 +36832,442 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" t="s">
+        <v>220</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" ref="D61:D66" si="40">B61&amp;C61</f>
+        <v>PWRSOL</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" ref="E61:E66" si="41">INDEX(SectorNamesLong,MATCH(B61,SectorNamesShort,0))&amp;" "&amp;INDEX(FuelNamesLong,MATCH(C61,FuelNamesShort,0))</f>
+        <v>Power Solar</v>
+      </c>
+      <c r="F61" t="s">
+        <v>241</v>
+      </c>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61"/>
+      <c r="J61"/>
+      <c r="K61" t="str">
+        <f t="shared" ref="K61:K66" si="42">"X"&amp;D61</f>
+        <v>XPWRSOL</v>
+      </c>
+      <c r="L61" t="str">
+        <f t="shared" ref="L61:L66" si="43">E61</f>
+        <v>Power Solar</v>
+      </c>
+      <c r="M61" t="s">
+        <v>241</v>
+      </c>
+      <c r="N61" t="s">
+        <v>440</v>
+      </c>
+      <c r="O61" t="s">
+        <v>369</v>
+      </c>
+      <c r="P61" t="s">
+        <v>619</v>
+      </c>
+      <c r="Q61"/>
+      <c r="R61"/>
+      <c r="S61" t="str">
+        <f t="shared" ref="S61:S66" si="44">K61</f>
+        <v>XPWRSOL</v>
+      </c>
+      <c r="T61" t="str">
+        <f t="shared" ref="T61:T66" si="45">C61</f>
+        <v>SOL</v>
+      </c>
+      <c r="U61" t="str">
+        <f t="shared" ref="U61:U66" si="46">D61</f>
+        <v>PWRSOL</v>
+      </c>
+      <c r="V61">
+        <v>1</v>
+      </c>
+      <c r="W61">
+        <v>60</v>
+      </c>
+      <c r="X61"/>
+      <c r="Y61">
+        <v>1</v>
+      </c>
+      <c r="Z61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>222</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="40"/>
+        <v>PWRWND</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="41"/>
+        <v>Power Wind</v>
+      </c>
+      <c r="F62" t="s">
+        <v>241</v>
+      </c>
+      <c r="G62"/>
+      <c r="H62"/>
+      <c r="I62"/>
+      <c r="J62"/>
+      <c r="K62" t="str">
+        <f t="shared" si="42"/>
+        <v>XPWRWND</v>
+      </c>
+      <c r="L62" t="str">
+        <f t="shared" si="43"/>
+        <v>Power Wind</v>
+      </c>
+      <c r="M62" t="s">
+        <v>241</v>
+      </c>
+      <c r="N62" t="s">
+        <v>440</v>
+      </c>
+      <c r="O62" t="s">
+        <v>369</v>
+      </c>
+      <c r="P62" t="s">
+        <v>619</v>
+      </c>
+      <c r="Q62"/>
+      <c r="R62"/>
+      <c r="S62" t="str">
+        <f t="shared" si="44"/>
+        <v>XPWRWND</v>
+      </c>
+      <c r="T62" t="str">
+        <f t="shared" si="45"/>
+        <v>WND</v>
+      </c>
+      <c r="U62" t="str">
+        <f t="shared" si="46"/>
+        <v>PWRWND</v>
+      </c>
+      <c r="V62">
+        <v>1</v>
+      </c>
+      <c r="W62">
+        <v>60</v>
+      </c>
+      <c r="X62"/>
+      <c r="Y62">
+        <v>1</v>
+      </c>
+      <c r="Z62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" t="s">
+        <v>198</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="40"/>
+        <v>PWRHYD</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="41"/>
+        <v>Power Hydro</v>
+      </c>
+      <c r="F63" t="s">
+        <v>241</v>
+      </c>
+      <c r="G63"/>
+      <c r="H63"/>
+      <c r="I63"/>
+      <c r="J63"/>
+      <c r="K63" t="str">
+        <f t="shared" si="42"/>
+        <v>XPWRHYD</v>
+      </c>
+      <c r="L63" t="str">
+        <f t="shared" si="43"/>
+        <v>Power Hydro</v>
+      </c>
+      <c r="M63" t="s">
+        <v>241</v>
+      </c>
+      <c r="N63" t="s">
+        <v>440</v>
+      </c>
+      <c r="O63" t="s">
+        <v>369</v>
+      </c>
+      <c r="P63" t="s">
+        <v>619</v>
+      </c>
+      <c r="Q63"/>
+      <c r="R63"/>
+      <c r="S63" t="str">
+        <f t="shared" si="44"/>
+        <v>XPWRHYD</v>
+      </c>
+      <c r="T63" t="str">
+        <f t="shared" si="45"/>
+        <v>HYD</v>
+      </c>
+      <c r="U63" t="str">
+        <f t="shared" si="46"/>
+        <v>PWRHYD</v>
+      </c>
+      <c r="V63">
+        <v>1</v>
+      </c>
+      <c r="W63">
+        <v>60</v>
+      </c>
+      <c r="X63"/>
+      <c r="Y63">
+        <v>1</v>
+      </c>
+      <c r="Z63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" t="s">
+        <v>154</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="40"/>
+        <v>PWRBIO</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="41"/>
+        <v>Power Biomass Other</v>
+      </c>
+      <c r="F64" t="s">
+        <v>241</v>
+      </c>
+      <c r="G64"/>
+      <c r="H64"/>
+      <c r="I64"/>
+      <c r="J64"/>
+      <c r="K64" t="str">
+        <f t="shared" si="42"/>
+        <v>XPWRBIO</v>
+      </c>
+      <c r="L64" t="str">
+        <f t="shared" si="43"/>
+        <v>Power Biomass Other</v>
+      </c>
+      <c r="M64" t="s">
+        <v>241</v>
+      </c>
+      <c r="N64" t="s">
+        <v>440</v>
+      </c>
+      <c r="O64" t="s">
+        <v>369</v>
+      </c>
+      <c r="P64" t="s">
+        <v>619</v>
+      </c>
+      <c r="Q64"/>
+      <c r="R64"/>
+      <c r="S64" t="str">
+        <f t="shared" si="44"/>
+        <v>XPWRBIO</v>
+      </c>
+      <c r="T64" t="str">
+        <f t="shared" si="45"/>
+        <v>BIO</v>
+      </c>
+      <c r="U64" t="str">
+        <f t="shared" si="46"/>
+        <v>PWRBIO</v>
+      </c>
+      <c r="V64">
+        <v>1</v>
+      </c>
+      <c r="W64">
+        <v>60</v>
+      </c>
+      <c r="X64"/>
+      <c r="Y64">
+        <v>1</v>
+      </c>
+      <c r="Z64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" t="s">
+        <v>202</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="40"/>
+        <v>PWRNUC</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="41"/>
+        <v>Power Nuclear</v>
+      </c>
+      <c r="F65" t="s">
+        <v>241</v>
+      </c>
+      <c r="G65"/>
+      <c r="H65"/>
+      <c r="I65"/>
+      <c r="J65"/>
+      <c r="K65" t="str">
+        <f t="shared" si="42"/>
+        <v>XPWRNUC</v>
+      </c>
+      <c r="L65" t="str">
+        <f t="shared" si="43"/>
+        <v>Power Nuclear</v>
+      </c>
+      <c r="M65" t="s">
+        <v>241</v>
+      </c>
+      <c r="N65" t="s">
+        <v>440</v>
+      </c>
+      <c r="O65" t="s">
+        <v>369</v>
+      </c>
+      <c r="P65" t="s">
+        <v>619</v>
+      </c>
+      <c r="Q65"/>
+      <c r="R65"/>
+      <c r="S65" t="str">
+        <f t="shared" si="44"/>
+        <v>XPWRNUC</v>
+      </c>
+      <c r="T65" t="str">
+        <f t="shared" si="45"/>
+        <v>NUC</v>
+      </c>
+      <c r="U65" t="str">
+        <f t="shared" si="46"/>
+        <v>PWRNUC</v>
+      </c>
+      <c r="V65">
+        <v>1</v>
+      </c>
+      <c r="W65">
+        <v>60</v>
+      </c>
+      <c r="X65"/>
+      <c r="Y65">
+        <v>1</v>
+      </c>
+      <c r="Z65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" t="s">
+        <v>164</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="40"/>
+        <v>PWRCLE</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="41"/>
+        <v>Power Coal low grade</v>
+      </c>
+      <c r="F66" t="s">
+        <v>241</v>
+      </c>
+      <c r="G66"/>
+      <c r="H66"/>
+      <c r="I66"/>
+      <c r="J66"/>
+      <c r="K66" t="str">
+        <f t="shared" si="42"/>
+        <v>XPWRCLE</v>
+      </c>
+      <c r="L66" t="str">
+        <f t="shared" si="43"/>
+        <v>Power Coal low grade</v>
+      </c>
+      <c r="M66" t="s">
+        <v>241</v>
+      </c>
+      <c r="N66" t="s">
+        <v>440</v>
+      </c>
+      <c r="O66" t="s">
+        <v>369</v>
+      </c>
+      <c r="P66" t="s">
+        <v>619</v>
+      </c>
+      <c r="Q66"/>
+      <c r="R66"/>
+      <c r="S66" t="str">
+        <f t="shared" si="44"/>
+        <v>XPWRCLE</v>
+      </c>
+      <c r="T66" t="str">
+        <f t="shared" si="45"/>
+        <v>CLE</v>
+      </c>
+      <c r="U66" t="str">
+        <f t="shared" si="46"/>
+        <v>PWRCLE</v>
+      </c>
+      <c r="V66">
+        <v>1</v>
+      </c>
+      <c r="W66">
+        <v>60</v>
+      </c>
+      <c r="X66"/>
+      <c r="Y66">
+        <v>1</v>
+      </c>
+      <c r="Z66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:26" ht="15" x14ac:dyDescent="0.25">
       <c r="B75"/>
     </row>
-    <row r="76" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:26" ht="15" x14ac:dyDescent="0.25">
       <c r="B76"/>
     </row>
-    <row r="77" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:26" ht="15" x14ac:dyDescent="0.25">
       <c r="B77"/>
     </row>
-    <row r="78" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:26" ht="15" x14ac:dyDescent="0.25">
       <c r="B78"/>
     </row>
-    <row r="79" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:26" ht="15" x14ac:dyDescent="0.25">
       <c r="B79"/>
     </row>
-    <row r="80" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:26" ht="15" x14ac:dyDescent="0.25">
       <c r="B80"/>
     </row>
     <row r="81" spans="2:2" ht="15" x14ac:dyDescent="0.25">
@@ -52138,18 +52572,18 @@
         <f>FORECAST(CR93,CP94:CQ94,CP93:CQ93)</f>
         <v>93</v>
       </c>
-      <c r="DL94" s="433" t="s">
+      <c r="DL94" s="429" t="s">
         <v>774</v>
       </c>
-      <c r="DM94" s="433"/>
-      <c r="DN94" s="433" t="s">
+      <c r="DM94" s="429"/>
+      <c r="DN94" s="429" t="s">
         <v>775</v>
       </c>
-      <c r="DO94" s="433"/>
-      <c r="DP94" s="433" t="s">
+      <c r="DO94" s="429"/>
+      <c r="DP94" s="429" t="s">
         <v>773</v>
       </c>
-      <c r="DQ94" s="433"/>
+      <c r="DQ94" s="429"/>
     </row>
     <row r="95" spans="1:121" x14ac:dyDescent="0.25">
       <c r="BK95" t="s">
@@ -57610,7 +58044,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="18">
         <f ca="1">NOW()</f>
-        <v>45163.415417939817</v>
+        <v>45176.505910532411</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -58434,7 +58868,7 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
         <f ca="1">NOW()</f>
-        <v>45163.415417939817</v>
+        <v>45176.505910532411</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -59132,67 +59566,67 @@
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C70" s="30">
-        <f>COUNTIF($C$5:$C$46,C5)</f>
+        <f t="shared" ref="C70:C80" si="1">COUNTIF($C$5:$C$46,C5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C71" s="30">
-        <f>COUNTIF($C$5:$C$46,C6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C72" s="30">
-        <f>COUNTIF($C$5:$C$46,C7)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C73" s="30">
-        <f>COUNTIF($C$5:$C$46,C8)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C74" s="30">
-        <f>COUNTIF($C$5:$C$46,C9)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C75" s="30">
-        <f>COUNTIF($C$5:$C$46,C10)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C76" s="30">
-        <f>COUNTIF($C$5:$C$46,C11)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C77" s="30">
-        <f>COUNTIF($C$5:$C$46,C12)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C78" s="30">
-        <f>COUNTIF($C$5:$C$46,C13)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C79" s="30">
-        <f>COUNTIF($C$5:$C$46,C14)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C80" s="30">
-        <f>COUNTIF($C$5:$C$46,C15)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -59201,7 +59635,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="30">
-        <f>COUNTIF($C$5:$C$46,C17)</f>
+        <f t="shared" ref="C81:C91" si="2">COUNTIF($C$5:$C$46,C17)</f>
         <v>1</v>
       </c>
     </row>
@@ -59210,7 +59644,7 @@
         <v>2</v>
       </c>
       <c r="C82" s="30">
-        <f>COUNTIF($C$5:$C$46,C18)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -59219,7 +59653,7 @@
         <v>3</v>
       </c>
       <c r="C83" s="30">
-        <f>COUNTIF($C$5:$C$46,C19)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -59228,7 +59662,7 @@
         <v>4</v>
       </c>
       <c r="C84" s="30">
-        <f>COUNTIF($C$5:$C$46,C20)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -59237,7 +59671,7 @@
         <v>5</v>
       </c>
       <c r="C85" s="30">
-        <f>COUNTIF($C$5:$C$46,C21)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -59246,7 +59680,7 @@
         <v>6</v>
       </c>
       <c r="C86" s="30">
-        <f>COUNTIF($C$5:$C$46,C22)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -59255,7 +59689,7 @@
         <v>7</v>
       </c>
       <c r="C87" s="30">
-        <f>COUNTIF($C$5:$C$46,C23)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -59264,7 +59698,7 @@
         <v>8</v>
       </c>
       <c r="C88" s="30">
-        <f>COUNTIF($C$5:$C$46,C24)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -59273,7 +59707,7 @@
         <v>9</v>
       </c>
       <c r="C89" s="30">
-        <f>COUNTIF($C$5:$C$46,C25)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -59282,7 +59716,7 @@
         <v>10</v>
       </c>
       <c r="C90" s="30">
-        <f>COUNTIF($C$5:$C$46,C26)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -59291,7 +59725,7 @@
         <v>11</v>
       </c>
       <c r="C91" s="30">
-        <f>COUNTIF($C$5:$C$46,C27)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -59300,7 +59734,7 @@
         <v>12</v>
       </c>
       <c r="C92" s="30">
-        <f>COUNTIF($C$5:$C$46,C29)</f>
+        <f t="shared" ref="C92:C109" si="3">COUNTIF($C$5:$C$46,C29)</f>
         <v>1</v>
       </c>
     </row>
@@ -59309,7 +59743,7 @@
         <v>13</v>
       </c>
       <c r="C93" s="30">
-        <f>COUNTIF($C$5:$C$46,C30)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -59318,7 +59752,7 @@
         <v>14</v>
       </c>
       <c r="C94" s="30">
-        <f>COUNTIF($C$5:$C$46,C31)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -59327,7 +59761,7 @@
         <v>15</v>
       </c>
       <c r="C95" s="30">
-        <f>COUNTIF($C$5:$C$46,C32)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -59336,7 +59770,7 @@
         <v>16</v>
       </c>
       <c r="C96" s="30">
-        <f>COUNTIF($C$5:$C$46,C33)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -59345,7 +59779,7 @@
         <v>17</v>
       </c>
       <c r="C97" s="30">
-        <f>COUNTIF($C$5:$C$46,C34)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -59354,7 +59788,7 @@
         <v>18</v>
       </c>
       <c r="C98" s="30">
-        <f>COUNTIF($C$5:$C$46,C35)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -59363,7 +59797,7 @@
         <v>19</v>
       </c>
       <c r="C99" s="30">
-        <f>COUNTIF($C$5:$C$46,C36)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -59372,7 +59806,7 @@
         <v>20</v>
       </c>
       <c r="C100" s="30">
-        <f>COUNTIF($C$5:$C$46,C37)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -59381,7 +59815,7 @@
         <v>21</v>
       </c>
       <c r="C101" s="30">
-        <f>COUNTIF($C$5:$C$46,C38)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -59390,56 +59824,56 @@
         <v>22</v>
       </c>
       <c r="C102" s="30">
-        <f>COUNTIF($C$5:$C$46,C39)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B103"/>
       <c r="C103" s="30">
-        <f>COUNTIF($C$5:$C$46,C40)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B104"/>
       <c r="C104" s="30">
-        <f>COUNTIF($C$5:$C$46,C41)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B105"/>
       <c r="C105" s="30">
-        <f>COUNTIF($C$5:$C$46,C42)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B106"/>
       <c r="C106" s="30">
-        <f>COUNTIF($C$5:$C$46,C43)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B107"/>
       <c r="C107" s="30">
-        <f>COUNTIF($C$5:$C$46,C44)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B108"/>
       <c r="C108" s="30">
-        <f>COUNTIF($C$5:$C$46,C45)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B109"/>
       <c r="C109" s="30">
-        <f>COUNTIF($C$5:$C$46,C46)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -62546,8 +62980,8 @@
   </sheetPr>
   <dimension ref="A1:BA149"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="S57" sqref="S57"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -68358,19 +68792,20 @@
         <v>0</v>
       </c>
       <c r="F83" s="82">
-        <v>8.1288130107613874</v>
+        <f>9.1*1.152</f>
+        <v>10.483199999999998</v>
       </c>
       <c r="G83" s="82">
         <f>F83</f>
-        <v>8.1288130107613874</v>
+        <v>10.483199999999998</v>
       </c>
       <c r="H83" s="82">
         <f>G83</f>
-        <v>8.1288130107613874</v>
+        <v>10.483199999999998</v>
       </c>
       <c r="I83" s="82">
         <f>H83</f>
-        <v>8.1288130107613874</v>
+        <v>10.483199999999998</v>
       </c>
       <c r="J83" s="82">
         <v>0</v>

</xml_diff>

<commit_message>
Fixing gas and liquid fuel balances
</commit_message>
<xml_diff>
--- a/VT_REGION1_SUP.xlsx
+++ b/VT_REGION1_SUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924A2E3F-267C-4B2D-9689-1CDF13F723EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD03344-50FE-4A84-A34A-1C145995EBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="1065" windowWidth="26610" windowHeight="11385" firstSheet="8" activeTab="11" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -223,7 +223,11 @@
     <author>tc={2D025629-877F-4A51-97DF-4B63BC17F90B}</author>
     <author>tc={00B9291C-0286-423F-9703-F64CCB57F70F}</author>
     <author>tc={87179AE4-EC17-4370-98D7-F32C73BD771A}</author>
+    <author>tc={E69A6D97-9056-4FB3-8A4E-00F5B2E78FD6}</author>
+    <author>tc={F93D2D09-DC95-4216-81E9-77B6F290F34D}</author>
     <author>tc={6A82080C-3A46-4F98-A8BB-1FF2F957BEF2}</author>
+    <author>tc={2FB1C6F0-AD57-4E16-BFAC-B7DB9955D691}</author>
+    <author>tc={B0A60D28-BB18-4A91-9004-62133F119943}</author>
     <author>tc={E56230BC-BD11-4915-915B-9473750B9EC2}</author>
   </authors>
   <commentList>
@@ -677,7 +681,23 @@
     IRP 2019 costs adjusted to 2022</t>
       </text>
     </comment>
-    <comment ref="K89" authorId="10" shapeId="0" xr:uid="{6A82080C-3A46-4F98-A8BB-1FF2F957BEF2}">
+    <comment ref="K86" authorId="10" shapeId="0" xr:uid="{E69A6D97-9056-4FB3-8A4E-00F5B2E78FD6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    From EB</t>
+      </text>
+    </comment>
+    <comment ref="K87" authorId="11" shapeId="0" xr:uid="{F93D2D09-DC95-4216-81E9-77B6F290F34D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    From EB</t>
+      </text>
+    </comment>
+    <comment ref="K89" authorId="12" shapeId="0" xr:uid="{6A82080C-3A46-4F98-A8BB-1FF2F957BEF2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -685,7 +705,23 @@
     .56 added to avoid zzs</t>
       </text>
     </comment>
-    <comment ref="F95" authorId="11" shapeId="0" xr:uid="{E56230BC-BD11-4915-915B-9473750B9EC2}">
+    <comment ref="K90" authorId="13" shapeId="0" xr:uid="{2FB1C6F0-AD57-4E16-BFAC-B7DB9955D691}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    From energy balance</t>
+      </text>
+    </comment>
+    <comment ref="K94" authorId="14" shapeId="0" xr:uid="{B0A60D28-BB18-4A91-9004-62133F119943}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    From gas balance</t>
+      </text>
+    </comment>
+    <comment ref="F95" authorId="15" shapeId="0" xr:uid="{E56230BC-BD11-4915-915B-9473750B9EC2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -7350,6 +7386,57 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7387,57 +7474,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -24775,8 +24811,20 @@
   <threadedComment ref="F83" dT="2023-09-07T10:07:04.92" personId="{8B1FB5F6-C05B-4C45-A9FE-3B209CC95A5D}" id="{87179AE4-EC17-4370-98D7-F32C73BD771A}">
     <text>IRP 2019 costs adjusted to 2022</text>
   </threadedComment>
+  <threadedComment ref="K86" dT="2023-09-20T09:30:23.94" personId="{8B1FB5F6-C05B-4C45-A9FE-3B209CC95A5D}" id="{E69A6D97-9056-4FB3-8A4E-00F5B2E78FD6}">
+    <text>From EB</text>
+  </threadedComment>
+  <threadedComment ref="K87" dT="2023-09-20T09:30:52.75" personId="{8B1FB5F6-C05B-4C45-A9FE-3B209CC95A5D}" id="{F93D2D09-DC95-4216-81E9-77B6F290F34D}">
+    <text>From EB</text>
+  </threadedComment>
   <threadedComment ref="K89" dT="2021-07-26T15:05:55.74" personId="{E500B1BD-2FF0-4DFA-88F6-72D20CDE0583}" id="{6A82080C-3A46-4F98-A8BB-1FF2F957BEF2}">
     <text>.56 added to avoid zzs</text>
+  </threadedComment>
+  <threadedComment ref="K90" dT="2023-09-20T10:17:52.15" personId="{8B1FB5F6-C05B-4C45-A9FE-3B209CC95A5D}" id="{2FB1C6F0-AD57-4E16-BFAC-B7DB9955D691}">
+    <text>From energy balance</text>
+  </threadedComment>
+  <threadedComment ref="K94" dT="2023-09-20T08:41:00.65" personId="{8B1FB5F6-C05B-4C45-A9FE-3B209CC95A5D}" id="{B0A60D28-BB18-4A91-9004-62133F119943}">
+    <text>From gas balance</text>
   </threadedComment>
   <threadedComment ref="F95" dT="2023-08-14T09:36:51.53" personId="{8B1FB5F6-C05B-4C45-A9FE-3B209CC95A5D}" id="{E56230BC-BD11-4915-915B-9473750B9EC2}">
     <text>LNG price minus liquefaction costs</text>
@@ -24902,25 +24950,25 @@
       <c r="W6" s="175" t="s">
         <v>362</v>
       </c>
-      <c r="AC6" s="416" t="s">
+      <c r="AC6" s="433" t="s">
         <v>363</v>
       </c>
-      <c r="AD6" s="416"/>
-      <c r="AE6" s="416"/>
+      <c r="AD6" s="433"/>
+      <c r="AE6" s="433"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="417" t="s">
+      <c r="A7" s="434" t="s">
         <v>364</v>
       </c>
-      <c r="B7" s="419" t="s">
+      <c r="B7" s="436" t="s">
         <v>365</v>
       </c>
-      <c r="C7" s="421" t="s">
+      <c r="C7" s="438" t="s">
         <v>366</v>
       </c>
-      <c r="D7" s="422"/>
-      <c r="E7" s="423"/>
-      <c r="F7" s="426" t="s">
+      <c r="D7" s="439"/>
+      <c r="E7" s="440"/>
+      <c r="F7" s="443" t="s">
         <v>367</v>
       </c>
       <c r="G7" s="176"/>
@@ -24948,12 +24996,12 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="418"/>
-      <c r="B8" s="420"/>
-      <c r="C8" s="424"/>
-      <c r="D8" s="425"/>
-      <c r="E8" s="425"/>
-      <c r="F8" s="427"/>
+      <c r="A8" s="435"/>
+      <c r="B8" s="437"/>
+      <c r="C8" s="441"/>
+      <c r="D8" s="442"/>
+      <c r="E8" s="442"/>
+      <c r="F8" s="444"/>
       <c r="G8" s="176"/>
       <c r="H8" s="176"/>
       <c r="I8" s="176"/>
@@ -25819,11 +25867,11 @@
       <c r="I25" s="57"/>
       <c r="J25" s="57"/>
       <c r="V25" s="217"/>
-      <c r="AC25" s="415" t="s">
+      <c r="AC25" s="432" t="s">
         <v>433</v>
       </c>
-      <c r="AD25" s="415"/>
-      <c r="AE25" s="415"/>
+      <c r="AD25" s="432"/>
+      <c r="AE25" s="432"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C26" s="57"/>
@@ -25902,8 +25950,8 @@
       <c r="D30" s="57"/>
     </row>
     <row r="31" spans="1:31" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H31" s="435"/>
-      <c r="I31" s="435"/>
+      <c r="H31" s="428"/>
+      <c r="I31" s="428"/>
       <c r="R31" t="s">
         <v>371</v>
       </c>
@@ -25924,10 +25972,10 @@
       </c>
     </row>
     <row r="32" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L32" s="428" t="s">
+      <c r="L32" s="420" t="s">
         <v>437</v>
       </c>
-      <c r="M32" s="436" t="s">
+      <c r="M32" s="429" t="s">
         <v>438</v>
       </c>
       <c r="N32" s="220" t="s">
@@ -25942,22 +25990,22 @@
       <c r="Q32" s="223" t="s">
         <v>440</v>
       </c>
-      <c r="R32" s="428" t="s">
+      <c r="R32" s="420" t="s">
         <v>390</v>
       </c>
-      <c r="S32" s="428" t="s">
+      <c r="S32" s="420" t="s">
         <v>394</v>
       </c>
-      <c r="T32" s="428" t="s">
+      <c r="T32" s="420" t="s">
         <v>441</v>
       </c>
-      <c r="U32" s="428" t="s">
+      <c r="U32" s="420" t="s">
         <v>390</v>
       </c>
-      <c r="V32" s="428" t="s">
+      <c r="V32" s="420" t="s">
         <v>394</v>
       </c>
-      <c r="W32" s="428" t="s">
+      <c r="W32" s="420" t="s">
         <v>441</v>
       </c>
     </row>
@@ -25980,28 +26028,28 @@
       <c r="G33" s="142" t="s">
         <v>445</v>
       </c>
-      <c r="H33" s="431" t="s">
+      <c r="H33" s="427" t="s">
         <v>446</v>
       </c>
-      <c r="I33" s="431"/>
+      <c r="I33" s="427"/>
       <c r="J33" s="142" t="s">
         <v>444</v>
       </c>
       <c r="K33" t="s">
         <v>445</v>
       </c>
-      <c r="L33" s="429"/>
-      <c r="M33" s="437"/>
+      <c r="L33" s="421"/>
+      <c r="M33" s="430"/>
       <c r="N33" s="16"/>
       <c r="O33" s="73"/>
       <c r="P33" s="73"/>
       <c r="Q33" s="224"/>
-      <c r="R33" s="429"/>
-      <c r="S33" s="429"/>
-      <c r="T33" s="429"/>
-      <c r="U33" s="429"/>
-      <c r="V33" s="429"/>
-      <c r="W33" s="429"/>
+      <c r="R33" s="421"/>
+      <c r="S33" s="421"/>
+      <c r="T33" s="421"/>
+      <c r="U33" s="421"/>
+      <c r="V33" s="421"/>
+      <c r="W33" s="421"/>
     </row>
     <row r="34" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -26021,8 +26069,8 @@
       <c r="K34" t="s">
         <v>448</v>
       </c>
-      <c r="L34" s="430"/>
-      <c r="M34" s="438"/>
+      <c r="L34" s="422"/>
+      <c r="M34" s="431"/>
       <c r="N34" s="225" t="s">
         <v>450</v>
       </c>
@@ -26035,12 +26083,12 @@
       <c r="Q34" s="227" t="s">
         <v>450</v>
       </c>
-      <c r="R34" s="430"/>
-      <c r="S34" s="430"/>
-      <c r="T34" s="430"/>
-      <c r="U34" s="430"/>
-      <c r="V34" s="430"/>
-      <c r="W34" s="430"/>
+      <c r="R34" s="422"/>
+      <c r="S34" s="422"/>
+      <c r="T34" s="422"/>
+      <c r="U34" s="422"/>
+      <c r="V34" s="422"/>
+      <c r="W34" s="422"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="228" t="s">
@@ -26106,7 +26154,7 @@
         <v>2.9</v>
       </c>
       <c r="I36" s="237"/>
-      <c r="L36" s="432" t="str">
+      <c r="L36" s="423" t="str">
         <f>A36</f>
         <v>Well completion</v>
       </c>
@@ -26186,7 +26234,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="I37" s="237"/>
-      <c r="L37" s="433"/>
+      <c r="L37" s="424"/>
       <c r="M37" t="str">
         <f t="shared" ref="M37:M45" si="5">B37</f>
         <v>Jiang et al. (2011)</v>
@@ -26257,7 +26305,7 @@
         <v>7.8</v>
       </c>
       <c r="I38" s="237"/>
-      <c r="L38" s="433"/>
+      <c r="L38" s="424"/>
       <c r="M38" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26332,7 +26380,7 @@
       </c>
       <c r="I39" s="237"/>
       <c r="K39" s="237"/>
-      <c r="L39" s="433"/>
+      <c r="L39" s="424"/>
       <c r="M39" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26403,7 +26451,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="I40" s="237"/>
-      <c r="L40" s="433"/>
+      <c r="L40" s="424"/>
       <c r="M40" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26477,7 +26525,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="I41" s="237"/>
-      <c r="L41" s="434"/>
+      <c r="L41" s="425"/>
       <c r="M41" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Broderick et al. (2011)</v>
@@ -26551,7 +26599,7 @@
         <v>4.2</v>
       </c>
       <c r="I42" s="237"/>
-      <c r="L42" s="432" t="s">
+      <c r="L42" s="423" t="s">
         <v>414</v>
       </c>
       <c r="M42" s="222" t="str">
@@ -26624,7 +26672,7 @@
         <v>3.5</v>
       </c>
       <c r="I43" s="237"/>
-      <c r="L43" s="433"/>
+      <c r="L43" s="424"/>
       <c r="M43" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26700,7 +26748,7 @@
       </c>
       <c r="I44" s="237"/>
       <c r="K44" s="237"/>
-      <c r="L44" s="433"/>
+      <c r="L44" s="424"/>
       <c r="M44" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26772,7 +26820,7 @@
         <v>8.9</v>
       </c>
       <c r="I45" s="237"/>
-      <c r="L45" s="434"/>
+      <c r="L45" s="425"/>
       <c r="M45" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26841,7 +26889,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="237"/>
-      <c r="L46" s="432" t="str">
+      <c r="L46" s="423" t="str">
         <f>A47</f>
         <v>Transport, storage and distribution</v>
       </c>
@@ -26917,7 +26965,7 @@
         <v>1.9</v>
       </c>
       <c r="I47" s="237"/>
-      <c r="L47" s="433"/>
+      <c r="L47" s="424"/>
       <c r="M47" t="str">
         <f>B48</f>
         <v>Skone et al. (2011)</v>
@@ -26988,7 +27036,7 @@
         <v>2.7</v>
       </c>
       <c r="I48" s="237"/>
-      <c r="L48" s="434"/>
+      <c r="L48" s="425"/>
       <c r="M48" s="95" t="str">
         <f>B49</f>
         <v>Howarth et al. (2011)</v>
@@ -27357,10 +27405,10 @@
       <c r="C79" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="D79" s="444" t="s">
+      <c r="D79" s="426" t="s">
         <v>499</v>
       </c>
-      <c r="E79" s="444"/>
+      <c r="E79" s="426"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
@@ -27462,13 +27510,13 @@
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="439" t="s">
+      <c r="A103" s="415" t="s">
         <v>509</v>
       </c>
       <c r="B103" s="266" t="s">
         <v>510</v>
       </c>
-      <c r="C103" s="441" t="s">
+      <c r="C103" s="417" t="s">
         <v>511</v>
       </c>
       <c r="D103" s="266">
@@ -27479,11 +27527,11 @@
       </c>
     </row>
     <row r="104" spans="1:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="440"/>
+      <c r="A104" s="416"/>
       <c r="B104" s="266" t="s">
         <v>512</v>
       </c>
-      <c r="C104" s="442"/>
+      <c r="C104" s="418"/>
       <c r="D104" s="266">
         <v>0.18</v>
       </c>
@@ -27496,13 +27544,13 @@
       </c>
     </row>
     <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="439" t="s">
+      <c r="A105" s="415" t="s">
         <v>513</v>
       </c>
       <c r="B105" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C105" s="442"/>
+      <c r="C105" s="418"/>
       <c r="D105" s="266">
         <v>0</v>
       </c>
@@ -27511,11 +27559,11 @@
       </c>
     </row>
     <row r="106" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="440"/>
+      <c r="A106" s="416"/>
       <c r="B106" s="266" t="s">
         <v>515</v>
       </c>
-      <c r="C106" s="443"/>
+      <c r="C106" s="419"/>
       <c r="D106" s="266">
         <v>0</v>
       </c>
@@ -27524,13 +27572,13 @@
       </c>
     </row>
     <row r="107" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="439" t="s">
+      <c r="A107" s="415" t="s">
         <v>509</v>
       </c>
       <c r="B107" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C107" s="441" t="s">
+      <c r="C107" s="417" t="s">
         <v>516</v>
       </c>
       <c r="D107" s="266">
@@ -27541,11 +27589,11 @@
       </c>
     </row>
     <row r="108" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="440"/>
+      <c r="A108" s="416"/>
       <c r="B108" s="266" t="s">
         <v>515</v>
       </c>
-      <c r="C108" s="442"/>
+      <c r="C108" s="418"/>
       <c r="D108" s="266">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -27554,13 +27602,13 @@
       </c>
     </row>
     <row r="109" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="439" t="s">
+      <c r="A109" s="415" t="s">
         <v>513</v>
       </c>
       <c r="B109" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C109" s="442"/>
+      <c r="C109" s="418"/>
       <c r="D109" s="266">
         <v>0</v>
       </c>
@@ -27569,11 +27617,11 @@
       </c>
     </row>
     <row r="110" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="440"/>
+      <c r="A110" s="416"/>
       <c r="B110" s="266" t="s">
         <v>515</v>
       </c>
-      <c r="C110" s="443"/>
+      <c r="C110" s="419"/>
       <c r="D110" s="266">
         <v>0</v>
       </c>
@@ -29036,6 +29084,22 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="AC25:AE25"/>
+    <mergeCell ref="AC6:AE6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="W32:W34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="L36:L41"/>
+    <mergeCell ref="L42:L45"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="L32:L34"/>
+    <mergeCell ref="M32:M34"/>
+    <mergeCell ref="R32:R34"/>
+    <mergeCell ref="S32:S34"/>
+    <mergeCell ref="T32:T34"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="C107:C110"/>
     <mergeCell ref="A109:A110"/>
@@ -29046,22 +29110,6 @@
     <mergeCell ref="A103:A104"/>
     <mergeCell ref="C103:C106"/>
     <mergeCell ref="A105:A106"/>
-    <mergeCell ref="W32:W34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="L36:L41"/>
-    <mergeCell ref="L42:L45"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="L32:L34"/>
-    <mergeCell ref="M32:M34"/>
-    <mergeCell ref="R32:R34"/>
-    <mergeCell ref="S32:S34"/>
-    <mergeCell ref="T32:T34"/>
-    <mergeCell ref="AC25:AE25"/>
-    <mergeCell ref="AC6:AE6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29812,7 +29860,7 @@
   </sheetPr>
   <dimension ref="A1:AE115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -49537,18 +49585,18 @@
         <f>FORECAST(CR93,CP94:CQ94,CP93:CQ93)</f>
         <v>93</v>
       </c>
-      <c r="DL94" s="431" t="s">
+      <c r="DL94" s="427" t="s">
         <v>763</v>
       </c>
-      <c r="DM94" s="431"/>
-      <c r="DN94" s="431" t="s">
+      <c r="DM94" s="427"/>
+      <c r="DN94" s="427" t="s">
         <v>764</v>
       </c>
-      <c r="DO94" s="431"/>
-      <c r="DP94" s="431" t="s">
+      <c r="DO94" s="427"/>
+      <c r="DP94" s="427" t="s">
         <v>762</v>
       </c>
-      <c r="DQ94" s="431"/>
+      <c r="DQ94" s="427"/>
     </row>
     <row r="95" spans="1:121" x14ac:dyDescent="0.25">
       <c r="BK95" t="s">
@@ -55009,7 +55057,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="18">
         <f ca="1">NOW()</f>
-        <v>45188.424600115737</v>
+        <v>45189.512249074076</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -55833,7 +55881,7 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
         <f ca="1">NOW()</f>
-        <v>45188.424600115737</v>
+        <v>45189.512249074076</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -59945,8 +59993,8 @@
   </sheetPr>
   <dimension ref="A1:BA149"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="L88" sqref="L88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -65776,7 +65824,7 @@
         <v>0</v>
       </c>
       <c r="K83" s="82">
-        <f t="shared" ref="K83:K88" si="37">SUMIF($C$8:$AZ$8,D83,$C$11:$AZ$11)</f>
+        <f t="shared" ref="K83:K85" si="37">SUMIF($C$8:$AZ$8,D83,$C$11:$AZ$11)</f>
         <v>170.374545454545</v>
       </c>
       <c r="L83" s="82"/>
@@ -66013,8 +66061,7 @@
         <v>0</v>
       </c>
       <c r="K86" s="82">
-        <f t="shared" si="37"/>
-        <v>140.06492</v>
+        <v>162</v>
       </c>
       <c r="L86" s="82"/>
       <c r="M86"/>
@@ -66091,8 +66138,7 @@
         <v>0</v>
       </c>
       <c r="K87" s="82">
-        <f t="shared" si="37"/>
-        <v>63.331960000000002</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="L87" s="82"/>
       <c r="M87"/>
@@ -66169,8 +66215,7 @@
         <v>0</v>
       </c>
       <c r="K88" s="82">
-        <f t="shared" si="37"/>
-        <v>4.206396917894736</v>
+        <v>0</v>
       </c>
       <c r="L88" s="82"/>
       <c r="M88"/>
@@ -66247,8 +66292,7 @@
         <v>0</v>
       </c>
       <c r="K89" s="82">
-        <f>0.66+0.56+1.22/0.79+0.57/0.65</f>
-        <v>3.6412268743914313</v>
+        <v>2.1</v>
       </c>
       <c r="L89" s="82"/>
       <c r="M89"/>
@@ -66325,8 +66369,7 @@
         <v>0</v>
       </c>
       <c r="K90" s="82">
-        <f>SUMIF($C$8:$AZ$8,D90,$C$11:$AZ$11)</f>
-        <v>9.3231960462962959</v>
+        <v>15</v>
       </c>
       <c r="L90" s="82"/>
       <c r="M90"/>
@@ -66599,7 +66642,7 @@
         <v>3</v>
       </c>
       <c r="K94" s="82">
-        <v>116</v>
+        <v>151.28700000000001</v>
       </c>
       <c r="L94" s="82">
         <v>156</v>

</xml_diff>

<commit_message>
discard coal price was missing
</commit_message>
<xml_diff>
--- a/VT_REGION1_SUP.xlsx
+++ b/VT_REGION1_SUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260F39EB-1676-466C-B0FC-99B925C2DD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74A8BAF-EA94-4778-BED4-771ECE671DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="26610" windowHeight="13740" firstSheet="4" activeTab="5" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="26610" windowHeight="13740" firstSheet="4" activeTab="6" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -7386,6 +7386,57 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7423,57 +7474,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -24950,25 +24950,25 @@
       <c r="W6" s="175" t="s">
         <v>361</v>
       </c>
-      <c r="AC6" s="416" t="s">
+      <c r="AC6" s="433" t="s">
         <v>362</v>
       </c>
-      <c r="AD6" s="416"/>
-      <c r="AE6" s="416"/>
+      <c r="AD6" s="433"/>
+      <c r="AE6" s="433"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="417" t="s">
+      <c r="A7" s="434" t="s">
         <v>363</v>
       </c>
-      <c r="B7" s="419" t="s">
+      <c r="B7" s="436" t="s">
         <v>364</v>
       </c>
-      <c r="C7" s="421" t="s">
+      <c r="C7" s="438" t="s">
         <v>365</v>
       </c>
-      <c r="D7" s="422"/>
-      <c r="E7" s="423"/>
-      <c r="F7" s="426" t="s">
+      <c r="D7" s="439"/>
+      <c r="E7" s="440"/>
+      <c r="F7" s="443" t="s">
         <v>366</v>
       </c>
       <c r="G7" s="176"/>
@@ -24996,12 +24996,12 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="418"/>
-      <c r="B8" s="420"/>
-      <c r="C8" s="424"/>
-      <c r="D8" s="425"/>
-      <c r="E8" s="425"/>
-      <c r="F8" s="427"/>
+      <c r="A8" s="435"/>
+      <c r="B8" s="437"/>
+      <c r="C8" s="441"/>
+      <c r="D8" s="442"/>
+      <c r="E8" s="442"/>
+      <c r="F8" s="444"/>
       <c r="G8" s="176"/>
       <c r="H8" s="176"/>
       <c r="I8" s="176"/>
@@ -25867,11 +25867,11 @@
       <c r="I25" s="57"/>
       <c r="J25" s="57"/>
       <c r="V25" s="217"/>
-      <c r="AC25" s="415" t="s">
+      <c r="AC25" s="432" t="s">
         <v>432</v>
       </c>
-      <c r="AD25" s="415"/>
-      <c r="AE25" s="415"/>
+      <c r="AD25" s="432"/>
+      <c r="AE25" s="432"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C26" s="57"/>
@@ -25950,8 +25950,8 @@
       <c r="D30" s="57"/>
     </row>
     <row r="31" spans="1:31" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H31" s="435"/>
-      <c r="I31" s="435"/>
+      <c r="H31" s="428"/>
+      <c r="I31" s="428"/>
       <c r="R31" t="s">
         <v>370</v>
       </c>
@@ -25972,10 +25972,10 @@
       </c>
     </row>
     <row r="32" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L32" s="428" t="s">
+      <c r="L32" s="420" t="s">
         <v>436</v>
       </c>
-      <c r="M32" s="436" t="s">
+      <c r="M32" s="429" t="s">
         <v>437</v>
       </c>
       <c r="N32" s="220" t="s">
@@ -25990,22 +25990,22 @@
       <c r="Q32" s="223" t="s">
         <v>439</v>
       </c>
-      <c r="R32" s="428" t="s">
+      <c r="R32" s="420" t="s">
         <v>389</v>
       </c>
-      <c r="S32" s="428" t="s">
+      <c r="S32" s="420" t="s">
         <v>393</v>
       </c>
-      <c r="T32" s="428" t="s">
+      <c r="T32" s="420" t="s">
         <v>440</v>
       </c>
-      <c r="U32" s="428" t="s">
+      <c r="U32" s="420" t="s">
         <v>389</v>
       </c>
-      <c r="V32" s="428" t="s">
+      <c r="V32" s="420" t="s">
         <v>393</v>
       </c>
-      <c r="W32" s="428" t="s">
+      <c r="W32" s="420" t="s">
         <v>440</v>
       </c>
     </row>
@@ -26028,28 +26028,28 @@
       <c r="G33" s="142" t="s">
         <v>444</v>
       </c>
-      <c r="H33" s="431" t="s">
+      <c r="H33" s="427" t="s">
         <v>445</v>
       </c>
-      <c r="I33" s="431"/>
+      <c r="I33" s="427"/>
       <c r="J33" s="142" t="s">
         <v>443</v>
       </c>
       <c r="K33" t="s">
         <v>444</v>
       </c>
-      <c r="L33" s="429"/>
-      <c r="M33" s="437"/>
+      <c r="L33" s="421"/>
+      <c r="M33" s="430"/>
       <c r="N33" s="16"/>
       <c r="O33" s="73"/>
       <c r="P33" s="73"/>
       <c r="Q33" s="224"/>
-      <c r="R33" s="429"/>
-      <c r="S33" s="429"/>
-      <c r="T33" s="429"/>
-      <c r="U33" s="429"/>
-      <c r="V33" s="429"/>
-      <c r="W33" s="429"/>
+      <c r="R33" s="421"/>
+      <c r="S33" s="421"/>
+      <c r="T33" s="421"/>
+      <c r="U33" s="421"/>
+      <c r="V33" s="421"/>
+      <c r="W33" s="421"/>
     </row>
     <row r="34" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -26069,8 +26069,8 @@
       <c r="K34" t="s">
         <v>447</v>
       </c>
-      <c r="L34" s="430"/>
-      <c r="M34" s="438"/>
+      <c r="L34" s="422"/>
+      <c r="M34" s="431"/>
       <c r="N34" s="225" t="s">
         <v>449</v>
       </c>
@@ -26083,12 +26083,12 @@
       <c r="Q34" s="227" t="s">
         <v>449</v>
       </c>
-      <c r="R34" s="430"/>
-      <c r="S34" s="430"/>
-      <c r="T34" s="430"/>
-      <c r="U34" s="430"/>
-      <c r="V34" s="430"/>
-      <c r="W34" s="430"/>
+      <c r="R34" s="422"/>
+      <c r="S34" s="422"/>
+      <c r="T34" s="422"/>
+      <c r="U34" s="422"/>
+      <c r="V34" s="422"/>
+      <c r="W34" s="422"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="228" t="s">
@@ -26154,7 +26154,7 @@
         <v>2.9</v>
       </c>
       <c r="I36" s="237"/>
-      <c r="L36" s="432" t="str">
+      <c r="L36" s="423" t="str">
         <f>A36</f>
         <v>Well completion</v>
       </c>
@@ -26234,7 +26234,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="I37" s="237"/>
-      <c r="L37" s="433"/>
+      <c r="L37" s="424"/>
       <c r="M37" t="str">
         <f t="shared" ref="M37:M45" si="5">B37</f>
         <v>Jiang et al. (2011)</v>
@@ -26305,7 +26305,7 @@
         <v>7.8</v>
       </c>
       <c r="I38" s="237"/>
-      <c r="L38" s="433"/>
+      <c r="L38" s="424"/>
       <c r="M38" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26380,7 +26380,7 @@
       </c>
       <c r="I39" s="237"/>
       <c r="K39" s="237"/>
-      <c r="L39" s="433"/>
+      <c r="L39" s="424"/>
       <c r="M39" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26451,7 +26451,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="I40" s="237"/>
-      <c r="L40" s="433"/>
+      <c r="L40" s="424"/>
       <c r="M40" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26525,7 +26525,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="I41" s="237"/>
-      <c r="L41" s="434"/>
+      <c r="L41" s="425"/>
       <c r="M41" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Broderick et al. (2011)</v>
@@ -26599,7 +26599,7 @@
         <v>4.2</v>
       </c>
       <c r="I42" s="237"/>
-      <c r="L42" s="432" t="s">
+      <c r="L42" s="423" t="s">
         <v>413</v>
       </c>
       <c r="M42" s="222" t="str">
@@ -26672,7 +26672,7 @@
         <v>3.5</v>
       </c>
       <c r="I43" s="237"/>
-      <c r="L43" s="433"/>
+      <c r="L43" s="424"/>
       <c r="M43" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26748,7 +26748,7 @@
       </c>
       <c r="I44" s="237"/>
       <c r="K44" s="237"/>
-      <c r="L44" s="433"/>
+      <c r="L44" s="424"/>
       <c r="M44" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26820,7 +26820,7 @@
         <v>8.9</v>
       </c>
       <c r="I45" s="237"/>
-      <c r="L45" s="434"/>
+      <c r="L45" s="425"/>
       <c r="M45" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26889,7 +26889,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="237"/>
-      <c r="L46" s="432" t="str">
+      <c r="L46" s="423" t="str">
         <f>A47</f>
         <v>Transport, storage and distribution</v>
       </c>
@@ -26965,7 +26965,7 @@
         <v>1.9</v>
       </c>
       <c r="I47" s="237"/>
-      <c r="L47" s="433"/>
+      <c r="L47" s="424"/>
       <c r="M47" t="str">
         <f>B48</f>
         <v>Skone et al. (2011)</v>
@@ -27036,7 +27036,7 @@
         <v>2.7</v>
       </c>
       <c r="I48" s="237"/>
-      <c r="L48" s="434"/>
+      <c r="L48" s="425"/>
       <c r="M48" s="95" t="str">
         <f>B49</f>
         <v>Howarth et al. (2011)</v>
@@ -27405,10 +27405,10 @@
       <c r="C79" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="D79" s="444" t="s">
+      <c r="D79" s="426" t="s">
         <v>498</v>
       </c>
-      <c r="E79" s="444"/>
+      <c r="E79" s="426"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
@@ -27510,13 +27510,13 @@
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="439" t="s">
+      <c r="A103" s="415" t="s">
         <v>508</v>
       </c>
       <c r="B103" s="266" t="s">
         <v>509</v>
       </c>
-      <c r="C103" s="441" t="s">
+      <c r="C103" s="417" t="s">
         <v>510</v>
       </c>
       <c r="D103" s="266">
@@ -27527,11 +27527,11 @@
       </c>
     </row>
     <row r="104" spans="1:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="440"/>
+      <c r="A104" s="416"/>
       <c r="B104" s="266" t="s">
         <v>511</v>
       </c>
-      <c r="C104" s="442"/>
+      <c r="C104" s="418"/>
       <c r="D104" s="266">
         <v>0.18</v>
       </c>
@@ -27544,13 +27544,13 @@
       </c>
     </row>
     <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="439" t="s">
+      <c r="A105" s="415" t="s">
         <v>512</v>
       </c>
       <c r="B105" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C105" s="442"/>
+      <c r="C105" s="418"/>
       <c r="D105" s="266">
         <v>0</v>
       </c>
@@ -27559,11 +27559,11 @@
       </c>
     </row>
     <row r="106" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="440"/>
+      <c r="A106" s="416"/>
       <c r="B106" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C106" s="443"/>
+      <c r="C106" s="419"/>
       <c r="D106" s="266">
         <v>0</v>
       </c>
@@ -27572,13 +27572,13 @@
       </c>
     </row>
     <row r="107" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="439" t="s">
+      <c r="A107" s="415" t="s">
         <v>508</v>
       </c>
       <c r="B107" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C107" s="441" t="s">
+      <c r="C107" s="417" t="s">
         <v>515</v>
       </c>
       <c r="D107" s="266">
@@ -27589,11 +27589,11 @@
       </c>
     </row>
     <row r="108" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="440"/>
+      <c r="A108" s="416"/>
       <c r="B108" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C108" s="442"/>
+      <c r="C108" s="418"/>
       <c r="D108" s="266">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -27602,13 +27602,13 @@
       </c>
     </row>
     <row r="109" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="439" t="s">
+      <c r="A109" s="415" t="s">
         <v>512</v>
       </c>
       <c r="B109" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C109" s="442"/>
+      <c r="C109" s="418"/>
       <c r="D109" s="266">
         <v>0</v>
       </c>
@@ -27617,11 +27617,11 @@
       </c>
     </row>
     <row r="110" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="440"/>
+      <c r="A110" s="416"/>
       <c r="B110" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C110" s="443"/>
+      <c r="C110" s="419"/>
       <c r="D110" s="266">
         <v>0</v>
       </c>
@@ -29084,6 +29084,22 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="AC25:AE25"/>
+    <mergeCell ref="AC6:AE6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="W32:W34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="L36:L41"/>
+    <mergeCell ref="L42:L45"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="L32:L34"/>
+    <mergeCell ref="M32:M34"/>
+    <mergeCell ref="R32:R34"/>
+    <mergeCell ref="S32:S34"/>
+    <mergeCell ref="T32:T34"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="C107:C110"/>
     <mergeCell ref="A109:A110"/>
@@ -29094,22 +29110,6 @@
     <mergeCell ref="A103:A104"/>
     <mergeCell ref="C103:C106"/>
     <mergeCell ref="A105:A106"/>
-    <mergeCell ref="W32:W34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="L36:L41"/>
-    <mergeCell ref="L42:L45"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="L32:L34"/>
-    <mergeCell ref="M32:M34"/>
-    <mergeCell ref="R32:R34"/>
-    <mergeCell ref="S32:S34"/>
-    <mergeCell ref="T32:T34"/>
-    <mergeCell ref="AC25:AE25"/>
-    <mergeCell ref="AC6:AE6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -49727,18 +49727,18 @@
         <f>FORECAST(CR93,CP94:CQ94,CP93:CQ93)</f>
         <v>93</v>
       </c>
-      <c r="DL94" s="431" t="s">
+      <c r="DL94" s="427" t="s">
         <v>762</v>
       </c>
-      <c r="DM94" s="431"/>
-      <c r="DN94" s="431" t="s">
+      <c r="DM94" s="427"/>
+      <c r="DN94" s="427" t="s">
         <v>763</v>
       </c>
-      <c r="DO94" s="431"/>
-      <c r="DP94" s="431" t="s">
+      <c r="DO94" s="427"/>
+      <c r="DP94" s="427" t="s">
         <v>761</v>
       </c>
-      <c r="DQ94" s="431"/>
+      <c r="DQ94" s="427"/>
     </row>
     <row r="95" spans="1:121" x14ac:dyDescent="0.25">
       <c r="BK95" t="s">
@@ -55199,7 +55199,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="18">
         <f ca="1">NOW()</f>
-        <v>45198.667928935189</v>
+        <v>45199.685924074074</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -56023,7 +56023,7 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
         <f ca="1">NOW()</f>
-        <v>45198.667928935189</v>
+        <v>45199.685924074074</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -58686,7 +58686,7 @@
   </sheetPr>
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
@@ -60135,8 +60135,8 @@
   </sheetPr>
   <dimension ref="A1:BA149"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="L97" sqref="L97"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62:I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -64510,10 +64510,22 @@
       <c r="E62" s="30">
         <v>0</v>
       </c>
-      <c r="F62" s="82"/>
-      <c r="G62" s="82"/>
-      <c r="H62" s="82"/>
-      <c r="I62" s="82"/>
+      <c r="F62" s="82">
+        <f>F61/2</f>
+        <v>14.13</v>
+      </c>
+      <c r="G62" s="82">
+        <f t="shared" ref="G62:I62" si="21">G61/2</f>
+        <v>14.13</v>
+      </c>
+      <c r="H62" s="82">
+        <f t="shared" si="21"/>
+        <v>14.13</v>
+      </c>
+      <c r="I62" s="82">
+        <f t="shared" si="21"/>
+        <v>14.13</v>
+      </c>
       <c r="J62" s="82"/>
       <c r="K62" s="82"/>
       <c r="L62" s="82"/>
@@ -64595,7 +64607,7 @@
         <v>0</v>
       </c>
       <c r="O63">
-        <f t="shared" ref="O63" si="21">N63</f>
+        <f t="shared" ref="O63" si="22">N63</f>
         <v>0</v>
       </c>
       <c r="P63"/>
@@ -64720,19 +64732,19 @@
         <v>0</v>
       </c>
       <c r="F65" s="82">
-        <f t="shared" ref="F65:I66" si="22">SUMIF($D$37:$D$42,$D65,F$37:F$42)*$E$54</f>
+        <f t="shared" ref="F65:I66" si="23">SUMIF($D$37:$D$42,$D65,F$37:F$42)*$E$54</f>
         <v>117.73934470134871</v>
       </c>
       <c r="G65" s="82">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>121.47218561739591</v>
       </c>
       <c r="H65" s="82">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>111.49620902079818</v>
       </c>
       <c r="I65" s="82">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>142.01096096333239</v>
       </c>
       <c r="J65" s="82">
@@ -64792,19 +64804,19 @@
         <v>0</v>
       </c>
       <c r="F66" s="82">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>106.47694185774681</v>
       </c>
       <c r="G66" s="82">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>106.47694185774681</v>
       </c>
       <c r="H66" s="82">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>106.47694185774681</v>
       </c>
       <c r="I66" s="82">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>106.47694185774681</v>
       </c>
       <c r="J66" s="82">
@@ -64967,11 +64979,11 @@
     </row>
     <row r="69" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="158" t="str">
-        <f t="shared" ref="A69:A76" si="23">"Extraction of "&amp;INDEX(FuelNamesLong,MATCH(D69,FuelNamesShort,0))</f>
+        <f t="shared" ref="A69:A76" si="24">"Extraction of "&amp;INDEX(FuelNamesLong,MATCH(D69,FuelNamesShort,0))</f>
         <v>Extraction of Biogas</v>
       </c>
       <c r="B69" s="30" t="str">
-        <f t="shared" ref="B69:B75" si="24">$B$46&amp;D69</f>
+        <f t="shared" ref="B69:B75" si="25">$B$46&amp;D69</f>
         <v>MINBIG</v>
       </c>
       <c r="D69" s="159" t="str">
@@ -64986,15 +64998,15 @@
         <v>59.346000000000004</v>
       </c>
       <c r="G69" s="82">
-        <f t="shared" ref="G69:I69" si="25">G71</f>
+        <f t="shared" ref="G69:I69" si="26">G71</f>
         <v>59.346000000000004</v>
       </c>
       <c r="H69" s="82">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>59.346000000000004</v>
       </c>
       <c r="I69" s="82">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>59.346000000000004</v>
       </c>
       <c r="J69" s="82"/>
@@ -65005,7 +65017,7 @@
       <c r="O69"/>
       <c r="P69"/>
       <c r="Q69" t="str">
-        <f t="shared" ref="Q69:Q76" si="26">$Q$60</f>
+        <f t="shared" ref="Q69:Q76" si="27">$Q$60</f>
         <v/>
       </c>
       <c r="V69" s="35"/>
@@ -65040,11 +65052,11 @@
     </row>
     <row r="70" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="158" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Extraction of Biomass bagasse</v>
       </c>
       <c r="B70" s="30" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>MINBIB</v>
       </c>
       <c r="D70" s="159" t="str">
@@ -65078,7 +65090,7 @@
       <c r="O70"/>
       <c r="P70"/>
       <c r="Q70" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="V70" s="35"/>
@@ -65113,11 +65125,11 @@
     </row>
     <row r="71" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="158" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Extraction of Biomass Other</v>
       </c>
       <c r="B71" s="30" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>MINBIO</v>
       </c>
       <c r="D71" s="159" t="str">
@@ -65128,19 +65140,19 @@
         <v>0</v>
       </c>
       <c r="F71" s="82">
-        <f t="shared" ref="F71:I71" si="27">F60*1.05</f>
+        <f t="shared" ref="F71:I71" si="28">F60*1.05</f>
         <v>59.346000000000004</v>
       </c>
       <c r="G71" s="82">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>59.346000000000004</v>
       </c>
       <c r="H71" s="82">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>59.346000000000004</v>
       </c>
       <c r="I71" s="82">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>59.346000000000004</v>
       </c>
       <c r="J71" s="82"/>
@@ -65151,7 +65163,7 @@
       <c r="O71"/>
       <c r="P71"/>
       <c r="Q71" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="V71" s="35"/>
@@ -65186,11 +65198,11 @@
     </row>
     <row r="72" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="158" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Extraction of Biomass Wood</v>
       </c>
       <c r="B72" s="30" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>MINBIW</v>
       </c>
       <c r="D72" s="159" t="str">
@@ -65205,15 +65217,15 @@
         <v>56.52</v>
       </c>
       <c r="G72" s="82">
-        <f t="shared" ref="G72:I73" si="28">F72</f>
+        <f t="shared" ref="G72:I73" si="29">F72</f>
         <v>56.52</v>
       </c>
       <c r="H72" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>56.52</v>
       </c>
       <c r="I72" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>56.52</v>
       </c>
       <c r="J72" s="82"/>
@@ -65224,7 +65236,7 @@
       <c r="O72"/>
       <c r="P72"/>
       <c r="Q72" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="V72" s="35"/>
@@ -65259,7 +65271,7 @@
     </row>
     <row r="73" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="158" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Extraction of Waste</v>
       </c>
       <c r="B73" s="30" t="str">
@@ -65277,15 +65289,15 @@
         <v>0</v>
       </c>
       <c r="G73" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="H73" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="I73" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="J73" s="82">
@@ -65300,7 +65312,7 @@
       <c r="O73"/>
       <c r="P73"/>
       <c r="Q73" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="V73" s="35"/>
@@ -65335,7 +65347,7 @@
     </row>
     <row r="74" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="158" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Extraction of Hydro</v>
       </c>
       <c r="B74" s="30" t="str">
@@ -65361,7 +65373,7 @@
       <c r="O74"/>
       <c r="P74"/>
       <c r="Q74" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="V74" s="35"/>
@@ -65396,11 +65408,11 @@
     </row>
     <row r="75" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="158" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Extraction of Solar</v>
       </c>
       <c r="B75" s="30" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>MINSOL</v>
       </c>
       <c r="D75" s="159" t="str">
@@ -65422,7 +65434,7 @@
       <c r="O75"/>
       <c r="P75"/>
       <c r="Q75" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="V75" s="35"/>
@@ -65457,7 +65469,7 @@
     </row>
     <row r="76" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="158" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Extraction of Wind</v>
       </c>
       <c r="B76" s="30" t="str">
@@ -65483,7 +65495,7 @@
       <c r="O76"/>
       <c r="P76"/>
       <c r="Q76" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="V76" s="35"/>
@@ -65566,7 +65578,7 @@
     </row>
     <row r="78" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="158" t="str">
-        <f t="shared" ref="A78:A92" si="29">"Imports of "&amp;INDEX(FuelNamesLong,MATCH(D78,FuelNamesShort,0))</f>
+        <f t="shared" ref="A78:A92" si="30">"Imports of "&amp;INDEX(FuelNamesLong,MATCH(D78,FuelNamesShort,0))</f>
         <v>Imports of Coal Coking</v>
       </c>
       <c r="B78" s="30" t="str">
@@ -65581,7 +65593,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="82">
-        <f t="shared" ref="F78" si="30">F60*1.5</f>
+        <f t="shared" ref="F78" si="31">F60*1.5</f>
         <v>84.78</v>
       </c>
       <c r="G78" s="82">
@@ -65589,11 +65601,11 @@
         <v>84.78</v>
       </c>
       <c r="H78" s="82">
-        <f t="shared" ref="H78:I78" si="31">H60*1.5</f>
+        <f t="shared" ref="H78:I78" si="32">H60*1.5</f>
         <v>84.78</v>
       </c>
       <c r="I78" s="82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>84.78</v>
       </c>
       <c r="J78" s="82">
@@ -65606,7 +65618,7 @@
       <c r="O78"/>
       <c r="P78"/>
       <c r="Q78" t="str">
-        <f t="shared" ref="Q78:Q92" si="32">$Q$60</f>
+        <f t="shared" ref="Q78:Q92" si="33">$Q$60</f>
         <v/>
       </c>
       <c r="V78" s="35"/>
@@ -65654,15 +65666,15 @@
         <v>8.7491242874264614</v>
       </c>
       <c r="G79" s="82">
-        <f t="shared" ref="G79:I79" si="33">G80/G15</f>
+        <f t="shared" ref="G79:I79" si="34">G80/G15</f>
         <v>9.0144883767620421</v>
       </c>
       <c r="H79" s="82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>8.3053057450005809</v>
       </c>
       <c r="I79" s="82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>10.474570265682702</v>
       </c>
       <c r="J79" s="82"/>
@@ -65705,7 +65717,7 @@
     </row>
     <row r="80" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="158" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Imports of Gas Regional LNG</v>
       </c>
       <c r="B80" s="30" t="str">
@@ -65720,19 +65732,19 @@
         <v>0</v>
       </c>
       <c r="F80" s="82">
-        <f t="shared" ref="F80:I81" si="34">SUMIF($C$37:$C$42,$B80,F$37:F$42)*$E$54</f>
+        <f t="shared" ref="F80:I81" si="35">SUMIF($C$37:$C$42,$B80,F$37:F$42)*$E$54</f>
         <v>143.92309452816528</v>
       </c>
       <c r="G80" s="82">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>148.28833379773559</v>
       </c>
       <c r="H80" s="82">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>136.62227950525954</v>
       </c>
       <c r="I80" s="82">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>172.30668087048045</v>
       </c>
       <c r="J80" s="82"/>
@@ -65745,7 +65757,7 @@
         <v>2027</v>
       </c>
       <c r="Q80" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="V80" s="35"/>
@@ -65780,7 +65792,7 @@
     </row>
     <row r="81" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="158" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Imports of Gas International LNG</v>
       </c>
       <c r="B81" s="30" t="str">
@@ -65795,19 +65807,19 @@
         <v>0</v>
       </c>
       <c r="F81" s="82">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>150.16006135280986</v>
       </c>
       <c r="G81" s="82">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>154.52530062238017</v>
       </c>
       <c r="H81" s="82">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>142.85924632990407</v>
       </c>
       <c r="I81" s="82">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>178.543647695125</v>
       </c>
       <c r="J81" s="82" t="s">
@@ -65830,7 +65842,7 @@
         <v>2027</v>
       </c>
       <c r="Q81" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="U81" s="161"/>
@@ -65879,15 +65891,15 @@
         <v>9.1282712068577432</v>
       </c>
       <c r="G82" s="82">
-        <f t="shared" ref="G82:I82" si="35">G81/G15</f>
+        <f t="shared" ref="G82:I82" si="36">G81/G15</f>
         <v>9.3936352961933238</v>
       </c>
       <c r="H82" s="82">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>8.6844526644318591</v>
       </c>
       <c r="I82" s="82">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>10.853717185113982</v>
       </c>
       <c r="J82" s="82"/>
@@ -65931,11 +65943,11 @@
     </row>
     <row r="83" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="158" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Imports of Nuclear</v>
       </c>
       <c r="B83" s="30" t="str">
-        <f t="shared" ref="B83:B91" si="36">"IMP"&amp;D83</f>
+        <f t="shared" ref="B83:B91" si="37">"IMP"&amp;D83</f>
         <v>IMPNUC</v>
       </c>
       <c r="D83" s="159" t="str">
@@ -65965,7 +65977,7 @@
         <v>0</v>
       </c>
       <c r="K83" s="82">
-        <f t="shared" ref="K83:K85" si="37">SUMIF($C$8:$AZ$8,D83,$C$11:$AZ$11)</f>
+        <f t="shared" ref="K83:K85" si="38">SUMIF($C$8:$AZ$8,D83,$C$11:$AZ$11)</f>
         <v>170.374545454545</v>
       </c>
       <c r="L83" s="82"/>
@@ -65974,7 +65986,7 @@
       <c r="O83"/>
       <c r="P83"/>
       <c r="Q83" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="T83" s="161" t="s">
@@ -66012,11 +66024,11 @@
     </row>
     <row r="84" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="158" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Imports of Oil Av Gasoline</v>
       </c>
       <c r="B84" s="30" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>IMPOAG</v>
       </c>
       <c r="D84" s="159" t="str">
@@ -66027,26 +66039,26 @@
         <v>0</v>
       </c>
       <c r="F84" s="82">
-        <f t="shared" ref="F84:I84" si="38">F87</f>
+        <f t="shared" ref="F84:I84" si="39">F87</f>
         <v>247.03405739193275</v>
       </c>
       <c r="G84" s="82">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>253.06623635843414</v>
       </c>
       <c r="H84" s="82">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>232.71621829347131</v>
       </c>
       <c r="I84" s="82">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>294.96333237453405</v>
       </c>
       <c r="J84" s="82">
         <v>0</v>
       </c>
       <c r="K84" s="82">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>1.394321535205479</v>
       </c>
       <c r="L84" s="82"/>
@@ -66055,7 +66067,7 @@
       <c r="O84"/>
       <c r="P84"/>
       <c r="Q84" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="V84" s="35"/>
@@ -66090,11 +66102,11 @@
     </row>
     <row r="85" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="158" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Imports of Oil Crude</v>
       </c>
       <c r="B85" s="30" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>IMPOCR</v>
       </c>
       <c r="D85" s="159" t="str">
@@ -66105,26 +66117,26 @@
         <v>0</v>
       </c>
       <c r="F85" s="82">
-        <f t="shared" ref="F85:I90" si="39">SUMIF($E$22:$E$34,$D85,F$22:F$34)</f>
+        <f t="shared" ref="F85:I90" si="40">SUMIF($E$22:$E$34,$D85,F$22:F$34)</f>
         <v>196.45298120195667</v>
       </c>
       <c r="G85" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>202.68138113207547</v>
       </c>
       <c r="H85" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>186.03605031446543</v>
       </c>
       <c r="I85" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>236.95117987421381</v>
       </c>
       <c r="J85" s="82">
         <v>0</v>
       </c>
       <c r="K85" s="82">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>941.22622485351599</v>
       </c>
       <c r="L85" s="82"/>
@@ -66133,7 +66145,7 @@
       <c r="O85"/>
       <c r="P85"/>
       <c r="Q85" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="V85" s="35"/>
@@ -66168,11 +66180,11 @@
     </row>
     <row r="86" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="158" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Imports of Oil Diesel</v>
       </c>
       <c r="B86" s="30" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>IMPODS</v>
       </c>
       <c r="D86" s="159" t="str">
@@ -66183,19 +66195,19 @@
         <v>0</v>
       </c>
       <c r="F86" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>236.56389169057414</v>
       </c>
       <c r="G86" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>244.65407088700817</v>
       </c>
       <c r="H86" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>224.41968109431471</v>
       </c>
       <c r="I86" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>286.31310869549469</v>
       </c>
       <c r="J86" s="82">
@@ -66210,7 +66222,7 @@
       <c r="O86"/>
       <c r="P86"/>
       <c r="Q86" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="V86" s="35"/>
@@ -66245,11 +66257,11 @@
     </row>
     <row r="87" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="158" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Imports of Oil Gasoline</v>
       </c>
       <c r="B87" s="30" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>IMPOGS</v>
       </c>
       <c r="D87" s="159" t="str">
@@ -66260,19 +66272,19 @@
         <v>0</v>
       </c>
       <c r="F87" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>247.03405739193275</v>
       </c>
       <c r="G87" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>253.06623635843414</v>
       </c>
       <c r="H87" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>232.71621829347131</v>
       </c>
       <c r="I87" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>294.96333237453405</v>
       </c>
       <c r="J87" s="82">
@@ -66287,7 +66299,7 @@
       <c r="O87"/>
       <c r="P87"/>
       <c r="Q87" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="V87" s="35"/>
@@ -66322,11 +66334,11 @@
     </row>
     <row r="88" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="158" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Imports of Oil HFO</v>
       </c>
       <c r="B88" s="30" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>IMPOHF</v>
       </c>
       <c r="D88" s="159" t="str">
@@ -66337,19 +66349,19 @@
         <v>0</v>
       </c>
       <c r="F88" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>196.45298120195667</v>
       </c>
       <c r="G88" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>202.68138113207547</v>
       </c>
       <c r="H88" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>186.03605031446543</v>
       </c>
       <c r="I88" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>236.95117987421381</v>
       </c>
       <c r="J88" s="82">
@@ -66364,7 +66376,7 @@
       <c r="O88"/>
       <c r="P88"/>
       <c r="Q88" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="V88" s="35"/>
@@ -66399,11 +66411,11 @@
     </row>
     <row r="89" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="158" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Imports of Oil LPG</v>
       </c>
       <c r="B89" s="30" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>IMPOLP</v>
       </c>
       <c r="D89" s="159" t="str">
@@ -66414,19 +66426,19 @@
         <v>0</v>
       </c>
       <c r="F89" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>376.62224144497708</v>
       </c>
       <c r="G89" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>382.94989907290471</v>
       </c>
       <c r="H89" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>366.03930314149977</v>
       </c>
       <c r="I89" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>417.76583187285604</v>
       </c>
       <c r="J89" s="82">
@@ -66441,7 +66453,7 @@
       <c r="O89"/>
       <c r="P89"/>
       <c r="Q89" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="V89" s="35"/>
@@ -66476,11 +66488,11 @@
     </row>
     <row r="90" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="158" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Imports of Oil Kerosene</v>
       </c>
       <c r="B90" s="30" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>IMPOKE</v>
       </c>
       <c r="D90" s="159" t="str">
@@ -66491,19 +66503,19 @@
         <v>0</v>
       </c>
       <c r="F90" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>243.45484454706207</v>
       </c>
       <c r="G90" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>250.76740309449676</v>
       </c>
       <c r="H90" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>231.22467020790273</v>
       </c>
       <c r="I90" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>291.00244139042559</v>
       </c>
       <c r="J90" s="82">
@@ -66518,7 +66530,7 @@
       <c r="O90"/>
       <c r="P90"/>
       <c r="Q90" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="V90" s="35"/>
@@ -66553,11 +66565,11 @@
     </row>
     <row r="91" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="158" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Imports of Biodiesel</v>
       </c>
       <c r="B91" s="30" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>IMPBID</v>
       </c>
       <c r="D91" s="159" t="str">
@@ -66572,15 +66584,15 @@
         <v>248.39208627510286</v>
       </c>
       <c r="G91" s="82">
-        <f t="shared" ref="G91:I92" si="40">G86*1.05</f>
+        <f t="shared" ref="G91:I92" si="41">G86*1.05</f>
         <v>256.88677443135862</v>
       </c>
       <c r="H91" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>235.64066514903047</v>
       </c>
       <c r="I91" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>300.62876413026942</v>
       </c>
       <c r="J91" s="82">
@@ -66593,7 +66605,7 @@
       <c r="O91"/>
       <c r="P91"/>
       <c r="Q91" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="V91" s="35"/>
@@ -66628,7 +66640,7 @@
     </row>
     <row r="92" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="158" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Imports of Bioethanol</v>
       </c>
       <c r="B92" s="30" t="str">
@@ -66647,15 +66659,15 @@
         <v>259.38576026152941</v>
       </c>
       <c r="G92" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>265.71954817635583</v>
       </c>
       <c r="H92" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>244.3520292081449</v>
       </c>
       <c r="I92" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>309.71149899326076</v>
       </c>
       <c r="J92" s="82">
@@ -66668,7 +66680,7 @@
       <c r="O92"/>
       <c r="P92"/>
       <c r="Q92" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="V92" s="35"/>
@@ -66844,15 +66856,15 @@
         <v>125.48506135280986</v>
       </c>
       <c r="G95" s="82">
-        <f t="shared" ref="G95:I95" si="41">G81-(1.5*G15)</f>
+        <f t="shared" ref="G95:I95" si="42">G81-(1.5*G15)</f>
         <v>129.85030062238019</v>
       </c>
       <c r="H95" s="82">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>118.18424632990407</v>
       </c>
       <c r="I95" s="82">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>153.86864769512499</v>
       </c>
       <c r="J95" s="82"/>
@@ -66949,11 +66961,11 @@
     </row>
     <row r="97" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="158" t="str">
-        <f t="shared" ref="A97:A104" si="42">"Exports of "&amp;INDEX(FuelNamesLong,MATCH(C97,FuelNamesShort,0))</f>
+        <f t="shared" ref="A97:A104" si="43">"Exports of "&amp;INDEX(FuelNamesLong,MATCH(C97,FuelNamesShort,0))</f>
         <v>Exports of Coal</v>
       </c>
       <c r="B97" s="30" t="str">
-        <f t="shared" ref="B97:B104" si="43">"PEX"&amp;C97</f>
+        <f t="shared" ref="B97:B104" si="44">"PEX"&amp;C97</f>
         <v>PEXCOA</v>
       </c>
       <c r="C97" s="159" t="str">
@@ -66995,7 +67007,7 @@
       </c>
       <c r="P97"/>
       <c r="Q97" t="str">
-        <f t="shared" ref="Q97:Q104" si="44">$Q$60</f>
+        <f t="shared" ref="Q97:Q104" si="45">$Q$60</f>
         <v/>
       </c>
       <c r="V97" s="35"/>
@@ -67030,11 +67042,11 @@
     </row>
     <row r="98" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="158" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>Exports of Coal Coking</v>
       </c>
       <c r="B98" s="30" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>PEXCOK</v>
       </c>
       <c r="C98" s="159" t="str">
@@ -67073,7 +67085,7 @@
       <c r="O98"/>
       <c r="P98"/>
       <c r="Q98" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="V98" s="35"/>
@@ -67108,11 +67120,11 @@
     </row>
     <row r="99" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="158" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>Exports of Oil Av Gasoline</v>
       </c>
       <c r="B99" s="30" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>PEXOAG</v>
       </c>
       <c r="C99" s="159" t="str">
@@ -67123,19 +67135,19 @@
         <v>0</v>
       </c>
       <c r="F99" s="82">
-        <f t="shared" ref="F99:I99" si="45">F102</f>
+        <f t="shared" ref="F99:I99" si="46">F102</f>
         <v>-234.68235452233611</v>
       </c>
       <c r="G99" s="82">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>-240.41292454051242</v>
       </c>
       <c r="H99" s="82">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>-221.08040737879773</v>
       </c>
       <c r="I99" s="82">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>-280.21516575580733</v>
       </c>
       <c r="J99" s="82">
@@ -67151,7 +67163,7 @@
       <c r="O99"/>
       <c r="P99"/>
       <c r="Q99" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="V99" s="35"/>
@@ -67186,11 +67198,11 @@
     </row>
     <row r="100" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="158" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>Exports of Oil Crude</v>
       </c>
       <c r="B100" s="30" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>PEXOCR</v>
       </c>
       <c r="C100" s="159" t="str">
@@ -67201,19 +67213,19 @@
         <v>0</v>
       </c>
       <c r="F100" s="82">
-        <f t="shared" ref="F100:I104" si="46">SUMIF($E$22:$E$34,$C100,F$22:F$34)*$B$96</f>
+        <f t="shared" ref="F100:I104" si="47">SUMIF($E$22:$E$34,$C100,F$22:F$34)*$B$96</f>
         <v>-186.63033214185884</v>
       </c>
       <c r="G100" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-192.54731207547169</v>
       </c>
       <c r="H100" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-176.73424779874216</v>
       </c>
       <c r="I100" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-225.10362088050312</v>
       </c>
       <c r="J100" s="82">
@@ -67229,7 +67241,7 @@
       <c r="O100"/>
       <c r="P100"/>
       <c r="Q100" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="V100" s="35"/>
@@ -67264,11 +67276,11 @@
     </row>
     <row r="101" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="158" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>Exports of Oil Diesel</v>
       </c>
       <c r="B101" s="30" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>PEXODS</v>
       </c>
       <c r="C101" s="159" t="str">
@@ -67279,19 +67291,19 @@
         <v>0</v>
       </c>
       <c r="F101" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-224.73569710604542</v>
       </c>
       <c r="G101" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-232.42136734265776</v>
       </c>
       <c r="H101" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-213.19869703959895</v>
       </c>
       <c r="I101" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-271.99745326071996</v>
       </c>
       <c r="J101" s="82">
@@ -67307,7 +67319,7 @@
       <c r="O101"/>
       <c r="P101"/>
       <c r="Q101" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="V101" s="35"/>
@@ -67342,11 +67354,11 @@
     </row>
     <row r="102" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="158" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>Exports of Oil Gasoline</v>
       </c>
       <c r="B102" s="30" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>PEXOGS</v>
       </c>
       <c r="C102" s="159" t="str">
@@ -67357,19 +67369,19 @@
         <v>0</v>
       </c>
       <c r="F102" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-234.68235452233611</v>
       </c>
       <c r="G102" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-240.41292454051242</v>
       </c>
       <c r="H102" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-221.08040737879773</v>
       </c>
       <c r="I102" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-280.21516575580733</v>
       </c>
       <c r="J102" s="82">
@@ -67385,7 +67397,7 @@
       <c r="O102"/>
       <c r="P102"/>
       <c r="Q102" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="V102" s="35"/>
@@ -67420,11 +67432,11 @@
     </row>
     <row r="103" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="158" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>Exports of Oil HFO</v>
       </c>
       <c r="B103" s="30" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>PEXOHF</v>
       </c>
       <c r="C103" s="159" t="str">
@@ -67435,19 +67447,19 @@
         <v>0</v>
       </c>
       <c r="F103" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-186.63033214185884</v>
       </c>
       <c r="G103" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-192.54731207547169</v>
       </c>
       <c r="H103" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-176.73424779874216</v>
       </c>
       <c r="I103" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-225.10362088050312</v>
       </c>
       <c r="J103" s="82">
@@ -67460,7 +67472,7 @@
       <c r="O103"/>
       <c r="P103"/>
       <c r="Q103" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="V103" s="35"/>
@@ -67495,11 +67507,11 @@
     </row>
     <row r="104" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="158" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>Exports of Oil Kerosene</v>
       </c>
       <c r="B104" s="30" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>PEXOKE</v>
       </c>
       <c r="C104" s="159" t="str">
@@ -67510,19 +67522,19 @@
         <v>0</v>
       </c>
       <c r="F104" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-231.28210231970894</v>
       </c>
       <c r="G104" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-238.22903293977191</v>
       </c>
       <c r="H104" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-219.66343669750759</v>
       </c>
       <c r="I104" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-276.45231932090428</v>
       </c>
       <c r="J104" s="82">
@@ -67538,7 +67550,7 @@
       <c r="O104"/>
       <c r="P104"/>
       <c r="Q104" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="V104" s="35"/>

</xml_diff>

<commit_message>
INDOMU added to model
</commit_message>
<xml_diff>
--- a/VT_REGION1_SUP.xlsx
+++ b/VT_REGION1_SUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74A8BAF-EA94-4778-BED4-771ECE671DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F580CBE-EB58-46E3-8E4F-F6648C2BA0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="26610" windowHeight="13740" firstSheet="4" activeTab="6" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="26610" windowHeight="13740" firstSheet="5" activeTab="11" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
     <definedName name="_AtRisk_SimSetting_StdRecalcBehavior" hidden="1">0</definedName>
     <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStatic" hidden="1">0</definedName>
     <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStaticPercentile" hidden="1">0.5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">FuelTechs!$B$8:$AA$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">FuelTechs!$B$8:$AA$64</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NameConv!#REF!</definedName>
     <definedName name="AGR">[1]Index!$C$7</definedName>
     <definedName name="COM">[1]Index!$C$8</definedName>
@@ -82,9 +82,9 @@
     <definedName name="emissions_start">[3]NameConv!$AY$4</definedName>
     <definedName name="emissions_types">[3]NameConv!$AX$3</definedName>
     <definedName name="eps">NameConv!$D$2</definedName>
-    <definedName name="FuelNames">NameConv!$B$5:$C$46</definedName>
-    <definedName name="FuelNamesLong">NameConv!$B$5:$B$46</definedName>
-    <definedName name="FuelNamesShort">NameConv!$C$5:$C$46</definedName>
+    <definedName name="FuelNames">NameConv!$B$5:$C$47</definedName>
+    <definedName name="FuelNamesLong">NameConv!$B$5:$B$47</definedName>
+    <definedName name="FuelNamesShort">NameConv!$C$5:$C$47</definedName>
     <definedName name="gwpch4">'[2]SASOL CC 2019 report'!$E$98</definedName>
     <definedName name="gwpn2o">'[2]SASOL CC 2019 report'!$E$97</definedName>
     <definedName name="H2.LHV.MJ_kg">'[3]Hydrogen-ELT'!$D$39</definedName>
@@ -135,9 +135,9 @@
     <definedName name="Sector.Transport">[3]Index!$G$2</definedName>
     <definedName name="sector_prefix" localSheetId="8">GasPipeLines!#REF!</definedName>
     <definedName name="sector_prefix">LNG!#REF!</definedName>
-    <definedName name="SectorNames">NameConv!$B$51:$C$59</definedName>
-    <definedName name="SectorNamesLong">NameConv!$C$51:$C$59</definedName>
-    <definedName name="SectorNamesShort">NameConv!$B$51:$B$59</definedName>
+    <definedName name="SectorNames">NameConv!$B$52:$C$60</definedName>
+    <definedName name="SectorNamesLong">NameConv!$C$52:$C$60</definedName>
+    <definedName name="SectorNamesShort">NameConv!$B$52:$B$60</definedName>
     <definedName name="solver_eng" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="6" hidden="1">0</definedName>
@@ -1631,7 +1631,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="1105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2652" uniqueCount="1107">
   <si>
     <t>Agriculture</t>
   </si>
@@ -5105,6 +5105,12 @@
   </si>
   <si>
     <t>PM10S</t>
+  </si>
+  <si>
+    <t>OMU</t>
+  </si>
+  <si>
+    <t>Oil HFO for material use</t>
   </si>
 </sst>
 </file>
@@ -29858,10 +29864,10 @@
   <sheetPr codeName="Sheet12">
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:AE117"/>
+  <dimension ref="A1:AE118"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="K46" workbookViewId="0">
+      <selection activeCell="T52" sqref="T52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -30116,7 +30122,7 @@
         <v>INDBIB</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" ref="E9:E63" si="0">INDEX(SectorNamesLong,MATCH(B9,SectorNamesShort,0))&amp;" "&amp;INDEX(FuelNamesLong,MATCH(C9,FuelNamesShort,0))</f>
+        <f t="shared" ref="E9:E64" si="0">INDEX(SectorNamesLong,MATCH(B9,SectorNamesShort,0))&amp;" "&amp;INDEX(FuelNamesLong,MATCH(C9,FuelNamesShort,0))</f>
         <v>Industry Biomass bagasse</v>
       </c>
       <c r="F9" t="s">
@@ -30183,7 +30189,7 @@
         <v>148</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" ref="D10:D63" si="1">B10&amp;C10</f>
+        <f t="shared" ref="D10:D64" si="1">B10&amp;C10</f>
         <v>UPSBID</v>
       </c>
       <c r="E10" t="str">
@@ -30198,11 +30204,11 @@
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10" t="str">
-        <f t="shared" ref="K10:K63" si="2">"X"&amp;D10</f>
+        <f t="shared" ref="K10:K64" si="2">"X"&amp;D10</f>
         <v>XUPSBID</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" ref="L10:L63" si="3">E10</f>
+        <f t="shared" ref="L10:L64" si="3">E10</f>
         <v>Upstream Biodiesel</v>
       </c>
       <c r="M10" t="s">
@@ -30220,11 +30226,11 @@
       <c r="Q10"/>
       <c r="R10"/>
       <c r="S10" t="str">
-        <f t="shared" ref="S10:S63" si="4">K10</f>
+        <f t="shared" ref="S10:S64" si="4">K10</f>
         <v>XUPSBID</v>
       </c>
       <c r="T10" t="str">
-        <f t="shared" ref="T10:U63" si="5">C10</f>
+        <f t="shared" ref="T10:U64" si="5">C10</f>
         <v>BID</v>
       </c>
       <c r="U10" t="str">
@@ -33138,18 +33144,18 @@
     </row>
     <row r="52" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>210</v>
+        <v>1105</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" si="1"/>
-        <v>TRAOHF</v>
+        <f t="shared" ref="D52" si="40">B52&amp;C52</f>
+        <v>INDOMU</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="0"/>
-        <v>Transport Oil HFO</v>
+        <f t="shared" ref="E52" si="41">INDEX(SectorNamesLong,MATCH(B52,SectorNamesShort,0))&amp;" "&amp;INDEX(FuelNamesLong,MATCH(C52,FuelNamesShort,0))</f>
+        <v>Industry Oil HFO for material use</v>
       </c>
       <c r="F52" t="s">
         <v>239</v>
@@ -33159,12 +33165,12 @@
       <c r="I52"/>
       <c r="J52"/>
       <c r="K52" t="str">
-        <f t="shared" si="2"/>
-        <v>XTRAOHF</v>
+        <f t="shared" ref="K52" si="42">"X"&amp;D52</f>
+        <v>XINDOMU</v>
       </c>
       <c r="L52" t="str">
-        <f t="shared" si="3"/>
-        <v>Transport Oil HFO</v>
+        <f t="shared" ref="L52" si="43">E52</f>
+        <v>Industry Oil HFO for material use</v>
       </c>
       <c r="M52" t="s">
         <v>239</v>
@@ -33181,16 +33187,15 @@
       <c r="Q52"/>
       <c r="R52"/>
       <c r="S52" t="str">
-        <f t="shared" si="4"/>
-        <v>XTRAOHF</v>
-      </c>
-      <c r="T52" t="str">
-        <f t="shared" si="5"/>
-        <v>OHF</v>
+        <f t="shared" ref="S52" si="44">K52</f>
+        <v>XINDOMU</v>
+      </c>
+      <c r="T52" s="237" t="s">
+        <v>210</v>
       </c>
       <c r="U52" t="str">
-        <f t="shared" si="5"/>
-        <v>TRAOHF</v>
+        <f t="shared" ref="U52" si="45">D52</f>
+        <v>INDOMU</v>
       </c>
       <c r="V52">
         <v>1</v>
@@ -33209,18 +33214,18 @@
     </row>
     <row r="53" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C53" t="s">
         <v>210</v>
       </c>
       <c r="D53" t="str">
-        <f t="shared" ref="D53" si="40">B53&amp;C53</f>
-        <v>PWROHF</v>
+        <f t="shared" si="1"/>
+        <v>TRAOHF</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" ref="E53" si="41">INDEX(SectorNamesLong,MATCH(B53,SectorNamesShort,0))&amp;" "&amp;INDEX(FuelNamesLong,MATCH(C53,FuelNamesShort,0))</f>
-        <v>Power Oil HFO</v>
+        <f t="shared" si="0"/>
+        <v>Transport Oil HFO</v>
       </c>
       <c r="F53" t="s">
         <v>239</v>
@@ -33230,12 +33235,12 @@
       <c r="I53"/>
       <c r="J53"/>
       <c r="K53" t="str">
-        <f t="shared" ref="K53" si="42">"X"&amp;D53</f>
-        <v>XPWROHF</v>
+        <f t="shared" si="2"/>
+        <v>XTRAOHF</v>
       </c>
       <c r="L53" t="str">
-        <f t="shared" ref="L53" si="43">E53</f>
-        <v>Power Oil HFO</v>
+        <f t="shared" si="3"/>
+        <v>Transport Oil HFO</v>
       </c>
       <c r="M53" t="s">
         <v>239</v>
@@ -33252,16 +33257,16 @@
       <c r="Q53"/>
       <c r="R53"/>
       <c r="S53" t="str">
-        <f t="shared" ref="S53" si="44">K53</f>
-        <v>XPWROHF</v>
+        <f t="shared" si="4"/>
+        <v>XTRAOHF</v>
       </c>
       <c r="T53" t="str">
-        <f t="shared" ref="T53" si="45">C53</f>
+        <f t="shared" si="5"/>
         <v>OHF</v>
       </c>
       <c r="U53" t="str">
-        <f t="shared" ref="U53" si="46">D53</f>
-        <v>PWROHF</v>
+        <f t="shared" si="5"/>
+        <v>TRAOHF</v>
       </c>
       <c r="V53">
         <v>1</v>
@@ -33280,18 +33285,18 @@
     </row>
     <row r="54" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C54" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D54" t="str">
-        <f t="shared" si="1"/>
-        <v>AGROKE</v>
+        <f t="shared" ref="D54" si="46">B54&amp;C54</f>
+        <v>PWROHF</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="0"/>
-        <v>Agriculture Oil Kerosene</v>
+        <f t="shared" ref="E54" si="47">INDEX(SectorNamesLong,MATCH(B54,SectorNamesShort,0))&amp;" "&amp;INDEX(FuelNamesLong,MATCH(C54,FuelNamesShort,0))</f>
+        <v>Power Oil HFO</v>
       </c>
       <c r="F54" t="s">
         <v>239</v>
@@ -33301,12 +33306,12 @@
       <c r="I54"/>
       <c r="J54"/>
       <c r="K54" t="str">
-        <f t="shared" si="2"/>
-        <v>XAGROKE</v>
+        <f t="shared" ref="K54" si="48">"X"&amp;D54</f>
+        <v>XPWROHF</v>
       </c>
       <c r="L54" t="str">
-        <f t="shared" si="3"/>
-        <v>Agriculture Oil Kerosene</v>
+        <f t="shared" ref="L54" si="49">E54</f>
+        <v>Power Oil HFO</v>
       </c>
       <c r="M54" t="s">
         <v>239</v>
@@ -33323,16 +33328,16 @@
       <c r="Q54"/>
       <c r="R54"/>
       <c r="S54" t="str">
-        <f t="shared" si="4"/>
-        <v>XAGROKE</v>
+        <f t="shared" ref="S54" si="50">K54</f>
+        <v>XPWROHF</v>
       </c>
       <c r="T54" t="str">
-        <f t="shared" si="5"/>
-        <v>OKE</v>
+        <f t="shared" ref="T54" si="51">C54</f>
+        <v>OHF</v>
       </c>
       <c r="U54" t="str">
-        <f t="shared" si="5"/>
-        <v>AGROKE</v>
+        <f t="shared" ref="U54" si="52">D54</f>
+        <v>PWROHF</v>
       </c>
       <c r="V54">
         <v>1</v>
@@ -33351,18 +33356,18 @@
     </row>
     <row r="55" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C55" t="s">
         <v>212</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="1"/>
-        <v>COMOKE</v>
+        <v>AGROKE</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
-        <v>Commerce Oil Kerosene</v>
+        <v>Agriculture Oil Kerosene</v>
       </c>
       <c r="F55" t="s">
         <v>239</v>
@@ -33373,11 +33378,11 @@
       <c r="J55"/>
       <c r="K55" t="str">
         <f t="shared" si="2"/>
-        <v>XCOMOKE</v>
+        <v>XAGROKE</v>
       </c>
       <c r="L55" t="str">
         <f t="shared" si="3"/>
-        <v>Commerce Oil Kerosene</v>
+        <v>Agriculture Oil Kerosene</v>
       </c>
       <c r="M55" t="s">
         <v>239</v>
@@ -33395,7 +33400,7 @@
       <c r="R55"/>
       <c r="S55" t="str">
         <f t="shared" si="4"/>
-        <v>XCOMOKE</v>
+        <v>XAGROKE</v>
       </c>
       <c r="T55" t="str">
         <f t="shared" si="5"/>
@@ -33403,7 +33408,7 @@
       </c>
       <c r="U55" t="str">
         <f t="shared" si="5"/>
-        <v>COMOKE</v>
+        <v>AGROKE</v>
       </c>
       <c r="V55">
         <v>1</v>
@@ -33422,18 +33427,18 @@
     </row>
     <row r="56" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
         <v>212</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="1"/>
-        <v>RESOKE</v>
+        <v>COMOKE</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
-        <v>Residential Oil Kerosene</v>
+        <v>Commerce Oil Kerosene</v>
       </c>
       <c r="F56" t="s">
         <v>239</v>
@@ -33444,11 +33449,11 @@
       <c r="J56"/>
       <c r="K56" t="str">
         <f t="shared" si="2"/>
-        <v>XRESOKE</v>
+        <v>XCOMOKE</v>
       </c>
       <c r="L56" t="str">
         <f t="shared" si="3"/>
-        <v>Residential Oil Kerosene</v>
+        <v>Commerce Oil Kerosene</v>
       </c>
       <c r="M56" t="s">
         <v>239</v>
@@ -33466,7 +33471,7 @@
       <c r="R56"/>
       <c r="S56" t="str">
         <f t="shared" si="4"/>
-        <v>XRESOKE</v>
+        <v>XCOMOKE</v>
       </c>
       <c r="T56" t="str">
         <f t="shared" si="5"/>
@@ -33474,7 +33479,7 @@
       </c>
       <c r="U56" t="str">
         <f t="shared" si="5"/>
-        <v>RESOKE</v>
+        <v>COMOKE</v>
       </c>
       <c r="V56">
         <v>1</v>
@@ -33493,18 +33498,18 @@
     </row>
     <row r="57" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C57" t="s">
         <v>212</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="1"/>
-        <v>TRAOKE</v>
+        <v>RESOKE</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
-        <v>Transport Oil Kerosene</v>
+        <v>Residential Oil Kerosene</v>
       </c>
       <c r="F57" t="s">
         <v>239</v>
@@ -33515,11 +33520,11 @@
       <c r="J57"/>
       <c r="K57" t="str">
         <f t="shared" si="2"/>
-        <v>XTRAOKE</v>
+        <v>XRESOKE</v>
       </c>
       <c r="L57" t="str">
         <f t="shared" si="3"/>
-        <v>Transport Oil Kerosene</v>
+        <v>Residential Oil Kerosene</v>
       </c>
       <c r="M57" t="s">
         <v>239</v>
@@ -33537,7 +33542,7 @@
       <c r="R57"/>
       <c r="S57" t="str">
         <f t="shared" si="4"/>
-        <v>XTRAOKE</v>
+        <v>XRESOKE</v>
       </c>
       <c r="T57" t="str">
         <f t="shared" si="5"/>
@@ -33545,7 +33550,7 @@
       </c>
       <c r="U57" t="str">
         <f t="shared" si="5"/>
-        <v>TRAOKE</v>
+        <v>RESOKE</v>
       </c>
       <c r="V57">
         <v>1</v>
@@ -33564,18 +33569,18 @@
     </row>
     <row r="58" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C58" t="s">
         <v>212</v>
       </c>
       <c r="D58" t="str">
-        <f t="shared" ref="D58" si="47">B58&amp;C58</f>
-        <v>PWROKE</v>
+        <f t="shared" si="1"/>
+        <v>TRAOKE</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" ref="E58" si="48">INDEX(SectorNamesLong,MATCH(B58,SectorNamesShort,0))&amp;" "&amp;INDEX(FuelNamesLong,MATCH(C58,FuelNamesShort,0))</f>
-        <v>Power Oil Kerosene</v>
+        <f t="shared" si="0"/>
+        <v>Transport Oil Kerosene</v>
       </c>
       <c r="F58" t="s">
         <v>239</v>
@@ -33585,12 +33590,12 @@
       <c r="I58"/>
       <c r="J58"/>
       <c r="K58" t="str">
-        <f t="shared" ref="K58" si="49">"X"&amp;D58</f>
-        <v>XPWROKE</v>
+        <f t="shared" si="2"/>
+        <v>XTRAOKE</v>
       </c>
       <c r="L58" t="str">
-        <f t="shared" ref="L58" si="50">E58</f>
-        <v>Power Oil Kerosene</v>
+        <f t="shared" si="3"/>
+        <v>Transport Oil Kerosene</v>
       </c>
       <c r="M58" t="s">
         <v>239</v>
@@ -33607,16 +33612,16 @@
       <c r="Q58"/>
       <c r="R58"/>
       <c r="S58" t="str">
-        <f t="shared" ref="S58" si="51">K58</f>
-        <v>XPWROKE</v>
+        <f t="shared" si="4"/>
+        <v>XTRAOKE</v>
       </c>
       <c r="T58" t="str">
-        <f t="shared" ref="T58" si="52">C58</f>
+        <f t="shared" si="5"/>
         <v>OKE</v>
       </c>
       <c r="U58" t="str">
-        <f t="shared" ref="U58" si="53">D58</f>
-        <v>PWROKE</v>
+        <f t="shared" si="5"/>
+        <v>TRAOKE</v>
       </c>
       <c r="V58">
         <v>1</v>
@@ -33635,18 +33640,18 @@
     </row>
     <row r="59" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C59" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" si="1"/>
-        <v>AGROLP</v>
+        <f t="shared" ref="D59" si="53">B59&amp;C59</f>
+        <v>PWROKE</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="0"/>
-        <v>Agriculture Oil LPG</v>
+        <f t="shared" ref="E59" si="54">INDEX(SectorNamesLong,MATCH(B59,SectorNamesShort,0))&amp;" "&amp;INDEX(FuelNamesLong,MATCH(C59,FuelNamesShort,0))</f>
+        <v>Power Oil Kerosene</v>
       </c>
       <c r="F59" t="s">
         <v>239</v>
@@ -33656,12 +33661,12 @@
       <c r="I59"/>
       <c r="J59"/>
       <c r="K59" t="str">
-        <f t="shared" si="2"/>
-        <v>XAGROLP</v>
+        <f t="shared" ref="K59" si="55">"X"&amp;D59</f>
+        <v>XPWROKE</v>
       </c>
       <c r="L59" t="str">
-        <f t="shared" si="3"/>
-        <v>Agriculture Oil LPG</v>
+        <f t="shared" ref="L59" si="56">E59</f>
+        <v>Power Oil Kerosene</v>
       </c>
       <c r="M59" t="s">
         <v>239</v>
@@ -33678,16 +33683,16 @@
       <c r="Q59"/>
       <c r="R59"/>
       <c r="S59" t="str">
-        <f t="shared" si="4"/>
-        <v>XAGROLP</v>
+        <f t="shared" ref="S59" si="57">K59</f>
+        <v>XPWROKE</v>
       </c>
       <c r="T59" t="str">
-        <f t="shared" si="5"/>
-        <v>OLP</v>
+        <f t="shared" ref="T59" si="58">C59</f>
+        <v>OKE</v>
       </c>
       <c r="U59" t="str">
-        <f t="shared" si="5"/>
-        <v>AGROLP</v>
+        <f t="shared" ref="U59" si="59">D59</f>
+        <v>PWROKE</v>
       </c>
       <c r="V59">
         <v>1</v>
@@ -33706,18 +33711,18 @@
     </row>
     <row r="60" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
         <v>214</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="1"/>
-        <v>COMOLP</v>
+        <v>AGROLP</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
-        <v>Commerce Oil LPG</v>
+        <v>Agriculture Oil LPG</v>
       </c>
       <c r="F60" t="s">
         <v>239</v>
@@ -33728,11 +33733,11 @@
       <c r="J60"/>
       <c r="K60" t="str">
         <f t="shared" si="2"/>
-        <v>XCOMOLP</v>
+        <v>XAGROLP</v>
       </c>
       <c r="L60" t="str">
         <f t="shared" si="3"/>
-        <v>Commerce Oil LPG</v>
+        <v>Agriculture Oil LPG</v>
       </c>
       <c r="M60" t="s">
         <v>239</v>
@@ -33750,7 +33755,7 @@
       <c r="R60"/>
       <c r="S60" t="str">
         <f t="shared" si="4"/>
-        <v>XCOMOLP</v>
+        <v>XAGROLP</v>
       </c>
       <c r="T60" t="str">
         <f t="shared" si="5"/>
@@ -33758,7 +33763,7 @@
       </c>
       <c r="U60" t="str">
         <f t="shared" si="5"/>
-        <v>COMOLP</v>
+        <v>AGROLP</v>
       </c>
       <c r="V60">
         <v>1</v>
@@ -33777,18 +33782,18 @@
     </row>
     <row r="61" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C61" t="s">
         <v>214</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="1"/>
-        <v>INDOLP</v>
+        <v>COMOLP</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="0"/>
-        <v>Industry Oil LPG</v>
+        <v>Commerce Oil LPG</v>
       </c>
       <c r="F61" t="s">
         <v>239</v>
@@ -33799,11 +33804,11 @@
       <c r="J61"/>
       <c r="K61" t="str">
         <f t="shared" si="2"/>
-        <v>XINDOLP</v>
+        <v>XCOMOLP</v>
       </c>
       <c r="L61" t="str">
         <f t="shared" si="3"/>
-        <v>Industry Oil LPG</v>
+        <v>Commerce Oil LPG</v>
       </c>
       <c r="M61" t="s">
         <v>239</v>
@@ -33821,7 +33826,7 @@
       <c r="R61"/>
       <c r="S61" t="str">
         <f t="shared" si="4"/>
-        <v>XINDOLP</v>
+        <v>XCOMOLP</v>
       </c>
       <c r="T61" t="str">
         <f t="shared" si="5"/>
@@ -33829,7 +33834,7 @@
       </c>
       <c r="U61" t="str">
         <f t="shared" si="5"/>
-        <v>INDOLP</v>
+        <v>COMOLP</v>
       </c>
       <c r="V61">
         <v>1</v>
@@ -33848,18 +33853,18 @@
     </row>
     <row r="62" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
         <v>214</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="1"/>
-        <v>RESOLP</v>
+        <v>INDOLP</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="0"/>
-        <v>Residential Oil LPG</v>
+        <v>Industry Oil LPG</v>
       </c>
       <c r="F62" t="s">
         <v>239</v>
@@ -33870,11 +33875,11 @@
       <c r="J62"/>
       <c r="K62" t="str">
         <f t="shared" si="2"/>
-        <v>XRESOLP</v>
+        <v>XINDOLP</v>
       </c>
       <c r="L62" t="str">
         <f t="shared" si="3"/>
-        <v>Residential Oil LPG</v>
+        <v>Industry Oil LPG</v>
       </c>
       <c r="M62" t="s">
         <v>239</v>
@@ -33892,7 +33897,7 @@
       <c r="R62"/>
       <c r="S62" t="str">
         <f t="shared" si="4"/>
-        <v>XRESOLP</v>
+        <v>XINDOLP</v>
       </c>
       <c r="T62" t="str">
         <f t="shared" si="5"/>
@@ -33900,7 +33905,7 @@
       </c>
       <c r="U62" t="str">
         <f t="shared" si="5"/>
-        <v>RESOLP</v>
+        <v>INDOLP</v>
       </c>
       <c r="V62">
         <v>1</v>
@@ -33919,18 +33924,18 @@
     </row>
     <row r="63" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="1"/>
-        <v>INDWAS</v>
+        <v>RESOLP</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="0"/>
-        <v>Industry Waste</v>
+        <v>Residential Oil LPG</v>
       </c>
       <c r="F63" t="s">
         <v>239</v>
@@ -33941,11 +33946,11 @@
       <c r="J63"/>
       <c r="K63" t="str">
         <f t="shared" si="2"/>
-        <v>XINDWAS</v>
+        <v>XRESOLP</v>
       </c>
       <c r="L63" t="str">
         <f t="shared" si="3"/>
-        <v>Industry Waste</v>
+        <v>Residential Oil LPG</v>
       </c>
       <c r="M63" t="s">
         <v>239</v>
@@ -33963,15 +33968,15 @@
       <c r="R63"/>
       <c r="S63" t="str">
         <f t="shared" si="4"/>
-        <v>XINDWAS</v>
+        <v>XRESOLP</v>
       </c>
       <c r="T63" t="str">
         <f t="shared" si="5"/>
-        <v>WAS</v>
+        <v>OLP</v>
       </c>
       <c r="U63" t="str">
         <f t="shared" si="5"/>
-        <v>INDWAS</v>
+        <v>RESOLP</v>
       </c>
       <c r="V63">
         <v>1</v>
@@ -33986,21 +33991,22 @@
       <c r="Z63">
         <v>1</v>
       </c>
+      <c r="AE63"/>
     </row>
     <row r="64" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D64" t="str">
-        <f t="shared" ref="D64:D69" si="54">B64&amp;C64</f>
-        <v>PWRSOL</v>
+        <f t="shared" si="1"/>
+        <v>INDWAS</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" ref="E64:E69" si="55">INDEX(SectorNamesLong,MATCH(B64,SectorNamesShort,0))&amp;" "&amp;INDEX(FuelNamesLong,MATCH(C64,FuelNamesShort,0))</f>
-        <v>Power Solar</v>
+        <f t="shared" si="0"/>
+        <v>Industry Waste</v>
       </c>
       <c r="F64" t="s">
         <v>239</v>
@@ -34010,12 +34016,12 @@
       <c r="I64"/>
       <c r="J64"/>
       <c r="K64" t="str">
-        <f t="shared" ref="K64:K69" si="56">"X"&amp;D64</f>
-        <v>XPWRSOL</v>
+        <f t="shared" si="2"/>
+        <v>XINDWAS</v>
       </c>
       <c r="L64" t="str">
-        <f t="shared" ref="L64:L69" si="57">E64</f>
-        <v>Power Solar</v>
+        <f t="shared" si="3"/>
+        <v>Industry Waste</v>
       </c>
       <c r="M64" t="s">
         <v>239</v>
@@ -34032,16 +34038,16 @@
       <c r="Q64"/>
       <c r="R64"/>
       <c r="S64" t="str">
-        <f t="shared" ref="S64:S69" si="58">K64</f>
-        <v>XPWRSOL</v>
+        <f t="shared" si="4"/>
+        <v>XINDWAS</v>
       </c>
       <c r="T64" t="str">
-        <f t="shared" ref="T64:T69" si="59">C64</f>
-        <v>SOL</v>
+        <f t="shared" si="5"/>
+        <v>WAS</v>
       </c>
       <c r="U64" t="str">
-        <f t="shared" ref="U64:U69" si="60">D64</f>
-        <v>PWRSOL</v>
+        <f t="shared" si="5"/>
+        <v>INDWAS</v>
       </c>
       <c r="V64">
         <v>1</v>
@@ -34062,15 +34068,15 @@
         <v>10</v>
       </c>
       <c r="C65" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D65" t="str">
-        <f t="shared" si="54"/>
-        <v>PWRWND</v>
+        <f t="shared" ref="D65:D70" si="60">B65&amp;C65</f>
+        <v>PWRSOL</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" si="55"/>
-        <v>Power Wind</v>
+        <f t="shared" ref="E65:E70" si="61">INDEX(SectorNamesLong,MATCH(B65,SectorNamesShort,0))&amp;" "&amp;INDEX(FuelNamesLong,MATCH(C65,FuelNamesShort,0))</f>
+        <v>Power Solar</v>
       </c>
       <c r="F65" t="s">
         <v>239</v>
@@ -34080,12 +34086,12 @@
       <c r="I65"/>
       <c r="J65"/>
       <c r="K65" t="str">
-        <f t="shared" si="56"/>
-        <v>XPWRWND</v>
+        <f t="shared" ref="K65:K70" si="62">"X"&amp;D65</f>
+        <v>XPWRSOL</v>
       </c>
       <c r="L65" t="str">
-        <f t="shared" si="57"/>
-        <v>Power Wind</v>
+        <f t="shared" ref="L65:L70" si="63">E65</f>
+        <v>Power Solar</v>
       </c>
       <c r="M65" t="s">
         <v>239</v>
@@ -34102,16 +34108,16 @@
       <c r="Q65"/>
       <c r="R65"/>
       <c r="S65" t="str">
-        <f t="shared" si="58"/>
-        <v>XPWRWND</v>
+        <f t="shared" ref="S65:S70" si="64">K65</f>
+        <v>XPWRSOL</v>
       </c>
       <c r="T65" t="str">
-        <f t="shared" si="59"/>
-        <v>WND</v>
+        <f t="shared" ref="T65:T70" si="65">C65</f>
+        <v>SOL</v>
       </c>
       <c r="U65" t="str">
-        <f t="shared" si="60"/>
-        <v>PWRWND</v>
+        <f t="shared" ref="U65:U70" si="66">D65</f>
+        <v>PWRSOL</v>
       </c>
       <c r="V65">
         <v>1</v>
@@ -34132,15 +34138,15 @@
         <v>10</v>
       </c>
       <c r="C66" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" si="54"/>
-        <v>PWRHYD</v>
+        <f t="shared" si="60"/>
+        <v>PWRWND</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" si="55"/>
-        <v>Power Hydro</v>
+        <f t="shared" si="61"/>
+        <v>Power Wind</v>
       </c>
       <c r="F66" t="s">
         <v>239</v>
@@ -34150,12 +34156,12 @@
       <c r="I66"/>
       <c r="J66"/>
       <c r="K66" t="str">
-        <f t="shared" si="56"/>
-        <v>XPWRHYD</v>
+        <f t="shared" si="62"/>
+        <v>XPWRWND</v>
       </c>
       <c r="L66" t="str">
-        <f t="shared" si="57"/>
-        <v>Power Hydro</v>
+        <f t="shared" si="63"/>
+        <v>Power Wind</v>
       </c>
       <c r="M66" t="s">
         <v>239</v>
@@ -34172,16 +34178,16 @@
       <c r="Q66"/>
       <c r="R66"/>
       <c r="S66" t="str">
-        <f t="shared" si="58"/>
-        <v>XPWRHYD</v>
+        <f t="shared" si="64"/>
+        <v>XPWRWND</v>
       </c>
       <c r="T66" t="str">
-        <f t="shared" si="59"/>
-        <v>HYD</v>
+        <f t="shared" si="65"/>
+        <v>WND</v>
       </c>
       <c r="U66" t="str">
-        <f t="shared" si="60"/>
-        <v>PWRHYD</v>
+        <f t="shared" si="66"/>
+        <v>PWRWND</v>
       </c>
       <c r="V66">
         <v>1</v>
@@ -34202,15 +34208,15 @@
         <v>10</v>
       </c>
       <c r="C67" t="s">
-        <v>152</v>
+        <v>196</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" si="54"/>
-        <v>PWRBIO</v>
+        <f t="shared" si="60"/>
+        <v>PWRHYD</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" si="55"/>
-        <v>Power Biomass Other</v>
+        <f t="shared" si="61"/>
+        <v>Power Hydro</v>
       </c>
       <c r="F67" t="s">
         <v>239</v>
@@ -34220,12 +34226,12 @@
       <c r="I67"/>
       <c r="J67"/>
       <c r="K67" t="str">
-        <f t="shared" si="56"/>
-        <v>XPWRBIO</v>
+        <f t="shared" si="62"/>
+        <v>XPWRHYD</v>
       </c>
       <c r="L67" t="str">
-        <f t="shared" si="57"/>
-        <v>Power Biomass Other</v>
+        <f t="shared" si="63"/>
+        <v>Power Hydro</v>
       </c>
       <c r="M67" t="s">
         <v>239</v>
@@ -34242,16 +34248,16 @@
       <c r="Q67"/>
       <c r="R67"/>
       <c r="S67" t="str">
-        <f t="shared" si="58"/>
-        <v>XPWRBIO</v>
+        <f t="shared" si="64"/>
+        <v>XPWRHYD</v>
       </c>
       <c r="T67" t="str">
-        <f t="shared" si="59"/>
-        <v>BIO</v>
+        <f t="shared" si="65"/>
+        <v>HYD</v>
       </c>
       <c r="U67" t="str">
-        <f t="shared" si="60"/>
-        <v>PWRBIO</v>
+        <f t="shared" si="66"/>
+        <v>PWRHYD</v>
       </c>
       <c r="V67">
         <v>1</v>
@@ -34272,15 +34278,15 @@
         <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>200</v>
+        <v>152</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" si="54"/>
-        <v>PWRNUC</v>
+        <f t="shared" si="60"/>
+        <v>PWRBIO</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="55"/>
-        <v>Power Nuclear</v>
+        <f t="shared" si="61"/>
+        <v>Power Biomass Other</v>
       </c>
       <c r="F68" t="s">
         <v>239</v>
@@ -34290,12 +34296,12 @@
       <c r="I68"/>
       <c r="J68"/>
       <c r="K68" t="str">
-        <f t="shared" si="56"/>
-        <v>XPWRNUC</v>
+        <f t="shared" si="62"/>
+        <v>XPWRBIO</v>
       </c>
       <c r="L68" t="str">
-        <f t="shared" si="57"/>
-        <v>Power Nuclear</v>
+        <f t="shared" si="63"/>
+        <v>Power Biomass Other</v>
       </c>
       <c r="M68" t="s">
         <v>239</v>
@@ -34312,16 +34318,16 @@
       <c r="Q68"/>
       <c r="R68"/>
       <c r="S68" t="str">
-        <f t="shared" si="58"/>
-        <v>XPWRNUC</v>
+        <f t="shared" si="64"/>
+        <v>XPWRBIO</v>
       </c>
       <c r="T68" t="str">
-        <f t="shared" si="59"/>
-        <v>NUC</v>
+        <f t="shared" si="65"/>
+        <v>BIO</v>
       </c>
       <c r="U68" t="str">
-        <f t="shared" si="60"/>
-        <v>PWRNUC</v>
+        <f t="shared" si="66"/>
+        <v>PWRBIO</v>
       </c>
       <c r="V68">
         <v>1</v>
@@ -34342,15 +34348,15 @@
         <v>10</v>
       </c>
       <c r="C69" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="54"/>
-        <v>PWRCLE</v>
+        <f t="shared" si="60"/>
+        <v>PWRNUC</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="55"/>
-        <v>Power Coal low grade</v>
+        <f t="shared" si="61"/>
+        <v>Power Nuclear</v>
       </c>
       <c r="F69" t="s">
         <v>239</v>
@@ -34360,12 +34366,12 @@
       <c r="I69"/>
       <c r="J69"/>
       <c r="K69" t="str">
-        <f t="shared" si="56"/>
-        <v>XPWRCLE</v>
+        <f t="shared" si="62"/>
+        <v>XPWRNUC</v>
       </c>
       <c r="L69" t="str">
-        <f t="shared" si="57"/>
-        <v>Power Coal low grade</v>
+        <f t="shared" si="63"/>
+        <v>Power Nuclear</v>
       </c>
       <c r="M69" t="s">
         <v>239</v>
@@ -34382,16 +34388,16 @@
       <c r="Q69"/>
       <c r="R69"/>
       <c r="S69" t="str">
-        <f t="shared" si="58"/>
-        <v>XPWRCLE</v>
+        <f t="shared" si="64"/>
+        <v>XPWRNUC</v>
       </c>
       <c r="T69" t="str">
-        <f t="shared" si="59"/>
-        <v>CLE</v>
+        <f t="shared" si="65"/>
+        <v>NUC</v>
       </c>
       <c r="U69" t="str">
-        <f t="shared" si="60"/>
-        <v>PWRCLE</v>
+        <f t="shared" si="66"/>
+        <v>PWRNUC</v>
       </c>
       <c r="V69">
         <v>1</v>
@@ -34407,8 +34413,75 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="B78"/>
+    <row r="70" spans="2:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" t="s">
+        <v>162</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="60"/>
+        <v>PWRCLE</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="61"/>
+        <v>Power Coal low grade</v>
+      </c>
+      <c r="F70" t="s">
+        <v>239</v>
+      </c>
+      <c r="G70"/>
+      <c r="H70"/>
+      <c r="I70"/>
+      <c r="J70"/>
+      <c r="K70" t="str">
+        <f t="shared" si="62"/>
+        <v>XPWRCLE</v>
+      </c>
+      <c r="L70" t="str">
+        <f t="shared" si="63"/>
+        <v>Power Coal low grade</v>
+      </c>
+      <c r="M70" t="s">
+        <v>239</v>
+      </c>
+      <c r="N70" t="s">
+        <v>428</v>
+      </c>
+      <c r="O70" t="s">
+        <v>357</v>
+      </c>
+      <c r="P70" t="s">
+        <v>607</v>
+      </c>
+      <c r="Q70"/>
+      <c r="R70"/>
+      <c r="S70" t="str">
+        <f t="shared" si="64"/>
+        <v>XPWRCLE</v>
+      </c>
+      <c r="T70" t="str">
+        <f t="shared" si="65"/>
+        <v>CLE</v>
+      </c>
+      <c r="U70" t="str">
+        <f t="shared" si="66"/>
+        <v>PWRCLE</v>
+      </c>
+      <c r="V70">
+        <v>1</v>
+      </c>
+      <c r="W70">
+        <v>60</v>
+      </c>
+      <c r="X70"/>
+      <c r="Y70">
+        <v>1</v>
+      </c>
+      <c r="Z70">
+        <v>1</v>
+      </c>
     </row>
     <row r="79" spans="2:26" ht="15" x14ac:dyDescent="0.25">
       <c r="B79"/>
@@ -34527,8 +34600,11 @@
     <row r="117" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B117"/>
     </row>
+    <row r="118" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B118"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B8:AA63" xr:uid="{00000000-0001-0000-2200-000000000000}"/>
+  <autoFilter ref="B8:AA64" xr:uid="{00000000-0001-0000-2200-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -55199,7 +55275,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="18">
         <f ca="1">NOW()</f>
-        <v>45199.685924074074</v>
+        <v>45201.46088136574</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -56023,7 +56099,7 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
         <f ca="1">NOW()</f>
-        <v>45199.685924074074</v>
+        <v>45201.46088136574</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -56054,10 +56130,10 @@
     <tabColor theme="5"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:D132"/>
+  <dimension ref="A2:D133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -56103,7 +56179,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="28">
-        <f t="shared" ref="A6:A47" si="0">A5+1</f>
+        <f t="shared" ref="A6:A48" si="0">A5+1</f>
         <v>2</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -56527,10 +56603,10 @@
         <v>37</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>211</v>
+        <v>1106</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>212</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -56539,10 +56615,10 @@
         <v>38</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -56551,10 +56627,10 @@
         <v>39</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -56563,10 +56639,10 @@
         <v>40</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -56575,10 +56651,10 @@
         <v>41</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -56587,10 +56663,10 @@
         <v>42</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -56599,87 +56675,94 @@
         <v>43</v>
       </c>
       <c r="B47" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="28">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B48" s="28" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D49" s="30"/>
-    </row>
-    <row r="50" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B50" s="26" t="s">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D50" s="30"/>
+    </row>
+    <row r="51" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B51" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="C50" s="26" t="s">
+      <c r="C51" s="26" t="s">
         <v>225</v>
-      </c>
-      <c r="D50" s="30"/>
-    </row>
-    <row r="51" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" t="s">
-        <v>0</v>
       </c>
       <c r="D51" s="30"/>
     </row>
     <row r="52" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>226</v>
+        <v>0</v>
       </c>
       <c r="D52" s="30"/>
     </row>
     <row r="53" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>1</v>
+        <v>226</v>
       </c>
       <c r="D53" s="30"/>
     </row>
     <row r="54" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>227</v>
+        <v>1</v>
       </c>
       <c r="D54" s="30"/>
     </row>
     <row r="55" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C55" t="s">
-        <v>3</v>
+        <v>227</v>
       </c>
       <c r="D55" s="30"/>
     </row>
     <row r="56" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D56" s="30"/>
     </row>
     <row r="57" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="30"/>
+    </row>
+    <row r="58" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>11</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>228</v>
       </c>
-      <c r="D57" s="30"/>
-    </row>
-    <row r="58" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B58"/>
-      <c r="C58"/>
       <c r="D58" s="30"/>
     </row>
     <row r="59" spans="2:4" ht="15" x14ac:dyDescent="0.25">
@@ -56687,7 +56770,9 @@
       <c r="C59"/>
       <c r="D59" s="30"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B60"/>
+      <c r="C60"/>
       <c r="D60" s="30"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
@@ -56715,19 +56800,16 @@
       <c r="D68" s="30"/>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C69" s="30" t="s">
+      <c r="D69" s="30"/>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C70" s="30" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C70" s="30">
-        <f t="shared" ref="C70:C80" si="1">COUNTIF($C$5:$C$46,C5)</f>
-        <v>1</v>
       </c>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C71" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C71:C81" si="1">COUNTIF($C$5:$C$47,C5)</f>
         <v>1</v>
       </c>
     </row>
@@ -56786,26 +56868,23 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="28">
-        <v>1</v>
-      </c>
       <c r="C81" s="30">
-        <f t="shared" ref="C81:C91" si="2">COUNTIF($C$5:$C$46,C17)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C82" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="C82:C92" si="2">COUNTIF($C$5:$C$47,C17)</f>
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C83" s="30">
         <f t="shared" si="2"/>
@@ -56814,7 +56893,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C84" s="30">
         <f t="shared" si="2"/>
@@ -56823,7 +56902,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C85" s="30">
         <f t="shared" si="2"/>
@@ -56832,7 +56911,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C86" s="30">
         <f t="shared" si="2"/>
@@ -56841,7 +56920,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C87" s="30">
         <f t="shared" si="2"/>
@@ -56850,7 +56929,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="28">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C88" s="30">
         <f t="shared" si="2"/>
@@ -56859,7 +56938,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="28">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C89" s="30">
         <f t="shared" si="2"/>
@@ -56868,7 +56947,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C90" s="30">
         <f t="shared" si="2"/>
@@ -56877,7 +56956,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="28">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C91" s="30">
         <f t="shared" si="2"/>
@@ -56886,25 +56965,25 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="28">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C92" s="30">
-        <f t="shared" ref="C92:C109" si="3">COUNTIF($C$5:$C$46,C29)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="28">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C93" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C93:C104" si="3">COUNTIF($C$5:$C$47,C29)</f>
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="28">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C94" s="30">
         <f t="shared" si="3"/>
@@ -56913,7 +56992,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="28">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C95" s="30">
         <f t="shared" si="3"/>
@@ -56922,7 +57001,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="28">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C96" s="30">
         <f t="shared" si="3"/>
@@ -56931,7 +57010,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="28">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C97" s="30">
         <f t="shared" si="3"/>
@@ -56940,7 +57019,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="28">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C98" s="30">
         <f t="shared" si="3"/>
@@ -56949,7 +57028,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="28">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C99" s="30">
         <f t="shared" si="3"/>
@@ -56958,7 +57037,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="28">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C100" s="30">
         <f t="shared" si="3"/>
@@ -56967,7 +57046,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="28">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C101" s="30">
         <f t="shared" si="3"/>
@@ -56976,15 +57055,17 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="28">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C102" s="30">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B103"/>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="28">
+        <v>22</v>
+      </c>
       <c r="C103" s="30">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -57000,41 +57081,44 @@
     <row r="105" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B105"/>
       <c r="C105" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C105:C110" si="4">COUNTIF($C$5:$C$47,C42)</f>
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B106"/>
       <c r="C106" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B107"/>
       <c r="C107" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B108"/>
       <c r="C108" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B109"/>
       <c r="C109" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B110"/>
-      <c r="C110" s="30"/>
+      <c r="C110" s="30">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="111" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B111"/>
@@ -57074,25 +57158,26 @@
     </row>
     <row r="120" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B120"/>
+      <c r="C120" s="30"/>
     </row>
     <row r="121" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B121"/>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B122" s="29"/>
-      <c r="C122" s="29"/>
-      <c r="D122" s="29"/>
-    </row>
-    <row r="123" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B123"/>
-      <c r="C123"/>
-    </row>
-    <row r="125" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B125" s="35"/>
-      <c r="C125"/>
-    </row>
-    <row r="129" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B129"/>
+    <row r="122" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B122"/>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B123" s="29"/>
+      <c r="C123" s="29"/>
+      <c r="D123" s="29"/>
+    </row>
+    <row r="124" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B124"/>
+      <c r="C124"/>
+    </row>
+    <row r="126" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B126" s="35"/>
+      <c r="C126"/>
     </row>
     <row r="130" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B130"/>
@@ -57102,6 +57187,9 @@
     </row>
     <row r="132" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B132"/>
+    </row>
+    <row r="133" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B133"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -59639,11 +59727,11 @@
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B43" s="380" t="str">
-        <f>NameConv!C41</f>
+        <f>NameConv!C42</f>
         <v>OKE</v>
       </c>
       <c r="C43" s="380" t="str">
-        <f>NameConv!B41</f>
+        <f>NameConv!B42</f>
         <v>Oil Kerosene</v>
       </c>
       <c r="D43" s="381" t="s">
@@ -59663,11 +59751,11 @@
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B44" s="380" t="str">
-        <f>NameConv!C42</f>
+        <f>NameConv!C43</f>
         <v>OLP</v>
       </c>
       <c r="C44" s="380" t="str">
-        <f>NameConv!B42</f>
+        <f>NameConv!B43</f>
         <v>Oil LPG</v>
       </c>
       <c r="D44" s="381" t="s">
@@ -59687,11 +59775,11 @@
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B45" s="380" t="str">
-        <f>NameConv!C43</f>
+        <f>NameConv!C44</f>
         <v>OTH</v>
       </c>
       <c r="C45" s="380" t="str">
-        <f>NameConv!B43</f>
+        <f>NameConv!B44</f>
         <v>Oil Other</v>
       </c>
       <c r="D45" s="381" t="s">
@@ -59711,11 +59799,11 @@
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B46" s="380" t="str">
-        <f>NameConv!C44</f>
+        <f>NameConv!C45</f>
         <v>SOL</v>
       </c>
       <c r="C46" s="380" t="str">
-        <f>NameConv!B44</f>
+        <f>NameConv!B45</f>
         <v>Solar</v>
       </c>
       <c r="D46" s="381" t="s">
@@ -59735,11 +59823,11 @@
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B47" s="380" t="str">
-        <f>NameConv!C45</f>
+        <f>NameConv!C46</f>
         <v>WND</v>
       </c>
       <c r="C47" s="380" t="str">
-        <f>NameConv!B45</f>
+        <f>NameConv!B46</f>
         <v>Wind</v>
       </c>
       <c r="D47" s="381" t="s">
@@ -59759,11 +59847,11 @@
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B48" s="380" t="str">
-        <f>NameConv!C46</f>
+        <f>NameConv!C47</f>
         <v>WAS</v>
       </c>
       <c r="C48" s="380" t="str">
-        <f>NameConv!B46</f>
+        <f>NameConv!B47</f>
         <v>Waste</v>
       </c>
       <c r="D48" s="381" t="s">
@@ -60135,7 +60223,7 @@
   </sheetPr>
   <dimension ref="A1:BA149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="F62" sqref="F62:I62"/>
     </sheetView>
   </sheetViews>
@@ -60597,23 +60685,23 @@
         <v>Oil HFO</v>
       </c>
       <c r="AU7" s="42" t="str">
-        <f>NameConv!$B$41</f>
+        <f>NameConv!$B$42</f>
         <v>Oil Kerosene</v>
       </c>
       <c r="AV7" s="42" t="str">
-        <f>NameConv!$B$42</f>
+        <f>NameConv!$B$43</f>
         <v>Oil LPG</v>
       </c>
       <c r="AW7" s="42" t="str">
-        <f>NameConv!$B$43</f>
+        <f>NameConv!$B$44</f>
         <v>Oil Other</v>
       </c>
       <c r="AX7" s="42" t="str">
-        <f>NameConv!$B$44</f>
+        <f>NameConv!$B$45</f>
         <v>Solar</v>
       </c>
       <c r="AY7" s="42" t="str">
-        <f>NameConv!$B$45</f>
+        <f>NameConv!$B$46</f>
         <v>Wind</v>
       </c>
     </row>
@@ -65279,7 +65367,7 @@
         <v>MINWAS</v>
       </c>
       <c r="D73" s="159" t="str">
-        <f>NameConv!C46</f>
+        <f>NameConv!C47</f>
         <v>WAS</v>
       </c>
       <c r="E73" s="30">
@@ -65416,7 +65504,7 @@
         <v>MINSOL</v>
       </c>
       <c r="D75" s="159" t="str">
-        <f>NameConv!C44</f>
+        <f>NameConv!C45</f>
         <v>SOL</v>
       </c>
       <c r="E75" s="30">
@@ -65477,7 +65565,7 @@
         <v>MINWND</v>
       </c>
       <c r="D76" s="159" t="str">
-        <f>NameConv!C45</f>
+        <f>NameConv!C46</f>
         <v>WND</v>
       </c>
       <c r="E76" s="30">
@@ -66419,7 +66507,7 @@
         <v>IMPOLP</v>
       </c>
       <c r="D89" s="159" t="str">
-        <f>NameConv!C42</f>
+        <f>NameConv!C43</f>
         <v>OLP</v>
       </c>
       <c r="E89" s="30">
@@ -66496,7 +66584,7 @@
         <v>IMPOKE</v>
       </c>
       <c r="D90" s="159" t="str">
-        <f>NameConv!C41</f>
+        <f>NameConv!C42</f>
         <v>OKE</v>
       </c>
       <c r="E90" s="30">
@@ -67515,7 +67603,7 @@
         <v>PEXOKE</v>
       </c>
       <c r="C104" s="159" t="str">
-        <f>NameConv!C41</f>
+        <f>NameConv!C42</f>
         <v>OKE</v>
       </c>
       <c r="E104" s="30">

</xml_diff>

<commit_message>
combustion emissions fixed on LPG and Waste, fuel supply for CLD added
</commit_message>
<xml_diff>
--- a/VT_REGION1_SUP.xlsx
+++ b/VT_REGION1_SUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F580CBE-EB58-46E3-8E4F-F6648C2BA0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585E59CF-A4DC-40FD-9929-B3FD556B7504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="26610" windowHeight="13740" firstSheet="5" activeTab="11" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="11" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,9 @@
     <definedName name="emissions_start">[3]NameConv!$AY$4</definedName>
     <definedName name="emissions_types">[3]NameConv!$AX$3</definedName>
     <definedName name="eps">NameConv!$D$2</definedName>
-    <definedName name="FuelNames">NameConv!$B$5:$C$47</definedName>
-    <definedName name="FuelNamesLong">NameConv!$B$5:$B$47</definedName>
-    <definedName name="FuelNamesShort">NameConv!$C$5:$C$47</definedName>
+    <definedName name="FuelNames">NameConv!$B$5:$C$48</definedName>
+    <definedName name="FuelNamesLong">NameConv!$B$5:$B$48</definedName>
+    <definedName name="FuelNamesShort">NameConv!$C$5:$C$48</definedName>
     <definedName name="gwpch4">'[2]SASOL CC 2019 report'!$E$98</definedName>
     <definedName name="gwpn2o">'[2]SASOL CC 2019 report'!$E$97</definedName>
     <definedName name="H2.LHV.MJ_kg">'[3]Hydrogen-ELT'!$D$39</definedName>
@@ -135,9 +135,9 @@
     <definedName name="Sector.Transport">[3]Index!$G$2</definedName>
     <definedName name="sector_prefix" localSheetId="8">GasPipeLines!#REF!</definedName>
     <definedName name="sector_prefix">LNG!#REF!</definedName>
-    <definedName name="SectorNames">NameConv!$B$52:$C$60</definedName>
-    <definedName name="SectorNamesLong">NameConv!$C$52:$C$60</definedName>
-    <definedName name="SectorNamesShort">NameConv!$B$52:$B$60</definedName>
+    <definedName name="SectorNames">NameConv!$B$53:$C$61</definedName>
+    <definedName name="SectorNamesLong">NameConv!$C$53:$C$61</definedName>
+    <definedName name="SectorNamesShort">NameConv!$B$53:$B$61</definedName>
     <definedName name="solver_eng" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="6" hidden="1">0</definedName>
@@ -1631,7 +1631,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2652" uniqueCount="1107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2669" uniqueCount="1109">
   <si>
     <t>Agriculture</t>
   </si>
@@ -5111,6 +5111,12 @@
   </si>
   <si>
     <t>Oil HFO for material use</t>
+  </si>
+  <si>
+    <t>WMU</t>
+  </si>
+  <si>
+    <t>Waste for material use</t>
   </si>
 </sst>
 </file>
@@ -7392,57 +7398,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="42" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7480,6 +7435,57 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -24956,25 +24962,25 @@
       <c r="W6" s="175" t="s">
         <v>361</v>
       </c>
-      <c r="AC6" s="433" t="s">
+      <c r="AC6" s="416" t="s">
         <v>362</v>
       </c>
-      <c r="AD6" s="433"/>
-      <c r="AE6" s="433"/>
+      <c r="AD6" s="416"/>
+      <c r="AE6" s="416"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="434" t="s">
+      <c r="A7" s="417" t="s">
         <v>363</v>
       </c>
-      <c r="B7" s="436" t="s">
+      <c r="B7" s="419" t="s">
         <v>364</v>
       </c>
-      <c r="C7" s="438" t="s">
+      <c r="C7" s="421" t="s">
         <v>365</v>
       </c>
-      <c r="D7" s="439"/>
-      <c r="E7" s="440"/>
-      <c r="F7" s="443" t="s">
+      <c r="D7" s="422"/>
+      <c r="E7" s="423"/>
+      <c r="F7" s="426" t="s">
         <v>366</v>
       </c>
       <c r="G7" s="176"/>
@@ -25002,12 +25008,12 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="435"/>
-      <c r="B8" s="437"/>
-      <c r="C8" s="441"/>
-      <c r="D8" s="442"/>
-      <c r="E8" s="442"/>
-      <c r="F8" s="444"/>
+      <c r="A8" s="418"/>
+      <c r="B8" s="420"/>
+      <c r="C8" s="424"/>
+      <c r="D8" s="425"/>
+      <c r="E8" s="425"/>
+      <c r="F8" s="427"/>
       <c r="G8" s="176"/>
       <c r="H8" s="176"/>
       <c r="I8" s="176"/>
@@ -25873,11 +25879,11 @@
       <c r="I25" s="57"/>
       <c r="J25" s="57"/>
       <c r="V25" s="217"/>
-      <c r="AC25" s="432" t="s">
+      <c r="AC25" s="415" t="s">
         <v>432</v>
       </c>
-      <c r="AD25" s="432"/>
-      <c r="AE25" s="432"/>
+      <c r="AD25" s="415"/>
+      <c r="AE25" s="415"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C26" s="57"/>
@@ -25956,8 +25962,8 @@
       <c r="D30" s="57"/>
     </row>
     <row r="31" spans="1:31" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H31" s="428"/>
-      <c r="I31" s="428"/>
+      <c r="H31" s="435"/>
+      <c r="I31" s="435"/>
       <c r="R31" t="s">
         <v>370</v>
       </c>
@@ -25978,10 +25984,10 @@
       </c>
     </row>
     <row r="32" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L32" s="420" t="s">
+      <c r="L32" s="428" t="s">
         <v>436</v>
       </c>
-      <c r="M32" s="429" t="s">
+      <c r="M32" s="436" t="s">
         <v>437</v>
       </c>
       <c r="N32" s="220" t="s">
@@ -25996,22 +26002,22 @@
       <c r="Q32" s="223" t="s">
         <v>439</v>
       </c>
-      <c r="R32" s="420" t="s">
+      <c r="R32" s="428" t="s">
         <v>389</v>
       </c>
-      <c r="S32" s="420" t="s">
+      <c r="S32" s="428" t="s">
         <v>393</v>
       </c>
-      <c r="T32" s="420" t="s">
+      <c r="T32" s="428" t="s">
         <v>440</v>
       </c>
-      <c r="U32" s="420" t="s">
+      <c r="U32" s="428" t="s">
         <v>389</v>
       </c>
-      <c r="V32" s="420" t="s">
+      <c r="V32" s="428" t="s">
         <v>393</v>
       </c>
-      <c r="W32" s="420" t="s">
+      <c r="W32" s="428" t="s">
         <v>440</v>
       </c>
     </row>
@@ -26034,28 +26040,28 @@
       <c r="G33" s="142" t="s">
         <v>444</v>
       </c>
-      <c r="H33" s="427" t="s">
+      <c r="H33" s="431" t="s">
         <v>445</v>
       </c>
-      <c r="I33" s="427"/>
+      <c r="I33" s="431"/>
       <c r="J33" s="142" t="s">
         <v>443</v>
       </c>
       <c r="K33" t="s">
         <v>444</v>
       </c>
-      <c r="L33" s="421"/>
-      <c r="M33" s="430"/>
+      <c r="L33" s="429"/>
+      <c r="M33" s="437"/>
       <c r="N33" s="16"/>
       <c r="O33" s="73"/>
       <c r="P33" s="73"/>
       <c r="Q33" s="224"/>
-      <c r="R33" s="421"/>
-      <c r="S33" s="421"/>
-      <c r="T33" s="421"/>
-      <c r="U33" s="421"/>
-      <c r="V33" s="421"/>
-      <c r="W33" s="421"/>
+      <c r="R33" s="429"/>
+      <c r="S33" s="429"/>
+      <c r="T33" s="429"/>
+      <c r="U33" s="429"/>
+      <c r="V33" s="429"/>
+      <c r="W33" s="429"/>
     </row>
     <row r="34" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -26075,8 +26081,8 @@
       <c r="K34" t="s">
         <v>447</v>
       </c>
-      <c r="L34" s="422"/>
-      <c r="M34" s="431"/>
+      <c r="L34" s="430"/>
+      <c r="M34" s="438"/>
       <c r="N34" s="225" t="s">
         <v>449</v>
       </c>
@@ -26089,12 +26095,12 @@
       <c r="Q34" s="227" t="s">
         <v>449</v>
       </c>
-      <c r="R34" s="422"/>
-      <c r="S34" s="422"/>
-      <c r="T34" s="422"/>
-      <c r="U34" s="422"/>
-      <c r="V34" s="422"/>
-      <c r="W34" s="422"/>
+      <c r="R34" s="430"/>
+      <c r="S34" s="430"/>
+      <c r="T34" s="430"/>
+      <c r="U34" s="430"/>
+      <c r="V34" s="430"/>
+      <c r="W34" s="430"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="228" t="s">
@@ -26160,7 +26166,7 @@
         <v>2.9</v>
       </c>
       <c r="I36" s="237"/>
-      <c r="L36" s="423" t="str">
+      <c r="L36" s="432" t="str">
         <f>A36</f>
         <v>Well completion</v>
       </c>
@@ -26240,7 +26246,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="I37" s="237"/>
-      <c r="L37" s="424"/>
+      <c r="L37" s="433"/>
       <c r="M37" t="str">
         <f t="shared" ref="M37:M45" si="5">B37</f>
         <v>Jiang et al. (2011)</v>
@@ -26311,7 +26317,7 @@
         <v>7.8</v>
       </c>
       <c r="I38" s="237"/>
-      <c r="L38" s="424"/>
+      <c r="L38" s="433"/>
       <c r="M38" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26386,7 +26392,7 @@
       </c>
       <c r="I39" s="237"/>
       <c r="K39" s="237"/>
-      <c r="L39" s="424"/>
+      <c r="L39" s="433"/>
       <c r="M39" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26457,7 +26463,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="I40" s="237"/>
-      <c r="L40" s="424"/>
+      <c r="L40" s="433"/>
       <c r="M40" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26531,7 +26537,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="I41" s="237"/>
-      <c r="L41" s="425"/>
+      <c r="L41" s="434"/>
       <c r="M41" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Broderick et al. (2011)</v>
@@ -26605,7 +26611,7 @@
         <v>4.2</v>
       </c>
       <c r="I42" s="237"/>
-      <c r="L42" s="423" t="s">
+      <c r="L42" s="432" t="s">
         <v>413</v>
       </c>
       <c r="M42" s="222" t="str">
@@ -26678,7 +26684,7 @@
         <v>3.5</v>
       </c>
       <c r="I43" s="237"/>
-      <c r="L43" s="424"/>
+      <c r="L43" s="433"/>
       <c r="M43" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26754,7 +26760,7 @@
       </c>
       <c r="I44" s="237"/>
       <c r="K44" s="237"/>
-      <c r="L44" s="424"/>
+      <c r="L44" s="433"/>
       <c r="M44" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26826,7 +26832,7 @@
         <v>8.9</v>
       </c>
       <c r="I45" s="237"/>
-      <c r="L45" s="425"/>
+      <c r="L45" s="434"/>
       <c r="M45" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26895,7 +26901,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="237"/>
-      <c r="L46" s="423" t="str">
+      <c r="L46" s="432" t="str">
         <f>A47</f>
         <v>Transport, storage and distribution</v>
       </c>
@@ -26971,7 +26977,7 @@
         <v>1.9</v>
       </c>
       <c r="I47" s="237"/>
-      <c r="L47" s="424"/>
+      <c r="L47" s="433"/>
       <c r="M47" t="str">
         <f>B48</f>
         <v>Skone et al. (2011)</v>
@@ -27042,7 +27048,7 @@
         <v>2.7</v>
       </c>
       <c r="I48" s="237"/>
-      <c r="L48" s="425"/>
+      <c r="L48" s="434"/>
       <c r="M48" s="95" t="str">
         <f>B49</f>
         <v>Howarth et al. (2011)</v>
@@ -27411,10 +27417,10 @@
       <c r="C79" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="D79" s="426" t="s">
+      <c r="D79" s="444" t="s">
         <v>498</v>
       </c>
-      <c r="E79" s="426"/>
+      <c r="E79" s="444"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
@@ -27516,13 +27522,13 @@
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="415" t="s">
+      <c r="A103" s="439" t="s">
         <v>508</v>
       </c>
       <c r="B103" s="266" t="s">
         <v>509</v>
       </c>
-      <c r="C103" s="417" t="s">
+      <c r="C103" s="441" t="s">
         <v>510</v>
       </c>
       <c r="D103" s="266">
@@ -27533,11 +27539,11 @@
       </c>
     </row>
     <row r="104" spans="1:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="416"/>
+      <c r="A104" s="440"/>
       <c r="B104" s="266" t="s">
         <v>511</v>
       </c>
-      <c r="C104" s="418"/>
+      <c r="C104" s="442"/>
       <c r="D104" s="266">
         <v>0.18</v>
       </c>
@@ -27550,13 +27556,13 @@
       </c>
     </row>
     <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="415" t="s">
+      <c r="A105" s="439" t="s">
         <v>512</v>
       </c>
       <c r="B105" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C105" s="418"/>
+      <c r="C105" s="442"/>
       <c r="D105" s="266">
         <v>0</v>
       </c>
@@ -27565,11 +27571,11 @@
       </c>
     </row>
     <row r="106" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="416"/>
+      <c r="A106" s="440"/>
       <c r="B106" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C106" s="419"/>
+      <c r="C106" s="443"/>
       <c r="D106" s="266">
         <v>0</v>
       </c>
@@ -27578,13 +27584,13 @@
       </c>
     </row>
     <row r="107" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="415" t="s">
+      <c r="A107" s="439" t="s">
         <v>508</v>
       </c>
       <c r="B107" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C107" s="417" t="s">
+      <c r="C107" s="441" t="s">
         <v>515</v>
       </c>
       <c r="D107" s="266">
@@ -27595,11 +27601,11 @@
       </c>
     </row>
     <row r="108" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="416"/>
+      <c r="A108" s="440"/>
       <c r="B108" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C108" s="418"/>
+      <c r="C108" s="442"/>
       <c r="D108" s="266">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -27608,13 +27614,13 @@
       </c>
     </row>
     <row r="109" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="415" t="s">
+      <c r="A109" s="439" t="s">
         <v>512</v>
       </c>
       <c r="B109" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C109" s="418"/>
+      <c r="C109" s="442"/>
       <c r="D109" s="266">
         <v>0</v>
       </c>
@@ -27623,11 +27629,11 @@
       </c>
     </row>
     <row r="110" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="416"/>
+      <c r="A110" s="440"/>
       <c r="B110" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C110" s="419"/>
+      <c r="C110" s="443"/>
       <c r="D110" s="266">
         <v>0</v>
       </c>
@@ -29090,12 +29096,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AC25:AE25"/>
-    <mergeCell ref="AC6:AE6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="C107:C110"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="U32:U34"/>
+    <mergeCell ref="V32:V34"/>
+    <mergeCell ref="L46:L48"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="C103:C106"/>
+    <mergeCell ref="A105:A106"/>
     <mergeCell ref="W32:W34"/>
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="L36:L41"/>
@@ -29106,16 +29116,12 @@
     <mergeCell ref="R32:R34"/>
     <mergeCell ref="S32:S34"/>
     <mergeCell ref="T32:T34"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="C107:C110"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="U32:U34"/>
-    <mergeCell ref="V32:V34"/>
-    <mergeCell ref="L46:L48"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="C103:C106"/>
-    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="AC25:AE25"/>
+    <mergeCell ref="AC6:AE6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29864,10 +29870,10 @@
   <sheetPr codeName="Sheet12">
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:AE118"/>
+  <dimension ref="A1:AE119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K46" workbookViewId="0">
-      <selection activeCell="T52" sqref="T52"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -34065,18 +34071,18 @@
     </row>
     <row r="65" spans="2:26" ht="15" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>218</v>
+        <v>1107</v>
       </c>
       <c r="D65" t="str">
-        <f t="shared" ref="D65:D70" si="60">B65&amp;C65</f>
-        <v>PWRSOL</v>
+        <f t="shared" ref="D65" si="60">B65&amp;C65</f>
+        <v>INDWMU</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" ref="E65:E70" si="61">INDEX(SectorNamesLong,MATCH(B65,SectorNamesShort,0))&amp;" "&amp;INDEX(FuelNamesLong,MATCH(C65,FuelNamesShort,0))</f>
-        <v>Power Solar</v>
+        <f t="shared" ref="E65" si="61">INDEX(SectorNamesLong,MATCH(B65,SectorNamesShort,0))&amp;" "&amp;INDEX(FuelNamesLong,MATCH(C65,FuelNamesShort,0))</f>
+        <v>Industry Waste for material use</v>
       </c>
       <c r="F65" t="s">
         <v>239</v>
@@ -34086,12 +34092,12 @@
       <c r="I65"/>
       <c r="J65"/>
       <c r="K65" t="str">
-        <f t="shared" ref="K65:K70" si="62">"X"&amp;D65</f>
-        <v>XPWRSOL</v>
+        <f t="shared" ref="K65" si="62">"X"&amp;D65</f>
+        <v>XINDWMU</v>
       </c>
       <c r="L65" t="str">
-        <f t="shared" ref="L65:L70" si="63">E65</f>
-        <v>Power Solar</v>
+        <f t="shared" ref="L65" si="63">E65</f>
+        <v>Industry Waste for material use</v>
       </c>
       <c r="M65" t="s">
         <v>239</v>
@@ -34108,16 +34114,15 @@
       <c r="Q65"/>
       <c r="R65"/>
       <c r="S65" t="str">
-        <f t="shared" ref="S65:S70" si="64">K65</f>
-        <v>XPWRSOL</v>
-      </c>
-      <c r="T65" t="str">
-        <f t="shared" ref="T65:T70" si="65">C65</f>
-        <v>SOL</v>
+        <f t="shared" ref="S65" si="64">K65</f>
+        <v>XINDWMU</v>
+      </c>
+      <c r="T65" s="237" t="s">
+        <v>222</v>
       </c>
       <c r="U65" t="str">
-        <f t="shared" ref="U65:U70" si="66">D65</f>
-        <v>PWRSOL</v>
+        <f t="shared" ref="U65" si="65">D65</f>
+        <v>INDWMU</v>
       </c>
       <c r="V65">
         <v>1</v>
@@ -34138,15 +34143,15 @@
         <v>10</v>
       </c>
       <c r="C66" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" si="60"/>
-        <v>PWRWND</v>
+        <f t="shared" ref="D66:D71" si="66">B66&amp;C66</f>
+        <v>PWRSOL</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" si="61"/>
-        <v>Power Wind</v>
+        <f t="shared" ref="E66:E71" si="67">INDEX(SectorNamesLong,MATCH(B66,SectorNamesShort,0))&amp;" "&amp;INDEX(FuelNamesLong,MATCH(C66,FuelNamesShort,0))</f>
+        <v>Power Solar</v>
       </c>
       <c r="F66" t="s">
         <v>239</v>
@@ -34156,12 +34161,12 @@
       <c r="I66"/>
       <c r="J66"/>
       <c r="K66" t="str">
-        <f t="shared" si="62"/>
-        <v>XPWRWND</v>
+        <f t="shared" ref="K66:K71" si="68">"X"&amp;D66</f>
+        <v>XPWRSOL</v>
       </c>
       <c r="L66" t="str">
-        <f t="shared" si="63"/>
-        <v>Power Wind</v>
+        <f t="shared" ref="L66:L71" si="69">E66</f>
+        <v>Power Solar</v>
       </c>
       <c r="M66" t="s">
         <v>239</v>
@@ -34178,16 +34183,16 @@
       <c r="Q66"/>
       <c r="R66"/>
       <c r="S66" t="str">
-        <f t="shared" si="64"/>
-        <v>XPWRWND</v>
+        <f t="shared" ref="S66:S71" si="70">K66</f>
+        <v>XPWRSOL</v>
       </c>
       <c r="T66" t="str">
-        <f t="shared" si="65"/>
-        <v>WND</v>
+        <f t="shared" ref="T66:T71" si="71">C66</f>
+        <v>SOL</v>
       </c>
       <c r="U66" t="str">
-        <f t="shared" si="66"/>
-        <v>PWRWND</v>
+        <f t="shared" ref="U66:U71" si="72">D66</f>
+        <v>PWRSOL</v>
       </c>
       <c r="V66">
         <v>1</v>
@@ -34208,15 +34213,15 @@
         <v>10</v>
       </c>
       <c r="C67" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" si="60"/>
-        <v>PWRHYD</v>
+        <f t="shared" si="66"/>
+        <v>PWRWND</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" si="61"/>
-        <v>Power Hydro</v>
+        <f t="shared" si="67"/>
+        <v>Power Wind</v>
       </c>
       <c r="F67" t="s">
         <v>239</v>
@@ -34226,12 +34231,12 @@
       <c r="I67"/>
       <c r="J67"/>
       <c r="K67" t="str">
-        <f t="shared" si="62"/>
-        <v>XPWRHYD</v>
+        <f t="shared" si="68"/>
+        <v>XPWRWND</v>
       </c>
       <c r="L67" t="str">
-        <f t="shared" si="63"/>
-        <v>Power Hydro</v>
+        <f t="shared" si="69"/>
+        <v>Power Wind</v>
       </c>
       <c r="M67" t="s">
         <v>239</v>
@@ -34248,16 +34253,16 @@
       <c r="Q67"/>
       <c r="R67"/>
       <c r="S67" t="str">
-        <f t="shared" si="64"/>
-        <v>XPWRHYD</v>
+        <f t="shared" si="70"/>
+        <v>XPWRWND</v>
       </c>
       <c r="T67" t="str">
-        <f t="shared" si="65"/>
-        <v>HYD</v>
+        <f t="shared" si="71"/>
+        <v>WND</v>
       </c>
       <c r="U67" t="str">
-        <f t="shared" si="66"/>
-        <v>PWRHYD</v>
+        <f t="shared" si="72"/>
+        <v>PWRWND</v>
       </c>
       <c r="V67">
         <v>1</v>
@@ -34278,15 +34283,15 @@
         <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>152</v>
+        <v>196</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" si="60"/>
-        <v>PWRBIO</v>
+        <f t="shared" si="66"/>
+        <v>PWRHYD</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="61"/>
-        <v>Power Biomass Other</v>
+        <f t="shared" si="67"/>
+        <v>Power Hydro</v>
       </c>
       <c r="F68" t="s">
         <v>239</v>
@@ -34296,12 +34301,12 @@
       <c r="I68"/>
       <c r="J68"/>
       <c r="K68" t="str">
-        <f t="shared" si="62"/>
-        <v>XPWRBIO</v>
+        <f t="shared" si="68"/>
+        <v>XPWRHYD</v>
       </c>
       <c r="L68" t="str">
-        <f t="shared" si="63"/>
-        <v>Power Biomass Other</v>
+        <f t="shared" si="69"/>
+        <v>Power Hydro</v>
       </c>
       <c r="M68" t="s">
         <v>239</v>
@@ -34318,16 +34323,16 @@
       <c r="Q68"/>
       <c r="R68"/>
       <c r="S68" t="str">
-        <f t="shared" si="64"/>
-        <v>XPWRBIO</v>
+        <f t="shared" si="70"/>
+        <v>XPWRHYD</v>
       </c>
       <c r="T68" t="str">
-        <f t="shared" si="65"/>
-        <v>BIO</v>
+        <f t="shared" si="71"/>
+        <v>HYD</v>
       </c>
       <c r="U68" t="str">
-        <f t="shared" si="66"/>
-        <v>PWRBIO</v>
+        <f t="shared" si="72"/>
+        <v>PWRHYD</v>
       </c>
       <c r="V68">
         <v>1</v>
@@ -34348,15 +34353,15 @@
         <v>10</v>
       </c>
       <c r="C69" t="s">
-        <v>200</v>
+        <v>152</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="60"/>
-        <v>PWRNUC</v>
+        <f t="shared" si="66"/>
+        <v>PWRBIO</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="61"/>
-        <v>Power Nuclear</v>
+        <f t="shared" si="67"/>
+        <v>Power Biomass Other</v>
       </c>
       <c r="F69" t="s">
         <v>239</v>
@@ -34366,12 +34371,12 @@
       <c r="I69"/>
       <c r="J69"/>
       <c r="K69" t="str">
-        <f t="shared" si="62"/>
-        <v>XPWRNUC</v>
+        <f t="shared" si="68"/>
+        <v>XPWRBIO</v>
       </c>
       <c r="L69" t="str">
-        <f t="shared" si="63"/>
-        <v>Power Nuclear</v>
+        <f t="shared" si="69"/>
+        <v>Power Biomass Other</v>
       </c>
       <c r="M69" t="s">
         <v>239</v>
@@ -34388,16 +34393,16 @@
       <c r="Q69"/>
       <c r="R69"/>
       <c r="S69" t="str">
-        <f t="shared" si="64"/>
-        <v>XPWRNUC</v>
+        <f t="shared" si="70"/>
+        <v>XPWRBIO</v>
       </c>
       <c r="T69" t="str">
-        <f t="shared" si="65"/>
-        <v>NUC</v>
+        <f t="shared" si="71"/>
+        <v>BIO</v>
       </c>
       <c r="U69" t="str">
-        <f t="shared" si="66"/>
-        <v>PWRNUC</v>
+        <f t="shared" si="72"/>
+        <v>PWRBIO</v>
       </c>
       <c r="V69">
         <v>1</v>
@@ -34418,15 +34423,15 @@
         <v>10</v>
       </c>
       <c r="C70" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" si="60"/>
-        <v>PWRCLE</v>
+        <f t="shared" si="66"/>
+        <v>PWRNUC</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="61"/>
-        <v>Power Coal low grade</v>
+        <f t="shared" si="67"/>
+        <v>Power Nuclear</v>
       </c>
       <c r="F70" t="s">
         <v>239</v>
@@ -34436,12 +34441,12 @@
       <c r="I70"/>
       <c r="J70"/>
       <c r="K70" t="str">
-        <f t="shared" si="62"/>
-        <v>XPWRCLE</v>
+        <f t="shared" si="68"/>
+        <v>XPWRNUC</v>
       </c>
       <c r="L70" t="str">
-        <f t="shared" si="63"/>
-        <v>Power Coal low grade</v>
+        <f t="shared" si="69"/>
+        <v>Power Nuclear</v>
       </c>
       <c r="M70" t="s">
         <v>239</v>
@@ -34458,16 +34463,16 @@
       <c r="Q70"/>
       <c r="R70"/>
       <c r="S70" t="str">
-        <f t="shared" si="64"/>
-        <v>XPWRCLE</v>
+        <f t="shared" si="70"/>
+        <v>XPWRNUC</v>
       </c>
       <c r="T70" t="str">
-        <f t="shared" si="65"/>
-        <v>CLE</v>
+        <f t="shared" si="71"/>
+        <v>NUC</v>
       </c>
       <c r="U70" t="str">
-        <f t="shared" si="66"/>
-        <v>PWRCLE</v>
+        <f t="shared" si="72"/>
+        <v>PWRNUC</v>
       </c>
       <c r="V70">
         <v>1</v>
@@ -34483,8 +34488,145 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="B79"/>
+    <row r="71" spans="2:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" t="s">
+        <v>162</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="66"/>
+        <v>PWRCLE</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="67"/>
+        <v>Power Coal low grade</v>
+      </c>
+      <c r="F71" t="s">
+        <v>239</v>
+      </c>
+      <c r="G71"/>
+      <c r="H71"/>
+      <c r="I71"/>
+      <c r="J71"/>
+      <c r="K71" t="str">
+        <f t="shared" si="68"/>
+        <v>XPWRCLE</v>
+      </c>
+      <c r="L71" t="str">
+        <f t="shared" si="69"/>
+        <v>Power Coal low grade</v>
+      </c>
+      <c r="M71" t="s">
+        <v>239</v>
+      </c>
+      <c r="N71" t="s">
+        <v>428</v>
+      </c>
+      <c r="O71" t="s">
+        <v>357</v>
+      </c>
+      <c r="P71" t="s">
+        <v>607</v>
+      </c>
+      <c r="Q71"/>
+      <c r="R71"/>
+      <c r="S71" t="str">
+        <f t="shared" si="70"/>
+        <v>XPWRCLE</v>
+      </c>
+      <c r="T71" t="str">
+        <f t="shared" si="71"/>
+        <v>CLE</v>
+      </c>
+      <c r="U71" t="str">
+        <f t="shared" si="72"/>
+        <v>PWRCLE</v>
+      </c>
+      <c r="V71">
+        <v>1</v>
+      </c>
+      <c r="W71">
+        <v>60</v>
+      </c>
+      <c r="X71"/>
+      <c r="Y71">
+        <v>1</v>
+      </c>
+      <c r="Z71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" t="s">
+        <v>160</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" ref="D72" si="73">B72&amp;C72</f>
+        <v>PWRCLD</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" ref="E72" si="74">INDEX(SectorNamesLong,MATCH(B72,SectorNamesShort,0))&amp;" "&amp;INDEX(FuelNamesLong,MATCH(C72,FuelNamesShort,0))</f>
+        <v>Power Coal Discard</v>
+      </c>
+      <c r="F72" t="s">
+        <v>239</v>
+      </c>
+      <c r="G72"/>
+      <c r="H72"/>
+      <c r="I72"/>
+      <c r="J72"/>
+      <c r="K72" t="str">
+        <f t="shared" ref="K72" si="75">"X"&amp;D72</f>
+        <v>XPWRCLD</v>
+      </c>
+      <c r="L72" t="str">
+        <f t="shared" ref="L72" si="76">E72</f>
+        <v>Power Coal Discard</v>
+      </c>
+      <c r="M72" t="s">
+        <v>239</v>
+      </c>
+      <c r="N72" t="s">
+        <v>428</v>
+      </c>
+      <c r="O72" t="s">
+        <v>357</v>
+      </c>
+      <c r="P72" t="s">
+        <v>607</v>
+      </c>
+      <c r="Q72"/>
+      <c r="R72"/>
+      <c r="S72" t="str">
+        <f t="shared" ref="S72" si="77">K72</f>
+        <v>XPWRCLD</v>
+      </c>
+      <c r="T72" t="str">
+        <f t="shared" ref="T72" si="78">C72</f>
+        <v>CLD</v>
+      </c>
+      <c r="U72" t="str">
+        <f t="shared" ref="U72" si="79">D72</f>
+        <v>PWRCLD</v>
+      </c>
+      <c r="V72">
+        <v>1</v>
+      </c>
+      <c r="W72">
+        <v>60</v>
+      </c>
+      <c r="X72"/>
+      <c r="Y72">
+        <v>1</v>
+      </c>
+      <c r="Z72">
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="2:26" ht="15" x14ac:dyDescent="0.25">
       <c r="B80"/>
@@ -34602,6 +34744,9 @@
     </row>
     <row r="118" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B118"/>
+    </row>
+    <row r="119" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B119"/>
     </row>
   </sheetData>
   <autoFilter ref="B8:AA64" xr:uid="{00000000-0001-0000-2200-000000000000}"/>
@@ -49803,18 +49948,18 @@
         <f>FORECAST(CR93,CP94:CQ94,CP93:CQ93)</f>
         <v>93</v>
       </c>
-      <c r="DL94" s="427" t="s">
+      <c r="DL94" s="431" t="s">
         <v>762</v>
       </c>
-      <c r="DM94" s="427"/>
-      <c r="DN94" s="427" t="s">
+      <c r="DM94" s="431"/>
+      <c r="DN94" s="431" t="s">
         <v>763</v>
       </c>
-      <c r="DO94" s="427"/>
-      <c r="DP94" s="427" t="s">
+      <c r="DO94" s="431"/>
+      <c r="DP94" s="431" t="s">
         <v>761</v>
       </c>
-      <c r="DQ94" s="427"/>
+      <c r="DQ94" s="431"/>
     </row>
     <row r="95" spans="1:121" x14ac:dyDescent="0.25">
       <c r="BK95" t="s">
@@ -55275,7 +55420,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="18">
         <f ca="1">NOW()</f>
-        <v>45201.46088136574</v>
+        <v>45201.73094212963</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -56099,7 +56244,7 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
         <f ca="1">NOW()</f>
-        <v>45201.46088136574</v>
+        <v>45201.73094212963</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -56130,10 +56275,10 @@
     <tabColor theme="5"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:D133"/>
+  <dimension ref="A2:D134"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -56179,7 +56324,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="28">
-        <f t="shared" ref="A6:A48" si="0">A5+1</f>
+        <f t="shared" ref="A6:A49" si="0">A5+1</f>
         <v>2</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -56687,104 +56832,113 @@
         <v>44</v>
       </c>
       <c r="B48" s="28" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="28">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B49" s="28" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D50" s="30"/>
-    </row>
-    <row r="51" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B51" s="26" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="30"/>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B52" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="C51" s="26" t="s">
+      <c r="C52" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="D51" s="30"/>
-    </row>
-    <row r="52" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+      <c r="D52" s="30"/>
+    </row>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>5</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>0</v>
       </c>
-      <c r="D52" s="30"/>
-    </row>
-    <row r="53" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="D53" s="30"/>
+    </row>
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>6</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>226</v>
       </c>
-      <c r="D53" s="30"/>
-    </row>
-    <row r="54" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="D54" s="30"/>
+    </row>
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>7</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>1</v>
       </c>
-      <c r="D54" s="30"/>
-    </row>
-    <row r="55" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+      <c r="D55" s="30"/>
+    </row>
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>10</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>227</v>
       </c>
-      <c r="D55" s="30"/>
-    </row>
-    <row r="56" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+      <c r="D56" s="30"/>
+    </row>
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
         <v>9</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>3</v>
       </c>
-      <c r="D56" s="30"/>
-    </row>
-    <row r="57" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+      <c r="D57" s="30"/>
+    </row>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>8</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>2</v>
       </c>
-      <c r="D57" s="30"/>
-    </row>
-    <row r="58" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+      <c r="D58" s="30"/>
+    </row>
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>11</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>228</v>
       </c>
-      <c r="D58" s="30"/>
-    </row>
-    <row r="59" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B59"/>
-      <c r="C59"/>
       <c r="D59" s="30"/>
     </row>
-    <row r="60" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60" s="30"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B61"/>
+      <c r="C61"/>
       <c r="D61" s="30"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D62" s="30"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D63" s="30"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D64" s="30"/>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.2">
@@ -56803,326 +56957,325 @@
       <c r="D69" s="30"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C70" s="30" t="s">
+      <c r="D70" s="30"/>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C71" s="30" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C71" s="30">
-        <f t="shared" ref="C71:C81" si="1">COUNTIF($C$5:$C$47,C5)</f>
-        <v>1</v>
       </c>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C72" s="30">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($C$5:$C$48,C5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C73" s="30">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($C$5:$C$48,C6)</f>
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C74" s="30">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($C$5:$C$48,C7)</f>
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C75" s="30">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($C$5:$C$48,C8)</f>
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C76" s="30">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($C$5:$C$48,C9)</f>
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C77" s="30">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($C$5:$C$48,C10)</f>
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C78" s="30">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($C$5:$C$48,C11)</f>
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C79" s="30">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($C$5:$C$48,C12)</f>
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C80" s="30">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($C$5:$C$48,C13)</f>
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C81" s="30">
-        <f t="shared" si="1"/>
+        <f>COUNTIF($C$5:$C$48,C14)</f>
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="28">
-        <v>1</v>
-      </c>
       <c r="C82" s="30">
-        <f t="shared" ref="C82:C92" si="2">COUNTIF($C$5:$C$47,C17)</f>
+        <f>COUNTIF($C$5:$C$48,C15)</f>
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C83" s="30">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($C$5:$C$48,C17)</f>
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C84" s="30">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($C$5:$C$48,C18)</f>
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C85" s="30">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($C$5:$C$48,C19)</f>
         <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C86" s="30">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($C$5:$C$48,C20)</f>
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C87" s="30">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($C$5:$C$48,C21)</f>
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C88" s="30">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($C$5:$C$48,C22)</f>
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="28">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C89" s="30">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($C$5:$C$48,C23)</f>
         <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="28">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C90" s="30">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($C$5:$C$48,C24)</f>
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C91" s="30">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($C$5:$C$48,C25)</f>
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="28">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C92" s="30">
-        <f t="shared" si="2"/>
+        <f>COUNTIF($C$5:$C$48,C26)</f>
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="28">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C93" s="30">
-        <f t="shared" ref="C93:C104" si="3">COUNTIF($C$5:$C$47,C29)</f>
+        <f>COUNTIF($C$5:$C$48,C27)</f>
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="28">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C94" s="30">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($C$5:$C$48,C29)</f>
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="28">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C95" s="30">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($C$5:$C$48,C30)</f>
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="28">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C96" s="30">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($C$5:$C$48,C31)</f>
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="28">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C97" s="30">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($C$5:$C$48,C32)</f>
         <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="28">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C98" s="30">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($C$5:$C$48,C33)</f>
         <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="28">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C99" s="30">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($C$5:$C$48,C34)</f>
         <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="28">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C100" s="30">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($C$5:$C$48,C35)</f>
         <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="28">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C101" s="30">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($C$5:$C$48,C36)</f>
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="28">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C102" s="30">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($C$5:$C$48,C37)</f>
         <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="28">
+        <v>21</v>
+      </c>
+      <c r="C103" s="30">
+        <f>COUNTIF($C$5:$C$48,C38)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="28">
         <v>22</v>
       </c>
-      <c r="C103" s="30">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B104"/>
       <c r="C104" s="30">
-        <f t="shared" si="3"/>
+        <f>COUNTIF($C$5:$C$48,C39)</f>
         <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B105"/>
       <c r="C105" s="30">
-        <f t="shared" ref="C105:C110" si="4">COUNTIF($C$5:$C$47,C42)</f>
+        <f>COUNTIF($C$5:$C$48,C40)</f>
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B106"/>
       <c r="C106" s="30">
-        <f t="shared" si="4"/>
+        <f>COUNTIF($C$5:$C$48,C42)</f>
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B107"/>
       <c r="C107" s="30">
-        <f t="shared" si="4"/>
+        <f>COUNTIF($C$5:$C$48,C43)</f>
         <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B108"/>
       <c r="C108" s="30">
-        <f t="shared" si="4"/>
+        <f>COUNTIF($C$5:$C$48,C44)</f>
         <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B109"/>
       <c r="C109" s="30">
-        <f t="shared" si="4"/>
+        <f>COUNTIF($C$5:$C$48,C45)</f>
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B110"/>
       <c r="C110" s="30">
-        <f t="shared" si="4"/>
+        <f>COUNTIF($C$5:$C$48,C46)</f>
         <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B111"/>
-      <c r="C111" s="30"/>
+      <c r="C111" s="30">
+        <f>COUNTIF($C$5:$C$48,C48)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="112" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B112"/>
@@ -57162,25 +57315,26 @@
     </row>
     <row r="121" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B121"/>
+      <c r="C121" s="30"/>
     </row>
     <row r="122" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B122"/>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B123" s="29"/>
-      <c r="C123" s="29"/>
-      <c r="D123" s="29"/>
-    </row>
-    <row r="124" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B124"/>
-      <c r="C124"/>
-    </row>
-    <row r="126" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B126" s="35"/>
-      <c r="C126"/>
-    </row>
-    <row r="130" spans="2:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="B130"/>
+    <row r="123" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B123"/>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B124" s="29"/>
+      <c r="C124" s="29"/>
+      <c r="D124" s="29"/>
+    </row>
+    <row r="125" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B125"/>
+      <c r="C125"/>
+    </row>
+    <row r="127" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B127" s="35"/>
+      <c r="C127"/>
     </row>
     <row r="131" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B131"/>
@@ -57190,6 +57344,9 @@
     </row>
     <row r="133" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B133"/>
+    </row>
+    <row r="134" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B134"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -57802,11 +57959,11 @@
       </c>
       <c r="B25" s="380" t="str">
         <f>IF(A25="*","",SUP!B73)</f>
-        <v>MINWAS</v>
+        <v>MINWMU</v>
       </c>
       <c r="C25" s="380" t="str">
         <f>IF(A25="*","",SUP!A73)</f>
-        <v>Extraction of Waste</v>
+        <v>Extraction of Waste for material use</v>
       </c>
       <c r="D25" t="s">
         <v>239</v>
@@ -59847,12 +60004,12 @@
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B48" s="380" t="str">
-        <f>NameConv!C47</f>
-        <v>WAS</v>
+        <f>NameConv!C48</f>
+        <v>WMU</v>
       </c>
       <c r="C48" s="380" t="str">
-        <f>NameConv!B47</f>
-        <v>Waste</v>
+        <f>NameConv!B48</f>
+        <v>Waste for material use</v>
       </c>
       <c r="D48" s="381" t="s">
         <v>239</v>
@@ -65360,15 +65517,15 @@
     <row r="73" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="158" t="str">
         <f t="shared" si="24"/>
-        <v>Extraction of Waste</v>
+        <v>Extraction of Waste for material use</v>
       </c>
       <c r="B73" s="30" t="str">
         <f>$B$46&amp;D73</f>
-        <v>MINWAS</v>
+        <v>MINWMU</v>
       </c>
       <c r="D73" s="159" t="str">
-        <f>NameConv!C47</f>
-        <v>WAS</v>
+        <f>NameConv!C48</f>
+        <v>WMU</v>
       </c>
       <c r="E73" s="30">
         <v>0</v>

</xml_diff>

<commit_message>
SetsAndMaps updated to accommodate Electric Trucks.
</commit_message>
<xml_diff>
--- a/VT_REGION1_SUP.xlsx
+++ b/VT_REGION1_SUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585E59CF-A4DC-40FD-9929-B3FD556B7504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C36BA9-7E79-44BD-85F8-5AB71E2DBD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="11" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
+    <workbookView xWindow="-1995" yWindow="-16155" windowWidth="26610" windowHeight="13740" firstSheet="4" activeTab="11" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -55420,7 +55420,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="18">
         <f ca="1">NOW()</f>
-        <v>45201.73094212963</v>
+        <v>45202.444356018517</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -56244,7 +56244,7 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
         <f ca="1">NOW()</f>
-        <v>45201.73094212963</v>
+        <v>45202.444356018517</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -56966,67 +56966,67 @@
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C72" s="30">
-        <f>COUNTIF($C$5:$C$48,C5)</f>
+        <f t="shared" ref="C72:C82" si="1">COUNTIF($C$5:$C$48,C5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C73" s="30">
-        <f>COUNTIF($C$5:$C$48,C6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C74" s="30">
-        <f>COUNTIF($C$5:$C$48,C7)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C75" s="30">
-        <f>COUNTIF($C$5:$C$48,C8)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C76" s="30">
-        <f>COUNTIF($C$5:$C$48,C9)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C77" s="30">
-        <f>COUNTIF($C$5:$C$48,C10)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C78" s="30">
-        <f>COUNTIF($C$5:$C$48,C11)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C79" s="30">
-        <f>COUNTIF($C$5:$C$48,C12)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C80" s="30">
-        <f>COUNTIF($C$5:$C$48,C13)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C81" s="30">
-        <f>COUNTIF($C$5:$C$48,C14)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C82" s="30">
-        <f>COUNTIF($C$5:$C$48,C15)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -57035,7 +57035,7 @@
         <v>1</v>
       </c>
       <c r="C83" s="30">
-        <f>COUNTIF($C$5:$C$48,C17)</f>
+        <f t="shared" ref="C83:C93" si="2">COUNTIF($C$5:$C$48,C17)</f>
         <v>1</v>
       </c>
     </row>
@@ -57044,7 +57044,7 @@
         <v>2</v>
       </c>
       <c r="C84" s="30">
-        <f>COUNTIF($C$5:$C$48,C18)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -57053,7 +57053,7 @@
         <v>3</v>
       </c>
       <c r="C85" s="30">
-        <f>COUNTIF($C$5:$C$48,C19)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -57062,7 +57062,7 @@
         <v>4</v>
       </c>
       <c r="C86" s="30">
-        <f>COUNTIF($C$5:$C$48,C20)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -57071,7 +57071,7 @@
         <v>5</v>
       </c>
       <c r="C87" s="30">
-        <f>COUNTIF($C$5:$C$48,C21)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -57080,7 +57080,7 @@
         <v>6</v>
       </c>
       <c r="C88" s="30">
-        <f>COUNTIF($C$5:$C$48,C22)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -57089,7 +57089,7 @@
         <v>7</v>
       </c>
       <c r="C89" s="30">
-        <f>COUNTIF($C$5:$C$48,C23)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -57098,7 +57098,7 @@
         <v>8</v>
       </c>
       <c r="C90" s="30">
-        <f>COUNTIF($C$5:$C$48,C24)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -57107,7 +57107,7 @@
         <v>9</v>
       </c>
       <c r="C91" s="30">
-        <f>COUNTIF($C$5:$C$48,C25)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -57116,7 +57116,7 @@
         <v>10</v>
       </c>
       <c r="C92" s="30">
-        <f>COUNTIF($C$5:$C$48,C26)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -57125,7 +57125,7 @@
         <v>11</v>
       </c>
       <c r="C93" s="30">
-        <f>COUNTIF($C$5:$C$48,C27)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -57134,7 +57134,7 @@
         <v>12</v>
       </c>
       <c r="C94" s="30">
-        <f>COUNTIF($C$5:$C$48,C29)</f>
+        <f t="shared" ref="C94:C105" si="3">COUNTIF($C$5:$C$48,C29)</f>
         <v>1</v>
       </c>
     </row>
@@ -57143,7 +57143,7 @@
         <v>13</v>
       </c>
       <c r="C95" s="30">
-        <f>COUNTIF($C$5:$C$48,C30)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -57152,7 +57152,7 @@
         <v>14</v>
       </c>
       <c r="C96" s="30">
-        <f>COUNTIF($C$5:$C$48,C31)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -57161,7 +57161,7 @@
         <v>15</v>
       </c>
       <c r="C97" s="30">
-        <f>COUNTIF($C$5:$C$48,C32)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -57170,7 +57170,7 @@
         <v>16</v>
       </c>
       <c r="C98" s="30">
-        <f>COUNTIF($C$5:$C$48,C33)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -57179,7 +57179,7 @@
         <v>17</v>
       </c>
       <c r="C99" s="30">
-        <f>COUNTIF($C$5:$C$48,C34)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -57188,7 +57188,7 @@
         <v>18</v>
       </c>
       <c r="C100" s="30">
-        <f>COUNTIF($C$5:$C$48,C35)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -57197,7 +57197,7 @@
         <v>19</v>
       </c>
       <c r="C101" s="30">
-        <f>COUNTIF($C$5:$C$48,C36)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -57206,7 +57206,7 @@
         <v>20</v>
       </c>
       <c r="C102" s="30">
-        <f>COUNTIF($C$5:$C$48,C37)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -57215,7 +57215,7 @@
         <v>21</v>
       </c>
       <c r="C103" s="30">
-        <f>COUNTIF($C$5:$C$48,C38)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -57224,14 +57224,14 @@
         <v>22</v>
       </c>
       <c r="C104" s="30">
-        <f>COUNTIF($C$5:$C$48,C39)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B105"/>
       <c r="C105" s="30">
-        <f>COUNTIF($C$5:$C$48,C40)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -57959,11 +57959,11 @@
       </c>
       <c r="B25" s="380" t="str">
         <f>IF(A25="*","",SUP!B73)</f>
-        <v>MINWMU</v>
+        <v>MINWAS</v>
       </c>
       <c r="C25" s="380" t="str">
         <f>IF(A25="*","",SUP!A73)</f>
-        <v>Extraction of Waste for material use</v>
+        <v>Extraction of Waste</v>
       </c>
       <c r="D25" t="s">
         <v>239</v>
@@ -58931,8 +58931,8 @@
   </sheetPr>
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -60004,8 +60004,8 @@
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B48" s="380" t="str">
-        <f>NameConv!C48</f>
-        <v>WMU</v>
+        <f>NameConv!C47</f>
+        <v>WAS</v>
       </c>
       <c r="C48" s="380" t="str">
         <f>NameConv!B48</f>
@@ -60380,8 +60380,8 @@
   </sheetPr>
   <dimension ref="A1:BA149"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62:I62"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -65517,15 +65517,15 @@
     <row r="73" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="158" t="str">
         <f t="shared" si="24"/>
-        <v>Extraction of Waste for material use</v>
+        <v>Extraction of Waste</v>
       </c>
       <c r="B73" s="30" t="str">
         <f>$B$46&amp;D73</f>
-        <v>MINWMU</v>
+        <v>MINWAS</v>
       </c>
       <c r="D73" s="159" t="str">
-        <f>NameConv!C48</f>
-        <v>WMU</v>
+        <f>NameConv!C47</f>
+        <v>WAS</v>
       </c>
       <c r="E73" s="30">
         <v>0</v>

</xml_diff>

<commit_message>
Added biomass upper limit
Limit is based on SAEON energy atlas.
Roughly 170PJ of woody type biomass, and another 165 PJ of other (residues mostly) biomass. Simple assumption that this can double by 2050.
</commit_message>
<xml_diff>
--- a/VT_REGION1_SUP.xlsx
+++ b/VT_REGION1_SUP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C36BA9-7E79-44BD-85F8-5AB71E2DBD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46FB913-A1D7-426D-897B-0B96F682DF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1995" yWindow="-16155" windowWidth="26610" windowHeight="13740" firstSheet="4" activeTab="11" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -222,6 +222,7 @@
     <author>tc={54934D05-AB8B-43EA-94D5-DA4230739148}</author>
     <author>tc={2D025629-877F-4A51-97DF-4B63BC17F90B}</author>
     <author>tc={00B9291C-0286-423F-9703-F64CCB57F70F}</author>
+    <author>tc={8CA7C0EF-537D-4038-B56F-15FCD6E67C52}</author>
     <author>tc={87179AE4-EC17-4370-98D7-F32C73BD771A}</author>
     <author>tc={E69A6D97-9056-4FB3-8A4E-00F5B2E78FD6}</author>
     <author>tc={F93D2D09-DC95-4216-81E9-77B6F290F34D}</author>
@@ -625,6 +626,14 @@
     Parity with coal in R/GJ assumed</t>
       </text>
     </comment>
+    <comment ref="K71" authorId="9" shapeId="0" xr:uid="{8CA7C0EF-537D-4038-B56F-15FCD6E67C52}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Bio and BIW estimates here from SAEON 2021 bio atlas report. Grouped the woody stuff together, and the other biomass like residues and agriculture residues together as biomass opther</t>
+      </text>
+    </comment>
     <comment ref="K73" authorId="1" shapeId="0" xr:uid="{7AD99044-2159-464B-9AD0-B1D99E091866}">
       <text>
         <r>
@@ -673,7 +682,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F83" authorId="9" shapeId="0" xr:uid="{87179AE4-EC17-4370-98D7-F32C73BD771A}">
+    <comment ref="F83" authorId="10" shapeId="0" xr:uid="{87179AE4-EC17-4370-98D7-F32C73BD771A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -681,7 +690,7 @@
     IRP 2019 costs adjusted to 2022</t>
       </text>
     </comment>
-    <comment ref="K86" authorId="10" shapeId="0" xr:uid="{E69A6D97-9056-4FB3-8A4E-00F5B2E78FD6}">
+    <comment ref="K86" authorId="11" shapeId="0" xr:uid="{E69A6D97-9056-4FB3-8A4E-00F5B2E78FD6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -689,7 +698,7 @@
     From EB</t>
       </text>
     </comment>
-    <comment ref="K87" authorId="11" shapeId="0" xr:uid="{F93D2D09-DC95-4216-81E9-77B6F290F34D}">
+    <comment ref="K87" authorId="12" shapeId="0" xr:uid="{F93D2D09-DC95-4216-81E9-77B6F290F34D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -697,7 +706,7 @@
     From EB</t>
       </text>
     </comment>
-    <comment ref="K89" authorId="12" shapeId="0" xr:uid="{8598790D-79A8-4FAB-8E0F-9A4DEE58CC36}">
+    <comment ref="K89" authorId="13" shapeId="0" xr:uid="{8598790D-79A8-4FAB-8E0F-9A4DEE58CC36}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -705,7 +714,7 @@
     Net imports from EB</t>
       </text>
     </comment>
-    <comment ref="K90" authorId="13" shapeId="0" xr:uid="{2FB1C6F0-AD57-4E16-BFAC-B7DB9955D691}">
+    <comment ref="K90" authorId="14" shapeId="0" xr:uid="{2FB1C6F0-AD57-4E16-BFAC-B7DB9955D691}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -713,7 +722,7 @@
     From energy balance</t>
       </text>
     </comment>
-    <comment ref="K94" authorId="14" shapeId="0" xr:uid="{B0A60D28-BB18-4A91-9004-62133F119943}">
+    <comment ref="K94" authorId="15" shapeId="0" xr:uid="{B0A60D28-BB18-4A91-9004-62133F119943}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -721,7 +730,7 @@
     From gas balance</t>
       </text>
     </comment>
-    <comment ref="F95" authorId="15" shapeId="0" xr:uid="{E56230BC-BD11-4915-915B-9473750B9EC2}">
+    <comment ref="F95" authorId="16" shapeId="0" xr:uid="{E56230BC-BD11-4915-915B-9473750B9EC2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -7398,6 +7407,57 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7435,57 +7495,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -24487,6 +24496,7 @@
   <person displayName="Bruno Merven" id="{E500B1BD-2FF0-4DFA-88F6-72D20CDE0583}" userId="Bruno Merven" providerId="None"/>
   <person displayName="bruno merven" id="{39BEAB33-522E-4FF7-A8C2-418D9E5A0410}" userId="144eb91ed0ec6402" providerId="Windows Live"/>
   <person displayName="Bruno Merven" id="{8B1FB5F6-C05B-4C45-A9FE-3B209CC95A5D}" userId="S::01405439@wf.uct.ac.za::c7f06137-2c3b-4c5c-8f38-fe1abbc96860" providerId="AD"/>
+  <person displayName="Bryce Mc Call" id="{C6B88F19-3945-4954-9F95-B87515BDF0C3}" userId="S::01425453@wf.uct.ac.za::bc1cdcf6-0dc9-4f2f-a1be-e4f2dea555d3" providerId="AD"/>
 </personList>
 </file>
 
@@ -24820,6 +24830,9 @@
   <threadedComment ref="F70" dT="2023-08-14T09:42:24.18" personId="{8B1FB5F6-C05B-4C45-A9FE-3B209CC95A5D}" id="{00B9291C-0286-423F-9703-F64CCB57F70F}">
     <text>Parity with coal in R/GJ assumed</text>
   </threadedComment>
+  <threadedComment ref="K71" dT="2023-10-09T13:11:28.72" personId="{C6B88F19-3945-4954-9F95-B87515BDF0C3}" id="{8CA7C0EF-537D-4038-B56F-15FCD6E67C52}">
+    <text>Bio and BIW estimates here from SAEON 2021 bio atlas report. Grouped the woody stuff together, and the other biomass like residues and agriculture residues together as biomass opther</text>
+  </threadedComment>
   <threadedComment ref="F83" dT="2023-09-07T10:07:04.92" personId="{8B1FB5F6-C05B-4C45-A9FE-3B209CC95A5D}" id="{87179AE4-EC17-4370-98D7-F32C73BD771A}">
     <text>IRP 2019 costs adjusted to 2022</text>
   </threadedComment>
@@ -24912,7 +24925,7 @@
   <dimension ref="A2:AE144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24962,25 +24975,25 @@
       <c r="W6" s="175" t="s">
         <v>361</v>
       </c>
-      <c r="AC6" s="416" t="s">
+      <c r="AC6" s="433" t="s">
         <v>362</v>
       </c>
-      <c r="AD6" s="416"/>
-      <c r="AE6" s="416"/>
+      <c r="AD6" s="433"/>
+      <c r="AE6" s="433"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="417" t="s">
+      <c r="A7" s="434" t="s">
         <v>363</v>
       </c>
-      <c r="B7" s="419" t="s">
+      <c r="B7" s="436" t="s">
         <v>364</v>
       </c>
-      <c r="C7" s="421" t="s">
+      <c r="C7" s="438" t="s">
         <v>365</v>
       </c>
-      <c r="D7" s="422"/>
-      <c r="E7" s="423"/>
-      <c r="F7" s="426" t="s">
+      <c r="D7" s="439"/>
+      <c r="E7" s="440"/>
+      <c r="F7" s="443" t="s">
         <v>366</v>
       </c>
       <c r="G7" s="176"/>
@@ -25008,12 +25021,12 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="418"/>
-      <c r="B8" s="420"/>
-      <c r="C8" s="424"/>
-      <c r="D8" s="425"/>
-      <c r="E8" s="425"/>
-      <c r="F8" s="427"/>
+      <c r="A8" s="435"/>
+      <c r="B8" s="437"/>
+      <c r="C8" s="441"/>
+      <c r="D8" s="442"/>
+      <c r="E8" s="442"/>
+      <c r="F8" s="444"/>
       <c r="G8" s="176"/>
       <c r="H8" s="176"/>
       <c r="I8" s="176"/>
@@ -25879,11 +25892,11 @@
       <c r="I25" s="57"/>
       <c r="J25" s="57"/>
       <c r="V25" s="217"/>
-      <c r="AC25" s="415" t="s">
+      <c r="AC25" s="432" t="s">
         <v>432</v>
       </c>
-      <c r="AD25" s="415"/>
-      <c r="AE25" s="415"/>
+      <c r="AD25" s="432"/>
+      <c r="AE25" s="432"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C26" s="57"/>
@@ -25962,8 +25975,8 @@
       <c r="D30" s="57"/>
     </row>
     <row r="31" spans="1:31" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H31" s="435"/>
-      <c r="I31" s="435"/>
+      <c r="H31" s="428"/>
+      <c r="I31" s="428"/>
       <c r="R31" t="s">
         <v>370</v>
       </c>
@@ -25984,10 +25997,10 @@
       </c>
     </row>
     <row r="32" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L32" s="428" t="s">
+      <c r="L32" s="420" t="s">
         <v>436</v>
       </c>
-      <c r="M32" s="436" t="s">
+      <c r="M32" s="429" t="s">
         <v>437</v>
       </c>
       <c r="N32" s="220" t="s">
@@ -26002,22 +26015,22 @@
       <c r="Q32" s="223" t="s">
         <v>439</v>
       </c>
-      <c r="R32" s="428" t="s">
+      <c r="R32" s="420" t="s">
         <v>389</v>
       </c>
-      <c r="S32" s="428" t="s">
+      <c r="S32" s="420" t="s">
         <v>393</v>
       </c>
-      <c r="T32" s="428" t="s">
+      <c r="T32" s="420" t="s">
         <v>440</v>
       </c>
-      <c r="U32" s="428" t="s">
+      <c r="U32" s="420" t="s">
         <v>389</v>
       </c>
-      <c r="V32" s="428" t="s">
+      <c r="V32" s="420" t="s">
         <v>393</v>
       </c>
-      <c r="W32" s="428" t="s">
+      <c r="W32" s="420" t="s">
         <v>440</v>
       </c>
     </row>
@@ -26040,28 +26053,28 @@
       <c r="G33" s="142" t="s">
         <v>444</v>
       </c>
-      <c r="H33" s="431" t="s">
+      <c r="H33" s="427" t="s">
         <v>445</v>
       </c>
-      <c r="I33" s="431"/>
+      <c r="I33" s="427"/>
       <c r="J33" s="142" t="s">
         <v>443</v>
       </c>
       <c r="K33" t="s">
         <v>444</v>
       </c>
-      <c r="L33" s="429"/>
-      <c r="M33" s="437"/>
+      <c r="L33" s="421"/>
+      <c r="M33" s="430"/>
       <c r="N33" s="16"/>
       <c r="O33" s="73"/>
       <c r="P33" s="73"/>
       <c r="Q33" s="224"/>
-      <c r="R33" s="429"/>
-      <c r="S33" s="429"/>
-      <c r="T33" s="429"/>
-      <c r="U33" s="429"/>
-      <c r="V33" s="429"/>
-      <c r="W33" s="429"/>
+      <c r="R33" s="421"/>
+      <c r="S33" s="421"/>
+      <c r="T33" s="421"/>
+      <c r="U33" s="421"/>
+      <c r="V33" s="421"/>
+      <c r="W33" s="421"/>
     </row>
     <row r="34" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -26081,8 +26094,8 @@
       <c r="K34" t="s">
         <v>447</v>
       </c>
-      <c r="L34" s="430"/>
-      <c r="M34" s="438"/>
+      <c r="L34" s="422"/>
+      <c r="M34" s="431"/>
       <c r="N34" s="225" t="s">
         <v>449</v>
       </c>
@@ -26095,12 +26108,12 @@
       <c r="Q34" s="227" t="s">
         <v>449</v>
       </c>
-      <c r="R34" s="430"/>
-      <c r="S34" s="430"/>
-      <c r="T34" s="430"/>
-      <c r="U34" s="430"/>
-      <c r="V34" s="430"/>
-      <c r="W34" s="430"/>
+      <c r="R34" s="422"/>
+      <c r="S34" s="422"/>
+      <c r="T34" s="422"/>
+      <c r="U34" s="422"/>
+      <c r="V34" s="422"/>
+      <c r="W34" s="422"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="228" t="s">
@@ -26166,7 +26179,7 @@
         <v>2.9</v>
       </c>
       <c r="I36" s="237"/>
-      <c r="L36" s="432" t="str">
+      <c r="L36" s="423" t="str">
         <f>A36</f>
         <v>Well completion</v>
       </c>
@@ -26246,7 +26259,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="I37" s="237"/>
-      <c r="L37" s="433"/>
+      <c r="L37" s="424"/>
       <c r="M37" t="str">
         <f t="shared" ref="M37:M45" si="5">B37</f>
         <v>Jiang et al. (2011)</v>
@@ -26317,7 +26330,7 @@
         <v>7.8</v>
       </c>
       <c r="I38" s="237"/>
-      <c r="L38" s="433"/>
+      <c r="L38" s="424"/>
       <c r="M38" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26392,7 +26405,7 @@
       </c>
       <c r="I39" s="237"/>
       <c r="K39" s="237"/>
-      <c r="L39" s="433"/>
+      <c r="L39" s="424"/>
       <c r="M39" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26463,7 +26476,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="I40" s="237"/>
-      <c r="L40" s="433"/>
+      <c r="L40" s="424"/>
       <c r="M40" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26537,7 +26550,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="I41" s="237"/>
-      <c r="L41" s="434"/>
+      <c r="L41" s="425"/>
       <c r="M41" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Broderick et al. (2011)</v>
@@ -26611,7 +26624,7 @@
         <v>4.2</v>
       </c>
       <c r="I42" s="237"/>
-      <c r="L42" s="432" t="s">
+      <c r="L42" s="423" t="s">
         <v>413</v>
       </c>
       <c r="M42" s="222" t="str">
@@ -26684,7 +26697,7 @@
         <v>3.5</v>
       </c>
       <c r="I43" s="237"/>
-      <c r="L43" s="433"/>
+      <c r="L43" s="424"/>
       <c r="M43" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26760,7 +26773,7 @@
       </c>
       <c r="I44" s="237"/>
       <c r="K44" s="237"/>
-      <c r="L44" s="433"/>
+      <c r="L44" s="424"/>
       <c r="M44" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26832,7 +26845,7 @@
         <v>8.9</v>
       </c>
       <c r="I45" s="237"/>
-      <c r="L45" s="434"/>
+      <c r="L45" s="425"/>
       <c r="M45" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26901,7 +26914,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="237"/>
-      <c r="L46" s="432" t="str">
+      <c r="L46" s="423" t="str">
         <f>A47</f>
         <v>Transport, storage and distribution</v>
       </c>
@@ -26977,7 +26990,7 @@
         <v>1.9</v>
       </c>
       <c r="I47" s="237"/>
-      <c r="L47" s="433"/>
+      <c r="L47" s="424"/>
       <c r="M47" t="str">
         <f>B48</f>
         <v>Skone et al. (2011)</v>
@@ -27048,7 +27061,7 @@
         <v>2.7</v>
       </c>
       <c r="I48" s="237"/>
-      <c r="L48" s="434"/>
+      <c r="L48" s="425"/>
       <c r="M48" s="95" t="str">
         <f>B49</f>
         <v>Howarth et al. (2011)</v>
@@ -27417,10 +27430,10 @@
       <c r="C79" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="D79" s="444" t="s">
+      <c r="D79" s="426" t="s">
         <v>498</v>
       </c>
-      <c r="E79" s="444"/>
+      <c r="E79" s="426"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
@@ -27522,13 +27535,13 @@
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="439" t="s">
+      <c r="A103" s="415" t="s">
         <v>508</v>
       </c>
       <c r="B103" s="266" t="s">
         <v>509</v>
       </c>
-      <c r="C103" s="441" t="s">
+      <c r="C103" s="417" t="s">
         <v>510</v>
       </c>
       <c r="D103" s="266">
@@ -27539,11 +27552,11 @@
       </c>
     </row>
     <row r="104" spans="1:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="440"/>
+      <c r="A104" s="416"/>
       <c r="B104" s="266" t="s">
         <v>511</v>
       </c>
-      <c r="C104" s="442"/>
+      <c r="C104" s="418"/>
       <c r="D104" s="266">
         <v>0.18</v>
       </c>
@@ -27556,13 +27569,13 @@
       </c>
     </row>
     <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="439" t="s">
+      <c r="A105" s="415" t="s">
         <v>512</v>
       </c>
       <c r="B105" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C105" s="442"/>
+      <c r="C105" s="418"/>
       <c r="D105" s="266">
         <v>0</v>
       </c>
@@ -27571,11 +27584,11 @@
       </c>
     </row>
     <row r="106" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="440"/>
+      <c r="A106" s="416"/>
       <c r="B106" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C106" s="443"/>
+      <c r="C106" s="419"/>
       <c r="D106" s="266">
         <v>0</v>
       </c>
@@ -27584,13 +27597,13 @@
       </c>
     </row>
     <row r="107" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="439" t="s">
+      <c r="A107" s="415" t="s">
         <v>508</v>
       </c>
       <c r="B107" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C107" s="441" t="s">
+      <c r="C107" s="417" t="s">
         <v>515</v>
       </c>
       <c r="D107" s="266">
@@ -27601,11 +27614,11 @@
       </c>
     </row>
     <row r="108" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="440"/>
+      <c r="A108" s="416"/>
       <c r="B108" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C108" s="442"/>
+      <c r="C108" s="418"/>
       <c r="D108" s="266">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -27614,13 +27627,13 @@
       </c>
     </row>
     <row r="109" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="439" t="s">
+      <c r="A109" s="415" t="s">
         <v>512</v>
       </c>
       <c r="B109" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C109" s="442"/>
+      <c r="C109" s="418"/>
       <c r="D109" s="266">
         <v>0</v>
       </c>
@@ -27629,11 +27642,11 @@
       </c>
     </row>
     <row r="110" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="440"/>
+      <c r="A110" s="416"/>
       <c r="B110" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C110" s="443"/>
+      <c r="C110" s="419"/>
       <c r="D110" s="266">
         <v>0</v>
       </c>
@@ -29096,6 +29109,22 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="AC25:AE25"/>
+    <mergeCell ref="AC6:AE6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="W32:W34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="L36:L41"/>
+    <mergeCell ref="L42:L45"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="L32:L34"/>
+    <mergeCell ref="M32:M34"/>
+    <mergeCell ref="R32:R34"/>
+    <mergeCell ref="S32:S34"/>
+    <mergeCell ref="T32:T34"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="C107:C110"/>
     <mergeCell ref="A109:A110"/>
@@ -29106,22 +29135,6 @@
     <mergeCell ref="A103:A104"/>
     <mergeCell ref="C103:C106"/>
     <mergeCell ref="A105:A106"/>
-    <mergeCell ref="W32:W34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="L36:L41"/>
-    <mergeCell ref="L42:L45"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="L32:L34"/>
-    <mergeCell ref="M32:M34"/>
-    <mergeCell ref="R32:R34"/>
-    <mergeCell ref="S32:S34"/>
-    <mergeCell ref="T32:T34"/>
-    <mergeCell ref="AC25:AE25"/>
-    <mergeCell ref="AC6:AE6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29872,7 +29885,7 @@
   </sheetPr>
   <dimension ref="A1:AE119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
@@ -49948,18 +49961,18 @@
         <f>FORECAST(CR93,CP94:CQ94,CP93:CQ93)</f>
         <v>93</v>
       </c>
-      <c r="DL94" s="431" t="s">
+      <c r="DL94" s="427" t="s">
         <v>762</v>
       </c>
-      <c r="DM94" s="431"/>
-      <c r="DN94" s="431" t="s">
+      <c r="DM94" s="427"/>
+      <c r="DN94" s="427" t="s">
         <v>763</v>
       </c>
-      <c r="DO94" s="431"/>
-      <c r="DP94" s="431" t="s">
+      <c r="DO94" s="427"/>
+      <c r="DP94" s="427" t="s">
         <v>761</v>
       </c>
-      <c r="DQ94" s="431"/>
+      <c r="DQ94" s="427"/>
     </row>
     <row r="95" spans="1:121" x14ac:dyDescent="0.25">
       <c r="BK95" t="s">
@@ -55420,7 +55433,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="18">
         <f ca="1">NOW()</f>
-        <v>45202.444356018517</v>
+        <v>45208.632217708335</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -56244,7 +56257,7 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
         <f ca="1">NOW()</f>
-        <v>45202.444356018517</v>
+        <v>45208.632217708335</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -60380,8 +60393,8 @@
   </sheetPr>
   <dimension ref="A1:BA149"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="U75" sqref="U75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -65400,12 +65413,18 @@
         <f t="shared" si="28"/>
         <v>59.346000000000004</v>
       </c>
-      <c r="J71" s="82"/>
-      <c r="K71" s="82"/>
-      <c r="L71" s="82"/>
+      <c r="J71" s="82">
+        <v>3</v>
+      </c>
+      <c r="K71" s="82">
+        <v>167</v>
+      </c>
       <c r="M71"/>
       <c r="N71"/>
-      <c r="O71"/>
+      <c r="O71" s="82">
+        <f>K71*2</f>
+        <v>334</v>
+      </c>
       <c r="P71"/>
       <c r="Q71" t="str">
         <f t="shared" si="27"/>
@@ -65473,12 +65492,18 @@
         <f t="shared" si="29"/>
         <v>56.52</v>
       </c>
-      <c r="J72" s="82"/>
-      <c r="K72" s="82"/>
-      <c r="L72" s="82"/>
+      <c r="J72" s="82">
+        <v>3</v>
+      </c>
+      <c r="K72" s="82">
+        <v>177</v>
+      </c>
       <c r="M72"/>
       <c r="N72"/>
-      <c r="O72"/>
+      <c r="O72" s="82">
+        <f>K72*2</f>
+        <v>354</v>
+      </c>
       <c r="P72"/>
       <c r="Q72" t="str">
         <f t="shared" si="27"/>

</xml_diff>

<commit_message>
Changed assumption about biomass availability
It was an assumption of being able to double by 2050. Reduced this to an inrease of only 50% by 2050 instead.
</commit_message>
<xml_diff>
--- a/VT_REGION1_SUP.xlsx
+++ b/VT_REGION1_SUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43E5C72-57F1-4C8B-9F1A-7C8EBC9814DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E255922-BBF7-4710-9F86-FF9047F61E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="345" windowWidth="23460" windowHeight="14985" activeTab="6" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -7411,6 +7411,17 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="8" fontId="10" fillId="0" borderId="0" xfId="12" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="6" fillId="5" borderId="68" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7418,6 +7429,57 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -7459,57 +7521,6 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7525,17 +7536,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="6" fillId="5" borderId="68" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Accent2" xfId="10" builtinId="33"/>
@@ -24999,25 +24999,25 @@
       <c r="W6" s="175" t="s">
         <v>361</v>
       </c>
-      <c r="AC6" s="416" t="s">
+      <c r="AC6" s="438" t="s">
         <v>362</v>
       </c>
-      <c r="AD6" s="416"/>
-      <c r="AE6" s="416"/>
+      <c r="AD6" s="438"/>
+      <c r="AE6" s="438"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="417" t="s">
+      <c r="A7" s="439" t="s">
         <v>363</v>
       </c>
-      <c r="B7" s="419" t="s">
+      <c r="B7" s="441" t="s">
         <v>364</v>
       </c>
-      <c r="C7" s="421" t="s">
+      <c r="C7" s="443" t="s">
         <v>365</v>
       </c>
-      <c r="D7" s="422"/>
-      <c r="E7" s="423"/>
-      <c r="F7" s="426" t="s">
+      <c r="D7" s="444"/>
+      <c r="E7" s="445"/>
+      <c r="F7" s="448" t="s">
         <v>366</v>
       </c>
       <c r="G7" s="176"/>
@@ -25045,12 +25045,12 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="418"/>
-      <c r="B8" s="420"/>
-      <c r="C8" s="424"/>
-      <c r="D8" s="425"/>
-      <c r="E8" s="425"/>
-      <c r="F8" s="427"/>
+      <c r="A8" s="440"/>
+      <c r="B8" s="442"/>
+      <c r="C8" s="446"/>
+      <c r="D8" s="447"/>
+      <c r="E8" s="447"/>
+      <c r="F8" s="449"/>
       <c r="G8" s="176"/>
       <c r="H8" s="176"/>
       <c r="I8" s="176"/>
@@ -25916,11 +25916,11 @@
       <c r="I25" s="57"/>
       <c r="J25" s="57"/>
       <c r="V25" s="217"/>
-      <c r="AC25" s="415" t="s">
+      <c r="AC25" s="437" t="s">
         <v>432</v>
       </c>
-      <c r="AD25" s="415"/>
-      <c r="AE25" s="415"/>
+      <c r="AD25" s="437"/>
+      <c r="AE25" s="437"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C26" s="57"/>
@@ -25999,8 +25999,8 @@
       <c r="D30" s="57"/>
     </row>
     <row r="31" spans="1:31" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H31" s="435"/>
-      <c r="I31" s="435"/>
+      <c r="H31" s="433"/>
+      <c r="I31" s="433"/>
       <c r="R31" t="s">
         <v>370</v>
       </c>
@@ -26021,10 +26021,10 @@
       </c>
     </row>
     <row r="32" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L32" s="428" t="s">
+      <c r="L32" s="425" t="s">
         <v>436</v>
       </c>
-      <c r="M32" s="436" t="s">
+      <c r="M32" s="434" t="s">
         <v>437</v>
       </c>
       <c r="N32" s="220" t="s">
@@ -26039,22 +26039,22 @@
       <c r="Q32" s="223" t="s">
         <v>439</v>
       </c>
-      <c r="R32" s="428" t="s">
+      <c r="R32" s="425" t="s">
         <v>389</v>
       </c>
-      <c r="S32" s="428" t="s">
+      <c r="S32" s="425" t="s">
         <v>393</v>
       </c>
-      <c r="T32" s="428" t="s">
+      <c r="T32" s="425" t="s">
         <v>440</v>
       </c>
-      <c r="U32" s="428" t="s">
+      <c r="U32" s="425" t="s">
         <v>389</v>
       </c>
-      <c r="V32" s="428" t="s">
+      <c r="V32" s="425" t="s">
         <v>393</v>
       </c>
-      <c r="W32" s="428" t="s">
+      <c r="W32" s="425" t="s">
         <v>440</v>
       </c>
     </row>
@@ -26077,28 +26077,28 @@
       <c r="G33" s="142" t="s">
         <v>444</v>
       </c>
-      <c r="H33" s="431" t="s">
+      <c r="H33" s="432" t="s">
         <v>445</v>
       </c>
-      <c r="I33" s="431"/>
+      <c r="I33" s="432"/>
       <c r="J33" s="142" t="s">
         <v>443</v>
       </c>
       <c r="K33" t="s">
         <v>444</v>
       </c>
-      <c r="L33" s="429"/>
-      <c r="M33" s="437"/>
+      <c r="L33" s="426"/>
+      <c r="M33" s="435"/>
       <c r="N33" s="16"/>
       <c r="O33" s="73"/>
       <c r="P33" s="73"/>
       <c r="Q33" s="224"/>
-      <c r="R33" s="429"/>
-      <c r="S33" s="429"/>
-      <c r="T33" s="429"/>
-      <c r="U33" s="429"/>
-      <c r="V33" s="429"/>
-      <c r="W33" s="429"/>
+      <c r="R33" s="426"/>
+      <c r="S33" s="426"/>
+      <c r="T33" s="426"/>
+      <c r="U33" s="426"/>
+      <c r="V33" s="426"/>
+      <c r="W33" s="426"/>
     </row>
     <row r="34" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -26118,8 +26118,8 @@
       <c r="K34" t="s">
         <v>447</v>
       </c>
-      <c r="L34" s="430"/>
-      <c r="M34" s="438"/>
+      <c r="L34" s="427"/>
+      <c r="M34" s="436"/>
       <c r="N34" s="225" t="s">
         <v>449</v>
       </c>
@@ -26132,12 +26132,12 @@
       <c r="Q34" s="227" t="s">
         <v>449</v>
       </c>
-      <c r="R34" s="430"/>
-      <c r="S34" s="430"/>
-      <c r="T34" s="430"/>
-      <c r="U34" s="430"/>
-      <c r="V34" s="430"/>
-      <c r="W34" s="430"/>
+      <c r="R34" s="427"/>
+      <c r="S34" s="427"/>
+      <c r="T34" s="427"/>
+      <c r="U34" s="427"/>
+      <c r="V34" s="427"/>
+      <c r="W34" s="427"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="228" t="s">
@@ -26203,7 +26203,7 @@
         <v>2.9</v>
       </c>
       <c r="I36" s="237"/>
-      <c r="L36" s="432" t="str">
+      <c r="L36" s="428" t="str">
         <f>A36</f>
         <v>Well completion</v>
       </c>
@@ -26283,7 +26283,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="I37" s="237"/>
-      <c r="L37" s="433"/>
+      <c r="L37" s="429"/>
       <c r="M37" t="str">
         <f t="shared" ref="M37:M45" si="5">B37</f>
         <v>Jiang et al. (2011)</v>
@@ -26354,7 +26354,7 @@
         <v>7.8</v>
       </c>
       <c r="I38" s="237"/>
-      <c r="L38" s="433"/>
+      <c r="L38" s="429"/>
       <c r="M38" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26429,7 +26429,7 @@
       </c>
       <c r="I39" s="237"/>
       <c r="K39" s="237"/>
-      <c r="L39" s="433"/>
+      <c r="L39" s="429"/>
       <c r="M39" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26500,7 +26500,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="I40" s="237"/>
-      <c r="L40" s="433"/>
+      <c r="L40" s="429"/>
       <c r="M40" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26574,7 +26574,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="I41" s="237"/>
-      <c r="L41" s="434"/>
+      <c r="L41" s="430"/>
       <c r="M41" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Broderick et al. (2011)</v>
@@ -26648,7 +26648,7 @@
         <v>4.2</v>
       </c>
       <c r="I42" s="237"/>
-      <c r="L42" s="432" t="s">
+      <c r="L42" s="428" t="s">
         <v>413</v>
       </c>
       <c r="M42" s="222" t="str">
@@ -26721,7 +26721,7 @@
         <v>3.5</v>
       </c>
       <c r="I43" s="237"/>
-      <c r="L43" s="433"/>
+      <c r="L43" s="429"/>
       <c r="M43" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26797,7 +26797,7 @@
       </c>
       <c r="I44" s="237"/>
       <c r="K44" s="237"/>
-      <c r="L44" s="433"/>
+      <c r="L44" s="429"/>
       <c r="M44" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26869,7 +26869,7 @@
         <v>8.9</v>
       </c>
       <c r="I45" s="237"/>
-      <c r="L45" s="434"/>
+      <c r="L45" s="430"/>
       <c r="M45" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26938,7 +26938,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="237"/>
-      <c r="L46" s="432" t="str">
+      <c r="L46" s="428" t="str">
         <f>A47</f>
         <v>Transport, storage and distribution</v>
       </c>
@@ -27014,7 +27014,7 @@
         <v>1.9</v>
       </c>
       <c r="I47" s="237"/>
-      <c r="L47" s="433"/>
+      <c r="L47" s="429"/>
       <c r="M47" t="str">
         <f>B48</f>
         <v>Skone et al. (2011)</v>
@@ -27085,7 +27085,7 @@
         <v>2.7</v>
       </c>
       <c r="I48" s="237"/>
-      <c r="L48" s="434"/>
+      <c r="L48" s="430"/>
       <c r="M48" s="95" t="str">
         <f>B49</f>
         <v>Howarth et al. (2011)</v>
@@ -27454,10 +27454,10 @@
       <c r="C79" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="D79" s="444" t="s">
+      <c r="D79" s="431" t="s">
         <v>498</v>
       </c>
-      <c r="E79" s="444"/>
+      <c r="E79" s="431"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
@@ -27559,13 +27559,13 @@
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="439" t="s">
+      <c r="A103" s="420" t="s">
         <v>508</v>
       </c>
       <c r="B103" s="266" t="s">
         <v>509</v>
       </c>
-      <c r="C103" s="441" t="s">
+      <c r="C103" s="422" t="s">
         <v>510</v>
       </c>
       <c r="D103" s="266">
@@ -27576,11 +27576,11 @@
       </c>
     </row>
     <row r="104" spans="1:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="440"/>
+      <c r="A104" s="421"/>
       <c r="B104" s="266" t="s">
         <v>511</v>
       </c>
-      <c r="C104" s="442"/>
+      <c r="C104" s="423"/>
       <c r="D104" s="266">
         <v>0.18</v>
       </c>
@@ -27593,13 +27593,13 @@
       </c>
     </row>
     <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="439" t="s">
+      <c r="A105" s="420" t="s">
         <v>512</v>
       </c>
       <c r="B105" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C105" s="442"/>
+      <c r="C105" s="423"/>
       <c r="D105" s="266">
         <v>0</v>
       </c>
@@ -27608,11 +27608,11 @@
       </c>
     </row>
     <row r="106" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="440"/>
+      <c r="A106" s="421"/>
       <c r="B106" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C106" s="443"/>
+      <c r="C106" s="424"/>
       <c r="D106" s="266">
         <v>0</v>
       </c>
@@ -27621,13 +27621,13 @@
       </c>
     </row>
     <row r="107" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="439" t="s">
+      <c r="A107" s="420" t="s">
         <v>508</v>
       </c>
       <c r="B107" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C107" s="441" t="s">
+      <c r="C107" s="422" t="s">
         <v>515</v>
       </c>
       <c r="D107" s="266">
@@ -27638,11 +27638,11 @@
       </c>
     </row>
     <row r="108" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="440"/>
+      <c r="A108" s="421"/>
       <c r="B108" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C108" s="442"/>
+      <c r="C108" s="423"/>
       <c r="D108" s="266">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -27651,13 +27651,13 @@
       </c>
     </row>
     <row r="109" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="439" t="s">
+      <c r="A109" s="420" t="s">
         <v>512</v>
       </c>
       <c r="B109" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C109" s="442"/>
+      <c r="C109" s="423"/>
       <c r="D109" s="266">
         <v>0</v>
       </c>
@@ -27666,11 +27666,11 @@
       </c>
     </row>
     <row r="110" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="440"/>
+      <c r="A110" s="421"/>
       <c r="B110" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C110" s="443"/>
+      <c r="C110" s="424"/>
       <c r="D110" s="266">
         <v>0</v>
       </c>
@@ -29133,6 +29133,22 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="AC25:AE25"/>
+    <mergeCell ref="AC6:AE6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="W32:W34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="L36:L41"/>
+    <mergeCell ref="L42:L45"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="L32:L34"/>
+    <mergeCell ref="M32:M34"/>
+    <mergeCell ref="R32:R34"/>
+    <mergeCell ref="S32:S34"/>
+    <mergeCell ref="T32:T34"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="C107:C110"/>
     <mergeCell ref="A109:A110"/>
@@ -29143,22 +29159,6 @@
     <mergeCell ref="A103:A104"/>
     <mergeCell ref="C103:C106"/>
     <mergeCell ref="A105:A106"/>
-    <mergeCell ref="W32:W34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="L36:L41"/>
-    <mergeCell ref="L42:L45"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="L32:L34"/>
-    <mergeCell ref="M32:M34"/>
-    <mergeCell ref="R32:R34"/>
-    <mergeCell ref="S32:S34"/>
-    <mergeCell ref="T32:T34"/>
-    <mergeCell ref="AC25:AE25"/>
-    <mergeCell ref="AC6:AE6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -49985,18 +49985,18 @@
         <f>FORECAST(CR93,CP94:CQ94,CP93:CQ93)</f>
         <v>93</v>
       </c>
-      <c r="DL94" s="431" t="s">
+      <c r="DL94" s="432" t="s">
         <v>762</v>
       </c>
-      <c r="DM94" s="431"/>
-      <c r="DN94" s="431" t="s">
+      <c r="DM94" s="432"/>
+      <c r="DN94" s="432" t="s">
         <v>763</v>
       </c>
-      <c r="DO94" s="431"/>
-      <c r="DP94" s="431" t="s">
+      <c r="DO94" s="432"/>
+      <c r="DP94" s="432" t="s">
         <v>761</v>
       </c>
-      <c r="DQ94" s="431"/>
+      <c r="DQ94" s="432"/>
     </row>
     <row r="95" spans="1:121" x14ac:dyDescent="0.25">
       <c r="BK95" t="s">
@@ -53285,10 +53285,10 @@
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.25">
       <c r="C32" s="8"/>
-      <c r="D32" s="445" t="s">
+      <c r="D32" s="450" t="s">
         <v>743</v>
       </c>
-      <c r="E32" s="445"/>
+      <c r="E32" s="450"/>
       <c r="F32" s="363">
         <f>AVERAGE(F25:F31)</f>
         <v>286.69885714285715</v>
@@ -54392,7 +54392,7 @@
       </c>
       <c r="Q73" s="8"/>
       <c r="R73" s="8"/>
-      <c r="S73" s="446">
+      <c r="S73" s="451">
         <v>1.59</v>
       </c>
       <c r="T73" s="374">
@@ -54430,7 +54430,7 @@
       </c>
       <c r="Q74" s="8"/>
       <c r="R74" s="8"/>
-      <c r="S74" s="447"/>
+      <c r="S74" s="452"/>
       <c r="T74" s="1">
         <v>11.1</v>
       </c>
@@ -54601,7 +54601,7 @@
       </c>
       <c r="Q79" s="8"/>
       <c r="R79" s="8"/>
-      <c r="S79" s="448">
+      <c r="S79" s="453">
         <f>S73*Z73</f>
         <v>1.955477980665951</v>
       </c>
@@ -54645,7 +54645,7 @@
       </c>
       <c r="Q80" s="8"/>
       <c r="R80" s="8"/>
-      <c r="S80" s="449"/>
+      <c r="S80" s="454"/>
       <c r="T80" s="374">
         <f>T74*$Z$73</f>
         <v>13.651450053705695</v>
@@ -54765,7 +54765,7 @@
       </c>
       <c r="Q85" s="8"/>
       <c r="R85" s="8"/>
-      <c r="S85" s="448">
+      <c r="S85" s="453">
         <f>S79*Y75</f>
         <v>22.096901181525247</v>
       </c>
@@ -54798,7 +54798,7 @@
       </c>
       <c r="Q86" s="8"/>
       <c r="R86" s="8"/>
-      <c r="S86" s="449"/>
+      <c r="S86" s="454"/>
       <c r="T86" s="374">
         <f>T80*$Y$75</f>
         <v>154.26138560687437</v>
@@ -55457,7 +55457,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="18">
         <f ca="1">NOW()</f>
-        <v>45209.719746643517</v>
+        <v>45211.606016666665</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -56281,7 +56281,7 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
         <f ca="1">NOW()</f>
-        <v>45209.719746643517</v>
+        <v>45211.606016666665</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -60418,11 +60418,11 @@
   <dimension ref="A1:BF149"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <pane xSplit="5" ySplit="10" topLeftCell="J84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="10" topLeftCell="F63" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A49" sqref="A49"/>
       <selection pane="topRight" activeCell="F49" sqref="F49"/>
       <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
-      <selection pane="bottomRight" activeCell="J97" sqref="J97"/>
+      <selection pane="bottomRight" activeCell="L73" sqref="L73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -60463,11 +60463,11 @@
       <c r="A3" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="B3" s="412" t="s">
+      <c r="B3" s="417" t="s">
         <v>231</v>
       </c>
-      <c r="C3" s="412"/>
-      <c r="D3" s="412"/>
+      <c r="C3" s="417"/>
+      <c r="D3" s="417"/>
       <c r="E3" s="37" t="s">
         <v>232</v>
       </c>
@@ -61577,11 +61577,11 @@
       </c>
       <c r="N13" s="48"/>
       <c r="O13" s="48"/>
-      <c r="P13" s="450"/>
-      <c r="Q13" s="450"/>
-      <c r="R13" s="450"/>
-      <c r="S13" s="450"/>
-      <c r="T13" s="450"/>
+      <c r="P13" s="412"/>
+      <c r="Q13" s="412"/>
+      <c r="R13" s="412"/>
+      <c r="S13" s="412"/>
+      <c r="T13" s="412"/>
       <c r="U13" s="49"/>
       <c r="V13" s="405"/>
       <c r="W13" s="47"/>
@@ -62366,11 +62366,11 @@
       </c>
       <c r="N28"/>
       <c r="O28" s="84"/>
-      <c r="P28" s="451"/>
-      <c r="Q28" s="451"/>
-      <c r="R28" s="451"/>
-      <c r="S28" s="451"/>
-      <c r="T28" s="451"/>
+      <c r="P28" s="413"/>
+      <c r="Q28" s="413"/>
+      <c r="R28" s="413"/>
+      <c r="S28" s="413"/>
+      <c r="T28" s="413"/>
       <c r="U28" s="85" t="s">
         <v>256</v>
       </c>
@@ -62450,11 +62450,11 @@
       <c r="O29" s="90" t="s">
         <v>252</v>
       </c>
-      <c r="P29" s="452"/>
-      <c r="Q29" s="452"/>
-      <c r="R29" s="452"/>
-      <c r="S29" s="452"/>
-      <c r="T29" s="452"/>
+      <c r="P29" s="414"/>
+      <c r="Q29" s="414"/>
+      <c r="R29" s="414"/>
+      <c r="S29" s="414"/>
+      <c r="T29" s="414"/>
       <c r="U29" s="91" t="s">
         <v>260</v>
       </c>
@@ -62558,11 +62558,11 @@
       <c r="O30" s="90" t="s">
         <v>266</v>
       </c>
-      <c r="P30" s="452"/>
-      <c r="Q30" s="452"/>
-      <c r="R30" s="452"/>
-      <c r="S30" s="452"/>
-      <c r="T30" s="452"/>
+      <c r="P30" s="414"/>
+      <c r="Q30" s="414"/>
+      <c r="R30" s="414"/>
+      <c r="S30" s="414"/>
+      <c r="T30" s="414"/>
       <c r="U30" s="93" t="s">
         <v>267</v>
       </c>
@@ -62666,11 +62666,11 @@
       <c r="O31" s="90" t="s">
         <v>273</v>
       </c>
-      <c r="P31" s="452"/>
-      <c r="Q31" s="452"/>
-      <c r="R31" s="452"/>
-      <c r="S31" s="452"/>
-      <c r="T31" s="452"/>
+      <c r="P31" s="414"/>
+      <c r="Q31" s="414"/>
+      <c r="R31" s="414"/>
+      <c r="S31" s="414"/>
+      <c r="T31" s="414"/>
       <c r="U31" s="93" t="s">
         <v>274</v>
       </c>
@@ -62774,11 +62774,11 @@
       <c r="O32" s="90" t="s">
         <v>277</v>
       </c>
-      <c r="P32" s="452"/>
-      <c r="Q32" s="452"/>
-      <c r="R32" s="452"/>
-      <c r="S32" s="452"/>
-      <c r="T32" s="452"/>
+      <c r="P32" s="414"/>
+      <c r="Q32" s="414"/>
+      <c r="R32" s="414"/>
+      <c r="S32" s="414"/>
+      <c r="T32" s="414"/>
       <c r="U32" s="93" t="s">
         <v>278</v>
       </c>
@@ -62882,11 +62882,11 @@
       <c r="O33" s="90" t="s">
         <v>283</v>
       </c>
-      <c r="P33" s="452"/>
-      <c r="Q33" s="452"/>
-      <c r="R33" s="452"/>
-      <c r="S33" s="452"/>
-      <c r="T33" s="452"/>
+      <c r="P33" s="414"/>
+      <c r="Q33" s="414"/>
+      <c r="R33" s="414"/>
+      <c r="S33" s="414"/>
+      <c r="T33" s="414"/>
       <c r="U33" s="93" t="s">
         <v>284</v>
       </c>
@@ -63175,15 +63175,15 @@
         <v>117.73934470134871</v>
       </c>
       <c r="G37" s="45">
-        <f>IF($J37,($E37*G$16+$AA37)*G$15/1.055,F37)</f>
+        <f t="shared" ref="G37:I42" si="10">IF($J37,($E37*G$16+$AA37)*G$15/1.055,F37)</f>
         <v>121.47218561739591</v>
       </c>
       <c r="H37" s="45">
-        <f>IF($J37,($E37*H$16+$AA37)*H$15/1.055,G37)</f>
+        <f t="shared" si="10"/>
         <v>111.49620902079818</v>
       </c>
       <c r="I37" s="45">
-        <f>IF($J37,($E37*I$16+$AA37)*I$15/1.055,H37)</f>
+        <f t="shared" si="10"/>
         <v>142.01096096333239</v>
       </c>
       <c r="J37" s="109">
@@ -63192,11 +63192,11 @@
       <c r="O37" s="110">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="P37" s="453"/>
-      <c r="Q37" s="453"/>
-      <c r="R37" s="453"/>
-      <c r="S37" s="453"/>
-      <c r="T37" s="453"/>
+      <c r="P37" s="415"/>
+      <c r="Q37" s="415"/>
+      <c r="R37" s="415"/>
+      <c r="S37" s="415"/>
+      <c r="T37" s="415"/>
       <c r="U37" s="89">
         <f>(O37+V37)/2</f>
         <v>9.5000000000000001E-2</v>
@@ -63205,15 +63205,15 @@
         <v>0.12</v>
       </c>
       <c r="W37" s="112">
-        <f t="shared" ref="W37:Y40" si="10">$Z37</f>
+        <f t="shared" ref="W37:Y40" si="11">$Z37</f>
         <v>0.10454194041570421</v>
       </c>
       <c r="X37" s="112">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10454194041570421</v>
       </c>
       <c r="Y37" s="112">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10454194041570421</v>
       </c>
       <c r="Z37" s="89">
@@ -63286,15 +63286,15 @@
         <v>106.47694185774681</v>
       </c>
       <c r="G38" s="45">
-        <f>IF($J38,($E38*G$16+$AA38)*G$15/1.055,F38)</f>
+        <f t="shared" si="10"/>
         <v>106.47694185774681</v>
       </c>
       <c r="H38" s="45">
-        <f>IF($J38,($E38*H$16+$AA38)*H$15/1.055,G38)</f>
+        <f t="shared" si="10"/>
         <v>106.47694185774681</v>
       </c>
       <c r="I38" s="45">
-        <f>IF($J38,($E38*I$16+$AA38)*I$15/1.055,H38)</f>
+        <f t="shared" si="10"/>
         <v>106.47694185774681</v>
       </c>
       <c r="J38" s="109">
@@ -63303,11 +63303,11 @@
       <c r="O38" s="110">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="P38" s="453"/>
-      <c r="Q38" s="453"/>
-      <c r="R38" s="453"/>
-      <c r="S38" s="453"/>
-      <c r="T38" s="453"/>
+      <c r="P38" s="415"/>
+      <c r="Q38" s="415"/>
+      <c r="R38" s="415"/>
+      <c r="S38" s="415"/>
+      <c r="T38" s="415"/>
       <c r="U38" s="89">
         <f>(O38+V38)/2</f>
         <v>8.5000000000000006E-2</v>
@@ -63316,15 +63316,15 @@
         <v>0.1</v>
       </c>
       <c r="W38" s="112">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.4541940415704198E-2</v>
       </c>
       <c r="X38" s="112">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.4541940415704198E-2</v>
       </c>
       <c r="Y38" s="112">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.4541940415704198E-2</v>
       </c>
       <c r="Z38" s="89">
@@ -63399,15 +63399,15 @@
         <v>113.39810629656337</v>
       </c>
       <c r="G39" s="45">
-        <f>IF($J39,($E39*G$16+$AA39)*G$15/1.055,F39)</f>
+        <f t="shared" si="10"/>
         <v>113.39810629656337</v>
       </c>
       <c r="H39" s="45">
-        <f>IF($J39,($E39*H$16+$AA39)*H$15/1.055,G39)</f>
+        <f t="shared" si="10"/>
         <v>113.39810629656337</v>
       </c>
       <c r="I39" s="45">
-        <f>IF($J39,($E39*I$16+$AA39)*I$15/1.055,H39)</f>
+        <f t="shared" si="10"/>
         <v>113.39810629656337</v>
       </c>
       <c r="J39" s="109">
@@ -63416,11 +63416,11 @@
       <c r="O39" s="110">
         <v>0.06</v>
       </c>
-      <c r="P39" s="453"/>
-      <c r="Q39" s="453"/>
-      <c r="R39" s="453"/>
-      <c r="S39" s="453"/>
-      <c r="T39" s="453"/>
+      <c r="P39" s="415"/>
+      <c r="Q39" s="415"/>
+      <c r="R39" s="415"/>
+      <c r="S39" s="415"/>
+      <c r="T39" s="415"/>
       <c r="U39" s="89">
         <f>(O39+V39)/2</f>
         <v>0.08</v>
@@ -63429,15 +63429,15 @@
         <v>0.1</v>
       </c>
       <c r="W39" s="112">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10068731146567374</v>
       </c>
       <c r="X39" s="112">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10068731146567374</v>
       </c>
       <c r="Y39" s="112">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10068731146567374</v>
       </c>
       <c r="Z39" s="114">
@@ -63512,15 +63512,15 @@
         <v>117.73934470134871</v>
       </c>
       <c r="G40" s="45">
-        <f>IF($J40,($E40*G$16+$AA40)*G$15/1.055,F40)</f>
+        <f t="shared" si="10"/>
         <v>117.73934470134871</v>
       </c>
       <c r="H40" s="45">
-        <f>IF($J40,($E40*H$16+$AA40)*H$15/1.055,G40)</f>
+        <f t="shared" si="10"/>
         <v>117.73934470134871</v>
       </c>
       <c r="I40" s="45">
-        <f>IF($J40,($E40*I$16+$AA40)*I$15/1.055,H40)</f>
+        <f t="shared" si="10"/>
         <v>117.73934470134871</v>
       </c>
       <c r="J40" s="109">
@@ -63529,11 +63529,11 @@
       <c r="O40" s="110">
         <v>0.03</v>
       </c>
-      <c r="P40" s="453"/>
-      <c r="Q40" s="453"/>
-      <c r="R40" s="453"/>
-      <c r="S40" s="453"/>
-      <c r="T40" s="453"/>
+      <c r="P40" s="415"/>
+      <c r="Q40" s="415"/>
+      <c r="R40" s="415"/>
+      <c r="S40" s="415"/>
+      <c r="T40" s="415"/>
       <c r="U40" s="89">
         <f>(O40+V40)/2</f>
         <v>5.5E-2</v>
@@ -63542,15 +63542,15 @@
         <v>0.08</v>
       </c>
       <c r="W40" s="112">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10454194041570421</v>
       </c>
       <c r="X40" s="112">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10454194041570421</v>
       </c>
       <c r="Y40" s="112">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.10454194041570421</v>
       </c>
       <c r="Z40" s="89">
@@ -63581,15 +63581,15 @@
         <v>143.92309452816528</v>
       </c>
       <c r="G41" s="45">
-        <f>IF($J41,($E41*G$16+$AA41)*G$15/1.055,F41)</f>
+        <f t="shared" si="10"/>
         <v>148.28833379773559</v>
       </c>
       <c r="H41" s="45">
-        <f>IF($J41,($E41*H$16+$AA41)*H$15/1.055,G41)</f>
+        <f t="shared" si="10"/>
         <v>136.62227950525954</v>
       </c>
       <c r="I41" s="45">
-        <f>IF($J41,($E41*I$16+$AA41)*I$15/1.055,H41)</f>
+        <f t="shared" si="10"/>
         <v>172.30668087048045</v>
       </c>
       <c r="J41" s="109">
@@ -63598,11 +63598,11 @@
       <c r="O41" s="110">
         <v>0.1</v>
       </c>
-      <c r="P41" s="453"/>
-      <c r="Q41" s="453"/>
-      <c r="R41" s="453"/>
-      <c r="S41" s="453"/>
-      <c r="T41" s="453"/>
+      <c r="P41" s="415"/>
+      <c r="Q41" s="415"/>
+      <c r="R41" s="415"/>
+      <c r="S41" s="415"/>
+      <c r="T41" s="415"/>
       <c r="U41" s="116"/>
       <c r="V41" s="113">
         <v>0.16</v>
@@ -63649,15 +63649,15 @@
         <v>150.16006135280986</v>
       </c>
       <c r="G42" s="45">
-        <f>IF($J42,($E42*G$16+$AA42)*G$15/1.055,F42)</f>
+        <f t="shared" si="10"/>
         <v>154.52530062238017</v>
       </c>
       <c r="H42" s="45">
-        <f>IF($J42,($E42*H$16+$AA42)*H$15/1.055,G42)</f>
+        <f t="shared" si="10"/>
         <v>142.85924632990407</v>
       </c>
       <c r="I42" s="45">
-        <f>IF($J42,($E42*I$16+$AA42)*I$15/1.055,H42)</f>
+        <f t="shared" si="10"/>
         <v>178.543647695125</v>
       </c>
       <c r="J42" s="109">
@@ -63667,11 +63667,11 @@
         <f>O41</f>
         <v>0.1</v>
       </c>
-      <c r="P42" s="454"/>
-      <c r="Q42" s="454"/>
-      <c r="R42" s="454"/>
-      <c r="S42" s="454"/>
-      <c r="T42" s="454"/>
+      <c r="P42" s="416"/>
+      <c r="Q42" s="416"/>
+      <c r="R42" s="416"/>
+      <c r="S42" s="416"/>
+      <c r="T42" s="416"/>
       <c r="U42" s="120"/>
       <c r="V42" s="121">
         <v>0.16</v>
@@ -63745,31 +63745,31 @@
         <v>2010</v>
       </c>
       <c r="AP43" s="28">
-        <f t="shared" ref="AP43:AV43" si="11">AH43</f>
+        <f t="shared" ref="AP43:AV43" si="12">AH43</f>
         <v>2020</v>
       </c>
       <c r="AQ43" s="28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2025</v>
       </c>
       <c r="AR43" s="28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2030</v>
       </c>
       <c r="AS43" s="28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2035</v>
       </c>
       <c r="AT43" s="28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2040</v>
       </c>
       <c r="AU43" s="28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2045</v>
       </c>
       <c r="AV43" s="28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2050</v>
       </c>
     </row>
@@ -64305,35 +64305,35 @@
         <v>6DS</v>
       </c>
       <c r="AG54">
-        <f t="shared" ref="AG54:AN55" si="12">AG50*$AC$51+AG52*$AC$53</f>
+        <f t="shared" ref="AG54:AN55" si="13">AG50*$AC$51+AG52*$AC$53</f>
         <v>9</v>
       </c>
       <c r="AH54">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>12.5</v>
       </c>
       <c r="AI54">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>13</v>
       </c>
       <c r="AJ54">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
       <c r="AK54">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
       <c r="AL54">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
       <c r="AM54">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
       <c r="AN54">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
       <c r="AO54" s="89">
@@ -64341,31 +64341,31 @@
         <v>0.11538461538461539</v>
       </c>
       <c r="AP54" s="89">
-        <f t="shared" ref="AP54:AV55" si="13">AH54/AH44</f>
+        <f t="shared" ref="AP54:AV55" si="14">AH54/AH44</f>
         <v>0.1059322033898305</v>
       </c>
       <c r="AQ54" s="89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.10236220472440945</v>
       </c>
       <c r="AR54" s="89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.1044776119402985</v>
       </c>
       <c r="AS54" s="89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.1</v>
       </c>
       <c r="AT54" s="89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9.7902097902097904E-2</v>
       </c>
       <c r="AU54" s="89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.10273972602739725</v>
       </c>
       <c r="AV54" s="89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.10067114093959731</v>
       </c>
     </row>
@@ -64411,35 +64411,35 @@
         <v>2DS</v>
       </c>
       <c r="AG55">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
       <c r="AH55">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="AI55">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="AJ55">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="AK55">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>10.5</v>
       </c>
       <c r="AL55">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>10.5</v>
       </c>
       <c r="AM55">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>10</v>
       </c>
       <c r="AN55">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>9.5</v>
       </c>
       <c r="AO55" s="89">
@@ -64447,31 +64447,31 @@
         <v>0.11538461538461539</v>
       </c>
       <c r="AP55" s="89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.1134020618556701</v>
       </c>
       <c r="AQ55" s="89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.1134020618556701</v>
       </c>
       <c r="AR55" s="89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.1134020618556701</v>
       </c>
       <c r="AS55" s="89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.10824742268041238</v>
       </c>
       <c r="AT55" s="89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.11413043478260869</v>
       </c>
       <c r="AU55" s="89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.11235955056179775</v>
       </c>
       <c r="AV55" s="89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.10919540229885058</v>
       </c>
       <c r="AW55" s="30"/>
@@ -64494,19 +64494,19 @@
         <v>COST~0</v>
       </c>
       <c r="F56" s="386" t="str">
-        <f t="shared" ref="F56:I56" si="14">"COST"&amp;$E$52&amp;F57</f>
+        <f t="shared" ref="F56:I56" si="15">"COST"&amp;$E$52&amp;F57</f>
         <v>COST~2017</v>
       </c>
       <c r="G56" s="386" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>COST~2021</v>
       </c>
       <c r="H56" s="386" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>COST~2030</v>
       </c>
       <c r="I56" s="386" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>COST~2050</v>
       </c>
       <c r="J56" s="386" t="str">
@@ -64514,23 +64514,23 @@
         <v>BNDACT~UP~0</v>
       </c>
       <c r="K56" s="386" t="str">
-        <f t="shared" ref="K56:O56" si="15">"BNDACT~UP"&amp;$E$52&amp;K57</f>
+        <f t="shared" ref="K56:O56" si="16">"BNDACT~UP"&amp;$E$52&amp;K57</f>
         <v>BNDACT~UP~2017</v>
       </c>
       <c r="L56" s="386" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>BNDACT~UP~2019</v>
       </c>
       <c r="M56" s="386" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>BNDACT~UP~2021</v>
       </c>
       <c r="N56" s="386" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>BNDACT~UP~2030</v>
       </c>
       <c r="O56" s="386" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>BNDACT~UP~2050</v>
       </c>
       <c r="P56" s="386" t="str">
@@ -64538,19 +64538,19 @@
         <v>BNDACT~FX~0</v>
       </c>
       <c r="Q56" s="386" t="str">
-        <f t="shared" ref="Q56:T56" si="16">"BNDACT~FX"&amp;$E$52&amp;Q57</f>
+        <f t="shared" ref="Q56:T56" si="17">"BNDACT~FX"&amp;$E$52&amp;Q57</f>
         <v>BNDACT~FX~2020</v>
       </c>
       <c r="R56" s="386" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>BNDACT~FX~2030</v>
       </c>
       <c r="S56" s="386" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>BNDACT~FX~2040</v>
       </c>
       <c r="T56" s="386" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>BNDACT~FX~2050</v>
       </c>
       <c r="U56" s="386" t="s">
@@ -64578,77 +64578,77 @@
         <v>341</v>
       </c>
       <c r="AE56" s="145">
-        <f t="shared" ref="AE56:AL56" si="17">AVERAGE(AG54:AG55)</f>
+        <f t="shared" ref="AE56:AL56" si="18">AVERAGE(AG54:AG55)</f>
         <v>9</v>
       </c>
       <c r="AF56" s="145">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11.75</v>
       </c>
       <c r="AG56" s="145">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="AH56" s="145">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12.5</v>
       </c>
       <c r="AI56" s="145">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12.25</v>
       </c>
       <c r="AJ56" s="145">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12.25</v>
       </c>
       <c r="AK56" s="145">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12.5</v>
       </c>
       <c r="AL56" s="145">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12.25</v>
       </c>
       <c r="AM56" s="146">
-        <f t="shared" ref="AM56:AT56" si="18">AE56/AVERAGE(AG44:AG45)</f>
+        <f t="shared" ref="AM56:AT56" si="19">AE56/AVERAGE(AG44:AG45)</f>
         <v>0.11538461538461539</v>
       </c>
       <c r="AN56" s="146">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.10930232558139535</v>
       </c>
       <c r="AO56" s="146">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.10714285714285714</v>
       </c>
       <c r="AP56" s="146">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.10822510822510822</v>
       </c>
       <c r="AQ56" s="146">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.10337552742616034</v>
       </c>
       <c r="AR56" s="146">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.10425531914893617</v>
       </c>
       <c r="AS56" s="146">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.10638297872340426</v>
       </c>
       <c r="AT56" s="146">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.1038135593220339</v>
       </c>
       <c r="AU56" s="145"/>
-      <c r="AW56" s="413"/>
-      <c r="AX56" s="413"/>
-      <c r="AY56" s="413"/>
-      <c r="AZ56" s="413"/>
-      <c r="BA56" s="413"/>
-      <c r="BB56" s="413"/>
-      <c r="BC56" s="413"/>
+      <c r="AW56" s="418"/>
+      <c r="AX56" s="418"/>
+      <c r="AY56" s="418"/>
+      <c r="AZ56" s="418"/>
+      <c r="BA56" s="418"/>
+      <c r="BB56" s="418"/>
+      <c r="BC56" s="418"/>
     </row>
     <row r="57" spans="1:58" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A57" s="147" t="s">
@@ -64740,12 +64740,12 @@
       <c r="AS57" s="149"/>
       <c r="AT57" s="149"/>
       <c r="AU57" s="149"/>
-      <c r="AX57" s="414"/>
-      <c r="AY57" s="413"/>
-      <c r="AZ57" s="413"/>
-      <c r="BA57" s="413"/>
-      <c r="BB57" s="413"/>
-      <c r="BC57" s="413"/>
+      <c r="AX57" s="419"/>
+      <c r="AY57" s="418"/>
+      <c r="AZ57" s="418"/>
+      <c r="BA57" s="418"/>
+      <c r="BB57" s="418"/>
+      <c r="BC57" s="418"/>
       <c r="BE57" s="42"/>
       <c r="BF57" s="42"/>
     </row>
@@ -64859,7 +64859,7 @@
     </row>
     <row r="60" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="158" t="str">
-        <f t="shared" ref="A60:A65" si="19">"Extraction of "&amp;INDEX(FuelNamesLong,MATCH(D60,FuelNamesShort,0))</f>
+        <f t="shared" ref="A60:A65" si="20">"Extraction of "&amp;INDEX(FuelNamesLong,MATCH(D60,FuelNamesShort,0))</f>
         <v>Extraction of Coal</v>
       </c>
       <c r="B60" s="30" t="str">
@@ -64942,11 +64942,11 @@
     </row>
     <row r="61" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="158" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Extraction of Coal low grade</v>
       </c>
       <c r="B61" s="30" t="str">
-        <f t="shared" ref="B61:B67" si="20">$B$46&amp;D61</f>
+        <f t="shared" ref="B61:B67" si="21">$B$46&amp;D61</f>
         <v>MINCLE</v>
       </c>
       <c r="D61" s="159" t="str">
@@ -65022,11 +65022,11 @@
     </row>
     <row r="62" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="158" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Extraction of Coal Discard</v>
       </c>
       <c r="B62" s="30" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>MINCLD</v>
       </c>
       <c r="D62" s="159" t="str">
@@ -65041,15 +65041,15 @@
         <v>14.13</v>
       </c>
       <c r="G62" s="82">
-        <f t="shared" ref="G62:I62" si="21">G61/2</f>
+        <f t="shared" ref="G62:I62" si="22">G61/2</f>
         <v>14.13</v>
       </c>
       <c r="H62" s="82">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>14.13</v>
       </c>
       <c r="I62" s="82">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>14.13</v>
       </c>
       <c r="J62" s="82"/>
@@ -65093,11 +65093,11 @@
     </row>
     <row r="63" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="158" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Extraction of Oil Crude</v>
       </c>
       <c r="B63" s="30" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>MINOCR</v>
       </c>
       <c r="D63" s="159" t="str">
@@ -65138,7 +65138,7 @@
         <v>0</v>
       </c>
       <c r="O63">
-        <f t="shared" ref="O63" si="22">N63</f>
+        <f t="shared" ref="O63" si="23">N63</f>
         <v>0</v>
       </c>
       <c r="P63"/>
@@ -65176,11 +65176,11 @@
     </row>
     <row r="64" spans="1:58" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="158" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Extraction of Coastal Gas</v>
       </c>
       <c r="B64" s="30" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>MINGIC</v>
       </c>
       <c r="D64" s="159" t="str">
@@ -65258,11 +65258,11 @@
     </row>
     <row r="65" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="158" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Extraction of Gas Indigenous Ibhubezi</v>
       </c>
       <c r="B65" s="30" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>MINGIB</v>
       </c>
       <c r="D65" s="159" t="str">
@@ -65273,19 +65273,19 @@
         <v>0</v>
       </c>
       <c r="F65" s="82">
-        <f t="shared" ref="F65:I66" si="23">SUMIF($D$37:$D$42,$D65,F$37:F$42)*$E$54</f>
+        <f t="shared" ref="F65:I66" si="24">SUMIF($D$37:$D$42,$D65,F$37:F$42)*$E$54</f>
         <v>117.73934470134871</v>
       </c>
       <c r="G65" s="82">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>121.47218561739591</v>
       </c>
       <c r="H65" s="82">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>111.49620902079818</v>
       </c>
       <c r="I65" s="82">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>142.01096096333239</v>
       </c>
       <c r="J65" s="82">
@@ -65350,19 +65350,19 @@
         <v>0</v>
       </c>
       <c r="F66" s="82">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>106.47694185774681</v>
       </c>
       <c r="G66" s="82">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>106.47694185774681</v>
       </c>
       <c r="H66" s="82">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>106.47694185774681</v>
       </c>
       <c r="I66" s="82">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>106.47694185774681</v>
       </c>
       <c r="J66" s="82">
@@ -65415,7 +65415,7 @@
         <v>Extraction of Gas Indigenous Shale</v>
       </c>
       <c r="B67" s="30" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>MINGIH</v>
       </c>
       <c r="D67" s="159" t="str">
@@ -65540,11 +65540,11 @@
     </row>
     <row r="69" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="158" t="str">
-        <f t="shared" ref="A69:A76" si="24">"Extraction of "&amp;INDEX(FuelNamesLong,MATCH(D69,FuelNamesShort,0))</f>
+        <f t="shared" ref="A69:A76" si="25">"Extraction of "&amp;INDEX(FuelNamesLong,MATCH(D69,FuelNamesShort,0))</f>
         <v>Extraction of Biogas</v>
       </c>
       <c r="B69" s="30" t="str">
-        <f t="shared" ref="B69:B75" si="25">$B$46&amp;D69</f>
+        <f t="shared" ref="B69:B75" si="26">$B$46&amp;D69</f>
         <v>MINBIG</v>
       </c>
       <c r="D69" s="159" t="str">
@@ -65559,15 +65559,15 @@
         <v>59.346000000000004</v>
       </c>
       <c r="G69" s="82">
-        <f t="shared" ref="G69:I69" si="26">G71</f>
+        <f t="shared" ref="G69:I69" si="27">G71</f>
         <v>59.346000000000004</v>
       </c>
       <c r="H69" s="82">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>59.346000000000004</v>
       </c>
       <c r="I69" s="82">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>59.346000000000004</v>
       </c>
       <c r="J69" s="82"/>
@@ -65583,7 +65583,7 @@
       <c r="T69"/>
       <c r="U69"/>
       <c r="V69" t="str">
-        <f t="shared" ref="V69:V76" si="27">$V$60</f>
+        <f t="shared" ref="V69:V76" si="28">$V$60</f>
         <v/>
       </c>
       <c r="AA69" s="35"/>
@@ -65618,11 +65618,11 @@
     </row>
     <row r="70" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="158" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Extraction of Biomass bagasse</v>
       </c>
       <c r="B70" s="30" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>MINBIB</v>
       </c>
       <c r="D70" s="159" t="str">
@@ -65661,7 +65661,7 @@
       <c r="T70"/>
       <c r="U70"/>
       <c r="V70" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AA70" s="35"/>
@@ -65696,11 +65696,11 @@
     </row>
     <row r="71" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="158" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Extraction of Biomass Other</v>
       </c>
       <c r="B71" s="30" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>MINBIO</v>
       </c>
       <c r="D71" s="159" t="str">
@@ -65711,19 +65711,19 @@
         <v>0</v>
       </c>
       <c r="F71" s="82">
-        <f t="shared" ref="F71:I71" si="28">F60*1.05</f>
+        <f t="shared" ref="F71:I71" si="29">F60*1.05</f>
         <v>59.346000000000004</v>
       </c>
       <c r="G71" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>59.346000000000004</v>
       </c>
       <c r="H71" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>59.346000000000004</v>
       </c>
       <c r="I71" s="82">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>59.346000000000004</v>
       </c>
       <c r="J71" s="82">
@@ -65735,8 +65735,8 @@
       <c r="M71"/>
       <c r="N71"/>
       <c r="O71" s="82">
-        <f>K71*2</f>
-        <v>334</v>
+        <f>K71*1.5</f>
+        <v>250.5</v>
       </c>
       <c r="P71" s="82"/>
       <c r="Q71" s="82"/>
@@ -65745,7 +65745,7 @@
       <c r="T71" s="82"/>
       <c r="U71"/>
       <c r="V71" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AA71" s="35"/>
@@ -65780,11 +65780,11 @@
     </row>
     <row r="72" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="158" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Extraction of Biomass Wood</v>
       </c>
       <c r="B72" s="30" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>MINBIW</v>
       </c>
       <c r="D72" s="159" t="str">
@@ -65799,15 +65799,15 @@
         <v>56.52</v>
       </c>
       <c r="G72" s="82">
-        <f t="shared" ref="G72:I73" si="29">F72</f>
+        <f t="shared" ref="G72:I73" si="30">F72</f>
         <v>56.52</v>
       </c>
       <c r="H72" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>56.52</v>
       </c>
       <c r="I72" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>56.52</v>
       </c>
       <c r="J72" s="82">
@@ -65819,8 +65819,8 @@
       <c r="M72"/>
       <c r="N72"/>
       <c r="O72" s="82">
-        <f>K72*2</f>
-        <v>354</v>
+        <f>K72*1.5</f>
+        <v>265.5</v>
       </c>
       <c r="P72" s="82"/>
       <c r="Q72" s="82"/>
@@ -65829,7 +65829,7 @@
       <c r="T72" s="82"/>
       <c r="U72"/>
       <c r="V72" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AA72" s="35"/>
@@ -65864,7 +65864,7 @@
     </row>
     <row r="73" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="158" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Extraction of Waste</v>
       </c>
       <c r="B73" s="30" t="str">
@@ -65882,15 +65882,15 @@
         <v>0</v>
       </c>
       <c r="G73" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="H73" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="I73" s="82">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="J73" s="82">
@@ -65910,7 +65910,7 @@
       <c r="T73"/>
       <c r="U73"/>
       <c r="V73" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AA73" s="35"/>
@@ -65945,7 +65945,7 @@
     </row>
     <row r="74" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="158" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Extraction of Hydro</v>
       </c>
       <c r="B74" s="30" t="str">
@@ -65976,7 +65976,7 @@
       <c r="T74"/>
       <c r="U74"/>
       <c r="V74" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AA74" s="35"/>
@@ -66011,11 +66011,11 @@
     </row>
     <row r="75" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="158" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Extraction of Solar</v>
       </c>
       <c r="B75" s="30" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>MINSOL</v>
       </c>
       <c r="D75" s="159" t="str">
@@ -66042,7 +66042,7 @@
       <c r="T75"/>
       <c r="U75"/>
       <c r="V75" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AA75" s="35"/>
@@ -66077,7 +66077,7 @@
     </row>
     <row r="76" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="158" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Extraction of Wind</v>
       </c>
       <c r="B76" s="30" t="str">
@@ -66108,7 +66108,7 @@
       <c r="T76"/>
       <c r="U76"/>
       <c r="V76" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AA76" s="35"/>
@@ -66196,7 +66196,7 @@
     </row>
     <row r="78" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="158" t="str">
-        <f t="shared" ref="A78:A92" si="30">"Imports of "&amp;INDEX(FuelNamesLong,MATCH(D78,FuelNamesShort,0))</f>
+        <f t="shared" ref="A78:A92" si="31">"Imports of "&amp;INDEX(FuelNamesLong,MATCH(D78,FuelNamesShort,0))</f>
         <v>Imports of Coal Coking</v>
       </c>
       <c r="B78" s="30" t="str">
@@ -66211,7 +66211,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="82">
-        <f t="shared" ref="F78" si="31">F60*1.5</f>
+        <f t="shared" ref="F78" si="32">F60*1.5</f>
         <v>84.78</v>
       </c>
       <c r="G78" s="82">
@@ -66219,11 +66219,11 @@
         <v>84.78</v>
       </c>
       <c r="H78" s="82">
-        <f t="shared" ref="H78:I78" si="32">H60*1.5</f>
+        <f t="shared" ref="H78:I78" si="33">H60*1.5</f>
         <v>84.78</v>
       </c>
       <c r="I78" s="82">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>84.78</v>
       </c>
       <c r="J78" s="82">
@@ -66241,7 +66241,7 @@
       <c r="T78"/>
       <c r="U78"/>
       <c r="V78" t="str">
-        <f t="shared" ref="V78:V92" si="33">$V$60</f>
+        <f t="shared" ref="V78:V92" si="34">$V$60</f>
         <v/>
       </c>
       <c r="AA78" s="35"/>
@@ -66289,15 +66289,15 @@
         <v>8.7491242874264614</v>
       </c>
       <c r="G79" s="82">
-        <f t="shared" ref="G79:I79" si="34">G80/G15</f>
+        <f t="shared" ref="G79:I79" si="35">G80/G15</f>
         <v>9.0144883767620421</v>
       </c>
       <c r="H79" s="82">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>8.3053057450005809</v>
       </c>
       <c r="I79" s="82">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>10.474570265682702</v>
       </c>
       <c r="J79" s="82"/>
@@ -66345,7 +66345,7 @@
     </row>
     <row r="80" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="158" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Imports of Gas Regional LNG</v>
       </c>
       <c r="B80" s="30" t="str">
@@ -66360,19 +66360,19 @@
         <v>0</v>
       </c>
       <c r="F80" s="82">
-        <f t="shared" ref="F80:I81" si="35">SUMIF($C$37:$C$42,$B80,F$37:F$42)*$E$54</f>
+        <f t="shared" ref="F80:I81" si="36">SUMIF($C$37:$C$42,$B80,F$37:F$42)*$E$54</f>
         <v>143.92309452816528</v>
       </c>
       <c r="G80" s="82">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>148.28833379773559</v>
       </c>
       <c r="H80" s="82">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>136.62227950525954</v>
       </c>
       <c r="I80" s="82">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>172.30668087048045</v>
       </c>
       <c r="J80" s="82"/>
@@ -66390,7 +66390,7 @@
         <v>2027</v>
       </c>
       <c r="V80" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AA80" s="35"/>
@@ -66425,7 +66425,7 @@
     </row>
     <row r="81" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="158" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Imports of Gas International LNG</v>
       </c>
       <c r="B81" s="30" t="str">
@@ -66440,19 +66440,19 @@
         <v>0</v>
       </c>
       <c r="F81" s="82">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>150.16006135280986</v>
       </c>
       <c r="G81" s="82">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>154.52530062238017</v>
       </c>
       <c r="H81" s="82">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>142.85924632990407</v>
       </c>
       <c r="I81" s="82">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>178.543647695125</v>
       </c>
       <c r="J81" s="82" t="s">
@@ -66480,7 +66480,7 @@
         <v>2027</v>
       </c>
       <c r="V81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="Z81" s="161"/>
@@ -66529,15 +66529,15 @@
         <v>9.1282712068577432</v>
       </c>
       <c r="G82" s="82">
-        <f t="shared" ref="G82:I82" si="36">G81/G15</f>
+        <f t="shared" ref="G82:I82" si="37">G81/G15</f>
         <v>9.3936352961933238</v>
       </c>
       <c r="H82" s="82">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>8.6844526644318591</v>
       </c>
       <c r="I82" s="82">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>10.853717185113982</v>
       </c>
       <c r="J82" s="82"/>
@@ -66586,11 +66586,11 @@
     </row>
     <row r="83" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="158" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Imports of Nuclear</v>
       </c>
       <c r="B83" s="30" t="str">
-        <f t="shared" ref="B83:B91" si="37">"IMP"&amp;D83</f>
+        <f t="shared" ref="B83:B91" si="38">"IMP"&amp;D83</f>
         <v>IMPNUC</v>
       </c>
       <c r="D83" s="159" t="str">
@@ -66620,7 +66620,7 @@
         <v>0</v>
       </c>
       <c r="K83" s="82">
-        <f t="shared" ref="K83:K85" si="38">SUMIF($C$8:$BE$8,D83,$C$11:$BE$11)</f>
+        <f t="shared" ref="K83:K85" si="39">SUMIF($C$8:$BE$8,D83,$C$11:$BE$11)</f>
         <v>170.374545454545</v>
       </c>
       <c r="L83" s="82"/>
@@ -66634,7 +66634,7 @@
       <c r="T83"/>
       <c r="U83"/>
       <c r="V83" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="Y83" s="161" t="s">
@@ -66672,11 +66672,11 @@
     </row>
     <row r="84" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="158" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Imports of Oil Av Gasoline</v>
       </c>
       <c r="B84" s="30" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>IMPOAG</v>
       </c>
       <c r="D84" s="159" t="str">
@@ -66687,26 +66687,26 @@
         <v>0</v>
       </c>
       <c r="F84" s="82">
-        <f t="shared" ref="F84:I84" si="39">F87</f>
+        <f t="shared" ref="F84:I84" si="40">F87</f>
         <v>247.03405739193275</v>
       </c>
       <c r="G84" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>253.06623635843414</v>
       </c>
       <c r="H84" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>232.71621829347131</v>
       </c>
       <c r="I84" s="82">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>294.96333237453405</v>
       </c>
       <c r="J84" s="82">
         <v>0</v>
       </c>
       <c r="K84" s="82">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>1.394321535205479</v>
       </c>
       <c r="L84" s="82"/>
@@ -66720,7 +66720,7 @@
       <c r="T84"/>
       <c r="U84"/>
       <c r="V84" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AA84" s="35"/>
@@ -66755,11 +66755,11 @@
     </row>
     <row r="85" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="158" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Imports of Oil Crude</v>
       </c>
       <c r="B85" s="30" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>IMPOCR</v>
       </c>
       <c r="D85" s="159" t="str">
@@ -66770,26 +66770,26 @@
         <v>0</v>
       </c>
       <c r="F85" s="82">
-        <f t="shared" ref="F85:I90" si="40">SUMIF($E$22:$E$34,$D85,F$22:F$34)</f>
+        <f t="shared" ref="F85:I90" si="41">SUMIF($E$22:$E$34,$D85,F$22:F$34)</f>
         <v>196.45298120195667</v>
       </c>
       <c r="G85" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>202.68138113207547</v>
       </c>
       <c r="H85" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>186.03605031446543</v>
       </c>
       <c r="I85" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>236.95117987421381</v>
       </c>
       <c r="J85" s="82">
         <v>0</v>
       </c>
       <c r="K85" s="82">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>941.22622485351599</v>
       </c>
       <c r="L85" s="82"/>
@@ -66803,7 +66803,7 @@
       <c r="T85"/>
       <c r="U85"/>
       <c r="V85" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AA85" s="35"/>
@@ -66838,11 +66838,11 @@
     </row>
     <row r="86" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="158" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Imports of Oil Diesel</v>
       </c>
       <c r="B86" s="30" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>IMPODS</v>
       </c>
       <c r="D86" s="159" t="str">
@@ -66853,19 +66853,19 @@
         <v>0</v>
       </c>
       <c r="F86" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>236.56389169057414</v>
       </c>
       <c r="G86" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>244.65407088700817</v>
       </c>
       <c r="H86" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>224.41968109431471</v>
       </c>
       <c r="I86" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>286.31310869549469</v>
       </c>
       <c r="J86" s="82">
@@ -66885,7 +66885,7 @@
       <c r="T86"/>
       <c r="U86"/>
       <c r="V86" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AA86" s="35"/>
@@ -66920,11 +66920,11 @@
     </row>
     <row r="87" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="158" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Imports of Oil Gasoline</v>
       </c>
       <c r="B87" s="30" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>IMPOGS</v>
       </c>
       <c r="D87" s="159" t="str">
@@ -66935,19 +66935,19 @@
         <v>0</v>
       </c>
       <c r="F87" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>247.03405739193275</v>
       </c>
       <c r="G87" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>253.06623635843414</v>
       </c>
       <c r="H87" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>232.71621829347131</v>
       </c>
       <c r="I87" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>294.96333237453405</v>
       </c>
       <c r="J87" s="82">
@@ -66967,7 +66967,7 @@
       <c r="T87"/>
       <c r="U87"/>
       <c r="V87" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AA87" s="35"/>
@@ -67002,11 +67002,11 @@
     </row>
     <row r="88" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="158" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Imports of Oil HFO</v>
       </c>
       <c r="B88" s="30" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>IMPOHF</v>
       </c>
       <c r="D88" s="159" t="str">
@@ -67017,19 +67017,19 @@
         <v>0</v>
       </c>
       <c r="F88" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>196.45298120195667</v>
       </c>
       <c r="G88" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>202.68138113207547</v>
       </c>
       <c r="H88" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>186.03605031446543</v>
       </c>
       <c r="I88" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>236.95117987421381</v>
       </c>
       <c r="J88" s="82">
@@ -67049,7 +67049,7 @@
       <c r="T88"/>
       <c r="U88"/>
       <c r="V88" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AA88" s="35"/>
@@ -67084,11 +67084,11 @@
     </row>
     <row r="89" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="158" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Imports of Oil LPG</v>
       </c>
       <c r="B89" s="30" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>IMPOLP</v>
       </c>
       <c r="D89" s="159" t="str">
@@ -67099,19 +67099,19 @@
         <v>0</v>
       </c>
       <c r="F89" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>376.62224144497708</v>
       </c>
       <c r="G89" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>382.94989907290471</v>
       </c>
       <c r="H89" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>366.03930314149977</v>
       </c>
       <c r="I89" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>417.76583187285604</v>
       </c>
       <c r="J89" s="82">
@@ -67131,7 +67131,7 @@
       <c r="T89"/>
       <c r="U89"/>
       <c r="V89" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AA89" s="35"/>
@@ -67166,11 +67166,11 @@
     </row>
     <row r="90" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="158" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Imports of Oil Kerosene</v>
       </c>
       <c r="B90" s="30" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>IMPOKE</v>
       </c>
       <c r="D90" s="159" t="str">
@@ -67181,19 +67181,19 @@
         <v>0</v>
       </c>
       <c r="F90" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>243.45484454706207</v>
       </c>
       <c r="G90" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>250.76740309449676</v>
       </c>
       <c r="H90" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>231.22467020790273</v>
       </c>
       <c r="I90" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>291.00244139042559</v>
       </c>
       <c r="J90" s="82">
@@ -67213,7 +67213,7 @@
       <c r="T90"/>
       <c r="U90"/>
       <c r="V90" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AA90" s="35"/>
@@ -67248,11 +67248,11 @@
     </row>
     <row r="91" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="158" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Imports of Biodiesel</v>
       </c>
       <c r="B91" s="30" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>IMPBID</v>
       </c>
       <c r="D91" s="159" t="str">
@@ -67267,15 +67267,15 @@
         <v>248.39208627510286</v>
       </c>
       <c r="G91" s="82">
-        <f t="shared" ref="G91:I92" si="41">G86*1.05</f>
+        <f t="shared" ref="G91:I92" si="42">G86*1.05</f>
         <v>256.88677443135862</v>
       </c>
       <c r="H91" s="82">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>235.64066514903047</v>
       </c>
       <c r="I91" s="82">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>300.62876413026942</v>
       </c>
       <c r="J91" s="82">
@@ -67293,7 +67293,7 @@
       <c r="T91"/>
       <c r="U91"/>
       <c r="V91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AA91" s="35"/>
@@ -67328,7 +67328,7 @@
     </row>
     <row r="92" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="158" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>Imports of Bioethanol</v>
       </c>
       <c r="B92" s="30" t="str">
@@ -67347,15 +67347,15 @@
         <v>259.38576026152941</v>
       </c>
       <c r="G92" s="82">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>265.71954817635583</v>
       </c>
       <c r="H92" s="82">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>244.3520292081449</v>
       </c>
       <c r="I92" s="82">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>309.71149899326076</v>
       </c>
       <c r="J92" s="82">
@@ -67373,7 +67373,7 @@
       <c r="T92"/>
       <c r="U92"/>
       <c r="V92" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AA92" s="35"/>
@@ -67559,15 +67559,15 @@
         <v>125.48506135280986</v>
       </c>
       <c r="G95" s="82">
-        <f t="shared" ref="G95:I95" si="42">G81-(1.5*G15)</f>
+        <f t="shared" ref="G95:I95" si="43">G81-(1.5*G15)</f>
         <v>129.85030062238019</v>
       </c>
       <c r="H95" s="82">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>118.18424632990407</v>
       </c>
       <c r="I95" s="82">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>153.86864769512499</v>
       </c>
       <c r="J95" s="82"/>
@@ -67674,11 +67674,11 @@
     </row>
     <row r="97" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="158" t="str">
-        <f t="shared" ref="A97:A104" si="43">"Exports of "&amp;INDEX(FuelNamesLong,MATCH(C97,FuelNamesShort,0))</f>
+        <f t="shared" ref="A97:A104" si="44">"Exports of "&amp;INDEX(FuelNamesLong,MATCH(C97,FuelNamesShort,0))</f>
         <v>Exports of Coal</v>
       </c>
       <c r="B97" s="30" t="str">
-        <f t="shared" ref="B97:B104" si="44">"PEX"&amp;C97</f>
+        <f t="shared" ref="B97:B104" si="45">"PEX"&amp;C97</f>
         <v>PEXCOA</v>
       </c>
       <c r="C97" s="159" t="str">
@@ -67727,7 +67727,7 @@
       </c>
       <c r="U97"/>
       <c r="V97" t="str">
-        <f t="shared" ref="V97:V104" si="45">$V$60</f>
+        <f t="shared" ref="V97:V104" si="46">$V$60</f>
         <v/>
       </c>
       <c r="AA97" s="35"/>
@@ -67762,11 +67762,11 @@
     </row>
     <row r="98" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="158" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Exports of Coal Coking</v>
       </c>
       <c r="B98" s="30" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>PEXCOK</v>
       </c>
       <c r="C98" s="159" t="str">
@@ -67810,7 +67810,7 @@
       <c r="T98"/>
       <c r="U98"/>
       <c r="V98" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="AA98" s="35"/>
@@ -67845,11 +67845,11 @@
     </row>
     <row r="99" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="158" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Exports of Oil Av Gasoline</v>
       </c>
       <c r="B99" s="30" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>PEXOAG</v>
       </c>
       <c r="C99" s="159" t="str">
@@ -67860,19 +67860,19 @@
         <v>0</v>
       </c>
       <c r="F99" s="82">
-        <f t="shared" ref="F99:I99" si="46">F102</f>
+        <f t="shared" ref="F99:I99" si="47">F102</f>
         <v>-234.68235452233611</v>
       </c>
       <c r="G99" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-240.41292454051242</v>
       </c>
       <c r="H99" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-221.08040737879773</v>
       </c>
       <c r="I99" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-280.21516575580733</v>
       </c>
       <c r="J99" s="82">
@@ -67893,7 +67893,7 @@
       <c r="T99"/>
       <c r="U99"/>
       <c r="V99" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="AA99" s="35"/>
@@ -67928,11 +67928,11 @@
     </row>
     <row r="100" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="158" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Exports of Oil Crude</v>
       </c>
       <c r="B100" s="30" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>PEXOCR</v>
       </c>
       <c r="C100" s="159" t="str">
@@ -67943,19 +67943,19 @@
         <v>0</v>
       </c>
       <c r="F100" s="82">
-        <f t="shared" ref="F100:I104" si="47">SUMIF($E$22:$E$34,$C100,F$22:F$34)*$B$96</f>
+        <f t="shared" ref="F100:I104" si="48">SUMIF($E$22:$E$34,$C100,F$22:F$34)*$B$96</f>
         <v>-186.63033214185884</v>
       </c>
       <c r="G100" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-192.54731207547169</v>
       </c>
       <c r="H100" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-176.73424779874216</v>
       </c>
       <c r="I100" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-225.10362088050312</v>
       </c>
       <c r="J100" s="82">
@@ -67976,7 +67976,7 @@
       <c r="T100"/>
       <c r="U100"/>
       <c r="V100" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="AA100" s="35"/>
@@ -68011,11 +68011,11 @@
     </row>
     <row r="101" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="158" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Exports of Oil Diesel</v>
       </c>
       <c r="B101" s="30" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>PEXODS</v>
       </c>
       <c r="C101" s="159" t="str">
@@ -68026,19 +68026,19 @@
         <v>0</v>
       </c>
       <c r="F101" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-224.73569710604542</v>
       </c>
       <c r="G101" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-232.42136734265776</v>
       </c>
       <c r="H101" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-213.19869703959895</v>
       </c>
       <c r="I101" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-271.99745326071996</v>
       </c>
       <c r="J101" s="82">
@@ -68059,7 +68059,7 @@
       <c r="T101"/>
       <c r="U101"/>
       <c r="V101" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="AA101" s="35"/>
@@ -68094,11 +68094,11 @@
     </row>
     <row r="102" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="158" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Exports of Oil Gasoline</v>
       </c>
       <c r="B102" s="30" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>PEXOGS</v>
       </c>
       <c r="C102" s="159" t="str">
@@ -68109,19 +68109,19 @@
         <v>0</v>
       </c>
       <c r="F102" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-234.68235452233611</v>
       </c>
       <c r="G102" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-240.41292454051242</v>
       </c>
       <c r="H102" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-221.08040737879773</v>
       </c>
       <c r="I102" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-280.21516575580733</v>
       </c>
       <c r="J102" s="82">
@@ -68142,7 +68142,7 @@
       <c r="T102"/>
       <c r="U102"/>
       <c r="V102" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="AA102" s="35"/>
@@ -68177,11 +68177,11 @@
     </row>
     <row r="103" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="158" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Exports of Oil HFO</v>
       </c>
       <c r="B103" s="30" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>PEXOHF</v>
       </c>
       <c r="C103" s="159" t="str">
@@ -68192,19 +68192,19 @@
         <v>0</v>
       </c>
       <c r="F103" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-186.63033214185884</v>
       </c>
       <c r="G103" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-192.54731207547169</v>
       </c>
       <c r="H103" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-176.73424779874216</v>
       </c>
       <c r="I103" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-225.10362088050312</v>
       </c>
       <c r="J103" s="82">
@@ -68222,7 +68222,7 @@
       <c r="T103"/>
       <c r="U103"/>
       <c r="V103" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="AA103" s="35"/>
@@ -68257,11 +68257,11 @@
     </row>
     <row r="104" spans="1:56" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="158" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>Exports of Oil Kerosene</v>
       </c>
       <c r="B104" s="30" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>PEXOKE</v>
       </c>
       <c r="C104" s="159" t="str">
@@ -68272,19 +68272,19 @@
         <v>0</v>
       </c>
       <c r="F104" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-231.28210231970894</v>
       </c>
       <c r="G104" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-238.22903293977191</v>
       </c>
       <c r="H104" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-219.66343669750759</v>
       </c>
       <c r="I104" s="82">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-276.45231932090428</v>
       </c>
       <c r="J104" s="82">
@@ -68305,7 +68305,7 @@
       <c r="T104"/>
       <c r="U104"/>
       <c r="V104" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v/>
       </c>
       <c r="AA104" s="35"/>

</xml_diff>

<commit_message>
Added Cement combustion emissions to COM AGG
It was left out. Have added.
</commit_message>
<xml_diff>
--- a/VT_REGION1_SUP.xlsx
+++ b/VT_REGION1_SUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E255922-BBF7-4710-9F86-FF9047F61E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AA9C97-D98F-4DE8-814B-BCFB8C729ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" firstSheet="3" activeTab="10" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -1640,7 +1640,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2669" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2670" uniqueCount="1110">
   <si>
     <t>Agriculture</t>
   </si>
@@ -5126,6 +5126,9 @@
   </si>
   <si>
     <t>Waste for material use</t>
+  </si>
+  <si>
+    <t>CO2SCCEM</t>
   </si>
 </sst>
 </file>
@@ -7431,57 +7434,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="42" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7519,6 +7471,57 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -24999,25 +25002,25 @@
       <c r="W6" s="175" t="s">
         <v>361</v>
       </c>
-      <c r="AC6" s="438" t="s">
+      <c r="AC6" s="421" t="s">
         <v>362</v>
       </c>
-      <c r="AD6" s="438"/>
-      <c r="AE6" s="438"/>
+      <c r="AD6" s="421"/>
+      <c r="AE6" s="421"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="439" t="s">
+      <c r="A7" s="422" t="s">
         <v>363</v>
       </c>
-      <c r="B7" s="441" t="s">
+      <c r="B7" s="424" t="s">
         <v>364</v>
       </c>
-      <c r="C7" s="443" t="s">
+      <c r="C7" s="426" t="s">
         <v>365</v>
       </c>
-      <c r="D7" s="444"/>
-      <c r="E7" s="445"/>
-      <c r="F7" s="448" t="s">
+      <c r="D7" s="427"/>
+      <c r="E7" s="428"/>
+      <c r="F7" s="431" t="s">
         <v>366</v>
       </c>
       <c r="G7" s="176"/>
@@ -25045,12 +25048,12 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="440"/>
-      <c r="B8" s="442"/>
-      <c r="C8" s="446"/>
-      <c r="D8" s="447"/>
-      <c r="E8" s="447"/>
-      <c r="F8" s="449"/>
+      <c r="A8" s="423"/>
+      <c r="B8" s="425"/>
+      <c r="C8" s="429"/>
+      <c r="D8" s="430"/>
+      <c r="E8" s="430"/>
+      <c r="F8" s="432"/>
       <c r="G8" s="176"/>
       <c r="H8" s="176"/>
       <c r="I8" s="176"/>
@@ -25916,11 +25919,11 @@
       <c r="I25" s="57"/>
       <c r="J25" s="57"/>
       <c r="V25" s="217"/>
-      <c r="AC25" s="437" t="s">
+      <c r="AC25" s="420" t="s">
         <v>432</v>
       </c>
-      <c r="AD25" s="437"/>
-      <c r="AE25" s="437"/>
+      <c r="AD25" s="420"/>
+      <c r="AE25" s="420"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C26" s="57"/>
@@ -25999,8 +26002,8 @@
       <c r="D30" s="57"/>
     </row>
     <row r="31" spans="1:31" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H31" s="433"/>
-      <c r="I31" s="433"/>
+      <c r="H31" s="440"/>
+      <c r="I31" s="440"/>
       <c r="R31" t="s">
         <v>370</v>
       </c>
@@ -26021,10 +26024,10 @@
       </c>
     </row>
     <row r="32" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L32" s="425" t="s">
+      <c r="L32" s="433" t="s">
         <v>436</v>
       </c>
-      <c r="M32" s="434" t="s">
+      <c r="M32" s="441" t="s">
         <v>437</v>
       </c>
       <c r="N32" s="220" t="s">
@@ -26039,22 +26042,22 @@
       <c r="Q32" s="223" t="s">
         <v>439</v>
       </c>
-      <c r="R32" s="425" t="s">
+      <c r="R32" s="433" t="s">
         <v>389</v>
       </c>
-      <c r="S32" s="425" t="s">
+      <c r="S32" s="433" t="s">
         <v>393</v>
       </c>
-      <c r="T32" s="425" t="s">
+      <c r="T32" s="433" t="s">
         <v>440</v>
       </c>
-      <c r="U32" s="425" t="s">
+      <c r="U32" s="433" t="s">
         <v>389</v>
       </c>
-      <c r="V32" s="425" t="s">
+      <c r="V32" s="433" t="s">
         <v>393</v>
       </c>
-      <c r="W32" s="425" t="s">
+      <c r="W32" s="433" t="s">
         <v>440</v>
       </c>
     </row>
@@ -26077,28 +26080,28 @@
       <c r="G33" s="142" t="s">
         <v>444</v>
       </c>
-      <c r="H33" s="432" t="s">
+      <c r="H33" s="436" t="s">
         <v>445</v>
       </c>
-      <c r="I33" s="432"/>
+      <c r="I33" s="436"/>
       <c r="J33" s="142" t="s">
         <v>443</v>
       </c>
       <c r="K33" t="s">
         <v>444</v>
       </c>
-      <c r="L33" s="426"/>
-      <c r="M33" s="435"/>
+      <c r="L33" s="434"/>
+      <c r="M33" s="442"/>
       <c r="N33" s="16"/>
       <c r="O33" s="73"/>
       <c r="P33" s="73"/>
       <c r="Q33" s="224"/>
-      <c r="R33" s="426"/>
-      <c r="S33" s="426"/>
-      <c r="T33" s="426"/>
-      <c r="U33" s="426"/>
-      <c r="V33" s="426"/>
-      <c r="W33" s="426"/>
+      <c r="R33" s="434"/>
+      <c r="S33" s="434"/>
+      <c r="T33" s="434"/>
+      <c r="U33" s="434"/>
+      <c r="V33" s="434"/>
+      <c r="W33" s="434"/>
     </row>
     <row r="34" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -26118,8 +26121,8 @@
       <c r="K34" t="s">
         <v>447</v>
       </c>
-      <c r="L34" s="427"/>
-      <c r="M34" s="436"/>
+      <c r="L34" s="435"/>
+      <c r="M34" s="443"/>
       <c r="N34" s="225" t="s">
         <v>449</v>
       </c>
@@ -26132,12 +26135,12 @@
       <c r="Q34" s="227" t="s">
         <v>449</v>
       </c>
-      <c r="R34" s="427"/>
-      <c r="S34" s="427"/>
-      <c r="T34" s="427"/>
-      <c r="U34" s="427"/>
-      <c r="V34" s="427"/>
-      <c r="W34" s="427"/>
+      <c r="R34" s="435"/>
+      <c r="S34" s="435"/>
+      <c r="T34" s="435"/>
+      <c r="U34" s="435"/>
+      <c r="V34" s="435"/>
+      <c r="W34" s="435"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="228" t="s">
@@ -26203,7 +26206,7 @@
         <v>2.9</v>
       </c>
       <c r="I36" s="237"/>
-      <c r="L36" s="428" t="str">
+      <c r="L36" s="437" t="str">
         <f>A36</f>
         <v>Well completion</v>
       </c>
@@ -26283,7 +26286,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="I37" s="237"/>
-      <c r="L37" s="429"/>
+      <c r="L37" s="438"/>
       <c r="M37" t="str">
         <f t="shared" ref="M37:M45" si="5">B37</f>
         <v>Jiang et al. (2011)</v>
@@ -26354,7 +26357,7 @@
         <v>7.8</v>
       </c>
       <c r="I38" s="237"/>
-      <c r="L38" s="429"/>
+      <c r="L38" s="438"/>
       <c r="M38" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26429,7 +26432,7 @@
       </c>
       <c r="I39" s="237"/>
       <c r="K39" s="237"/>
-      <c r="L39" s="429"/>
+      <c r="L39" s="438"/>
       <c r="M39" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26500,7 +26503,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="I40" s="237"/>
-      <c r="L40" s="429"/>
+      <c r="L40" s="438"/>
       <c r="M40" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26574,7 +26577,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="I41" s="237"/>
-      <c r="L41" s="430"/>
+      <c r="L41" s="439"/>
       <c r="M41" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Broderick et al. (2011)</v>
@@ -26648,7 +26651,7 @@
         <v>4.2</v>
       </c>
       <c r="I42" s="237"/>
-      <c r="L42" s="428" t="s">
+      <c r="L42" s="437" t="s">
         <v>413</v>
       </c>
       <c r="M42" s="222" t="str">
@@ -26721,7 +26724,7 @@
         <v>3.5</v>
       </c>
       <c r="I43" s="237"/>
-      <c r="L43" s="429"/>
+      <c r="L43" s="438"/>
       <c r="M43" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26797,7 +26800,7 @@
       </c>
       <c r="I44" s="237"/>
       <c r="K44" s="237"/>
-      <c r="L44" s="429"/>
+      <c r="L44" s="438"/>
       <c r="M44" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26869,7 +26872,7 @@
         <v>8.9</v>
       </c>
       <c r="I45" s="237"/>
-      <c r="L45" s="430"/>
+      <c r="L45" s="439"/>
       <c r="M45" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26938,7 +26941,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="237"/>
-      <c r="L46" s="428" t="str">
+      <c r="L46" s="437" t="str">
         <f>A47</f>
         <v>Transport, storage and distribution</v>
       </c>
@@ -27014,7 +27017,7 @@
         <v>1.9</v>
       </c>
       <c r="I47" s="237"/>
-      <c r="L47" s="429"/>
+      <c r="L47" s="438"/>
       <c r="M47" t="str">
         <f>B48</f>
         <v>Skone et al. (2011)</v>
@@ -27085,7 +27088,7 @@
         <v>2.7</v>
       </c>
       <c r="I48" s="237"/>
-      <c r="L48" s="430"/>
+      <c r="L48" s="439"/>
       <c r="M48" s="95" t="str">
         <f>B49</f>
         <v>Howarth et al. (2011)</v>
@@ -27454,10 +27457,10 @@
       <c r="C79" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="D79" s="431" t="s">
+      <c r="D79" s="449" t="s">
         <v>498</v>
       </c>
-      <c r="E79" s="431"/>
+      <c r="E79" s="449"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
@@ -27559,13 +27562,13 @@
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="420" t="s">
+      <c r="A103" s="444" t="s">
         <v>508</v>
       </c>
       <c r="B103" s="266" t="s">
         <v>509</v>
       </c>
-      <c r="C103" s="422" t="s">
+      <c r="C103" s="446" t="s">
         <v>510</v>
       </c>
       <c r="D103" s="266">
@@ -27576,11 +27579,11 @@
       </c>
     </row>
     <row r="104" spans="1:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="421"/>
+      <c r="A104" s="445"/>
       <c r="B104" s="266" t="s">
         <v>511</v>
       </c>
-      <c r="C104" s="423"/>
+      <c r="C104" s="447"/>
       <c r="D104" s="266">
         <v>0.18</v>
       </c>
@@ -27593,13 +27596,13 @@
       </c>
     </row>
     <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="420" t="s">
+      <c r="A105" s="444" t="s">
         <v>512</v>
       </c>
       <c r="B105" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C105" s="423"/>
+      <c r="C105" s="447"/>
       <c r="D105" s="266">
         <v>0</v>
       </c>
@@ -27608,11 +27611,11 @@
       </c>
     </row>
     <row r="106" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="421"/>
+      <c r="A106" s="445"/>
       <c r="B106" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C106" s="424"/>
+      <c r="C106" s="448"/>
       <c r="D106" s="266">
         <v>0</v>
       </c>
@@ -27621,13 +27624,13 @@
       </c>
     </row>
     <row r="107" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="420" t="s">
+      <c r="A107" s="444" t="s">
         <v>508</v>
       </c>
       <c r="B107" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C107" s="422" t="s">
+      <c r="C107" s="446" t="s">
         <v>515</v>
       </c>
       <c r="D107" s="266">
@@ -27638,11 +27641,11 @@
       </c>
     </row>
     <row r="108" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="421"/>
+      <c r="A108" s="445"/>
       <c r="B108" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C108" s="423"/>
+      <c r="C108" s="447"/>
       <c r="D108" s="266">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -27651,13 +27654,13 @@
       </c>
     </row>
     <row r="109" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="420" t="s">
+      <c r="A109" s="444" t="s">
         <v>512</v>
       </c>
       <c r="B109" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C109" s="423"/>
+      <c r="C109" s="447"/>
       <c r="D109" s="266">
         <v>0</v>
       </c>
@@ -27666,11 +27669,11 @@
       </c>
     </row>
     <row r="110" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="421"/>
+      <c r="A110" s="445"/>
       <c r="B110" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C110" s="424"/>
+      <c r="C110" s="448"/>
       <c r="D110" s="266">
         <v>0</v>
       </c>
@@ -29133,12 +29136,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AC25:AE25"/>
-    <mergeCell ref="AC6:AE6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="C107:C110"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="U32:U34"/>
+    <mergeCell ref="V32:V34"/>
+    <mergeCell ref="L46:L48"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="C103:C106"/>
+    <mergeCell ref="A105:A106"/>
     <mergeCell ref="W32:W34"/>
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="L36:L41"/>
@@ -29149,16 +29156,12 @@
     <mergeCell ref="R32:R34"/>
     <mergeCell ref="S32:S34"/>
     <mergeCell ref="T32:T34"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="C107:C110"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="U32:U34"/>
-    <mergeCell ref="V32:V34"/>
-    <mergeCell ref="L46:L48"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="C103:C106"/>
-    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="AC25:AE25"/>
+    <mergeCell ref="AC6:AE6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29174,8 +29177,8 @@
   </sheetPr>
   <dimension ref="A1:BB96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29289,6 +29292,9 @@
       <c r="H10" t="s">
         <v>586</v>
       </c>
+      <c r="I10" t="s">
+        <v>1109</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -29310,6 +29316,9 @@
         <v>1</v>
       </c>
       <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
         <v>1</v>
       </c>
     </row>
@@ -49985,18 +49994,18 @@
         <f>FORECAST(CR93,CP94:CQ94,CP93:CQ93)</f>
         <v>93</v>
       </c>
-      <c r="DL94" s="432" t="s">
+      <c r="DL94" s="436" t="s">
         <v>762</v>
       </c>
-      <c r="DM94" s="432"/>
-      <c r="DN94" s="432" t="s">
+      <c r="DM94" s="436"/>
+      <c r="DN94" s="436" t="s">
         <v>763</v>
       </c>
-      <c r="DO94" s="432"/>
-      <c r="DP94" s="432" t="s">
+      <c r="DO94" s="436"/>
+      <c r="DP94" s="436" t="s">
         <v>761</v>
       </c>
-      <c r="DQ94" s="432"/>
+      <c r="DQ94" s="436"/>
     </row>
     <row r="95" spans="1:121" x14ac:dyDescent="0.25">
       <c r="BK95" t="s">
@@ -55457,7 +55466,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="18">
         <f ca="1">NOW()</f>
-        <v>45211.606016666665</v>
+        <v>45215.654102546294</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -56281,7 +56290,7 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
         <f ca="1">NOW()</f>
-        <v>45211.606016666665</v>
+        <v>45215.654102546294</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -60417,7 +60426,7 @@
   </sheetPr>
   <dimension ref="A1:BF149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <pane xSplit="5" ySplit="10" topLeftCell="F63" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A49" sqref="A49"/>
       <selection pane="topRight" activeCell="F49" sqref="F49"/>

</xml_diff>

<commit_message>
Biomass limit causing troubles for ferrochrome
Was reaching the limits on biomass and instead of going with furnaces using more coal/coke and less biomass and adding CCS, it would rather use backstop at R200k/tonne of ferrochrome
</commit_message>
<xml_diff>
--- a/VT_REGION1_SUP.xlsx
+++ b/VT_REGION1_SUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AA9C97-D98F-4DE8-814B-BCFB8C729ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEE6BA1-86DB-4F44-A75A-3982ED671E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" firstSheet="3" activeTab="10" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
+    <workbookView xWindow="2835" yWindow="3420" windowWidth="28800" windowHeight="14985" firstSheet="3" activeTab="6" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -7434,6 +7434,57 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7471,57 +7522,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -25002,25 +25002,25 @@
       <c r="W6" s="175" t="s">
         <v>361</v>
       </c>
-      <c r="AC6" s="421" t="s">
+      <c r="AC6" s="438" t="s">
         <v>362</v>
       </c>
-      <c r="AD6" s="421"/>
-      <c r="AE6" s="421"/>
+      <c r="AD6" s="438"/>
+      <c r="AE6" s="438"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="422" t="s">
+      <c r="A7" s="439" t="s">
         <v>363</v>
       </c>
-      <c r="B7" s="424" t="s">
+      <c r="B7" s="441" t="s">
         <v>364</v>
       </c>
-      <c r="C7" s="426" t="s">
+      <c r="C7" s="443" t="s">
         <v>365</v>
       </c>
-      <c r="D7" s="427"/>
-      <c r="E7" s="428"/>
-      <c r="F7" s="431" t="s">
+      <c r="D7" s="444"/>
+      <c r="E7" s="445"/>
+      <c r="F7" s="448" t="s">
         <v>366</v>
       </c>
       <c r="G7" s="176"/>
@@ -25048,12 +25048,12 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="423"/>
-      <c r="B8" s="425"/>
-      <c r="C8" s="429"/>
-      <c r="D8" s="430"/>
-      <c r="E8" s="430"/>
-      <c r="F8" s="432"/>
+      <c r="A8" s="440"/>
+      <c r="B8" s="442"/>
+      <c r="C8" s="446"/>
+      <c r="D8" s="447"/>
+      <c r="E8" s="447"/>
+      <c r="F8" s="449"/>
       <c r="G8" s="176"/>
       <c r="H8" s="176"/>
       <c r="I8" s="176"/>
@@ -25919,11 +25919,11 @@
       <c r="I25" s="57"/>
       <c r="J25" s="57"/>
       <c r="V25" s="217"/>
-      <c r="AC25" s="420" t="s">
+      <c r="AC25" s="437" t="s">
         <v>432</v>
       </c>
-      <c r="AD25" s="420"/>
-      <c r="AE25" s="420"/>
+      <c r="AD25" s="437"/>
+      <c r="AE25" s="437"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C26" s="57"/>
@@ -26002,8 +26002,8 @@
       <c r="D30" s="57"/>
     </row>
     <row r="31" spans="1:31" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H31" s="440"/>
-      <c r="I31" s="440"/>
+      <c r="H31" s="433"/>
+      <c r="I31" s="433"/>
       <c r="R31" t="s">
         <v>370</v>
       </c>
@@ -26024,10 +26024,10 @@
       </c>
     </row>
     <row r="32" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L32" s="433" t="s">
+      <c r="L32" s="425" t="s">
         <v>436</v>
       </c>
-      <c r="M32" s="441" t="s">
+      <c r="M32" s="434" t="s">
         <v>437</v>
       </c>
       <c r="N32" s="220" t="s">
@@ -26042,22 +26042,22 @@
       <c r="Q32" s="223" t="s">
         <v>439</v>
       </c>
-      <c r="R32" s="433" t="s">
+      <c r="R32" s="425" t="s">
         <v>389</v>
       </c>
-      <c r="S32" s="433" t="s">
+      <c r="S32" s="425" t="s">
         <v>393</v>
       </c>
-      <c r="T32" s="433" t="s">
+      <c r="T32" s="425" t="s">
         <v>440</v>
       </c>
-      <c r="U32" s="433" t="s">
+      <c r="U32" s="425" t="s">
         <v>389</v>
       </c>
-      <c r="V32" s="433" t="s">
+      <c r="V32" s="425" t="s">
         <v>393</v>
       </c>
-      <c r="W32" s="433" t="s">
+      <c r="W32" s="425" t="s">
         <v>440</v>
       </c>
     </row>
@@ -26080,28 +26080,28 @@
       <c r="G33" s="142" t="s">
         <v>444</v>
       </c>
-      <c r="H33" s="436" t="s">
+      <c r="H33" s="432" t="s">
         <v>445</v>
       </c>
-      <c r="I33" s="436"/>
+      <c r="I33" s="432"/>
       <c r="J33" s="142" t="s">
         <v>443</v>
       </c>
       <c r="K33" t="s">
         <v>444</v>
       </c>
-      <c r="L33" s="434"/>
-      <c r="M33" s="442"/>
+      <c r="L33" s="426"/>
+      <c r="M33" s="435"/>
       <c r="N33" s="16"/>
       <c r="O33" s="73"/>
       <c r="P33" s="73"/>
       <c r="Q33" s="224"/>
-      <c r="R33" s="434"/>
-      <c r="S33" s="434"/>
-      <c r="T33" s="434"/>
-      <c r="U33" s="434"/>
-      <c r="V33" s="434"/>
-      <c r="W33" s="434"/>
+      <c r="R33" s="426"/>
+      <c r="S33" s="426"/>
+      <c r="T33" s="426"/>
+      <c r="U33" s="426"/>
+      <c r="V33" s="426"/>
+      <c r="W33" s="426"/>
     </row>
     <row r="34" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -26121,8 +26121,8 @@
       <c r="K34" t="s">
         <v>447</v>
       </c>
-      <c r="L34" s="435"/>
-      <c r="M34" s="443"/>
+      <c r="L34" s="427"/>
+      <c r="M34" s="436"/>
       <c r="N34" s="225" t="s">
         <v>449</v>
       </c>
@@ -26135,12 +26135,12 @@
       <c r="Q34" s="227" t="s">
         <v>449</v>
       </c>
-      <c r="R34" s="435"/>
-      <c r="S34" s="435"/>
-      <c r="T34" s="435"/>
-      <c r="U34" s="435"/>
-      <c r="V34" s="435"/>
-      <c r="W34" s="435"/>
+      <c r="R34" s="427"/>
+      <c r="S34" s="427"/>
+      <c r="T34" s="427"/>
+      <c r="U34" s="427"/>
+      <c r="V34" s="427"/>
+      <c r="W34" s="427"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="228" t="s">
@@ -26206,7 +26206,7 @@
         <v>2.9</v>
       </c>
       <c r="I36" s="237"/>
-      <c r="L36" s="437" t="str">
+      <c r="L36" s="428" t="str">
         <f>A36</f>
         <v>Well completion</v>
       </c>
@@ -26286,7 +26286,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="I37" s="237"/>
-      <c r="L37" s="438"/>
+      <c r="L37" s="429"/>
       <c r="M37" t="str">
         <f t="shared" ref="M37:M45" si="5">B37</f>
         <v>Jiang et al. (2011)</v>
@@ -26357,7 +26357,7 @@
         <v>7.8</v>
       </c>
       <c r="I38" s="237"/>
-      <c r="L38" s="438"/>
+      <c r="L38" s="429"/>
       <c r="M38" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26432,7 +26432,7 @@
       </c>
       <c r="I39" s="237"/>
       <c r="K39" s="237"/>
-      <c r="L39" s="438"/>
+      <c r="L39" s="429"/>
       <c r="M39" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26503,7 +26503,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="I40" s="237"/>
-      <c r="L40" s="438"/>
+      <c r="L40" s="429"/>
       <c r="M40" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26577,7 +26577,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="I41" s="237"/>
-      <c r="L41" s="439"/>
+      <c r="L41" s="430"/>
       <c r="M41" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Broderick et al. (2011)</v>
@@ -26651,7 +26651,7 @@
         <v>4.2</v>
       </c>
       <c r="I42" s="237"/>
-      <c r="L42" s="437" t="s">
+      <c r="L42" s="428" t="s">
         <v>413</v>
       </c>
       <c r="M42" s="222" t="str">
@@ -26724,7 +26724,7 @@
         <v>3.5</v>
       </c>
       <c r="I43" s="237"/>
-      <c r="L43" s="438"/>
+      <c r="L43" s="429"/>
       <c r="M43" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26800,7 +26800,7 @@
       </c>
       <c r="I44" s="237"/>
       <c r="K44" s="237"/>
-      <c r="L44" s="438"/>
+      <c r="L44" s="429"/>
       <c r="M44" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26872,7 +26872,7 @@
         <v>8.9</v>
       </c>
       <c r="I45" s="237"/>
-      <c r="L45" s="439"/>
+      <c r="L45" s="430"/>
       <c r="M45" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26941,7 +26941,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="237"/>
-      <c r="L46" s="437" t="str">
+      <c r="L46" s="428" t="str">
         <f>A47</f>
         <v>Transport, storage and distribution</v>
       </c>
@@ -27017,7 +27017,7 @@
         <v>1.9</v>
       </c>
       <c r="I47" s="237"/>
-      <c r="L47" s="438"/>
+      <c r="L47" s="429"/>
       <c r="M47" t="str">
         <f>B48</f>
         <v>Skone et al. (2011)</v>
@@ -27088,7 +27088,7 @@
         <v>2.7</v>
       </c>
       <c r="I48" s="237"/>
-      <c r="L48" s="439"/>
+      <c r="L48" s="430"/>
       <c r="M48" s="95" t="str">
         <f>B49</f>
         <v>Howarth et al. (2011)</v>
@@ -27457,10 +27457,10 @@
       <c r="C79" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="D79" s="449" t="s">
+      <c r="D79" s="431" t="s">
         <v>498</v>
       </c>
-      <c r="E79" s="449"/>
+      <c r="E79" s="431"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
@@ -27562,13 +27562,13 @@
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="444" t="s">
+      <c r="A103" s="420" t="s">
         <v>508</v>
       </c>
       <c r="B103" s="266" t="s">
         <v>509</v>
       </c>
-      <c r="C103" s="446" t="s">
+      <c r="C103" s="422" t="s">
         <v>510</v>
       </c>
       <c r="D103" s="266">
@@ -27579,11 +27579,11 @@
       </c>
     </row>
     <row r="104" spans="1:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="445"/>
+      <c r="A104" s="421"/>
       <c r="B104" s="266" t="s">
         <v>511</v>
       </c>
-      <c r="C104" s="447"/>
+      <c r="C104" s="423"/>
       <c r="D104" s="266">
         <v>0.18</v>
       </c>
@@ -27596,13 +27596,13 @@
       </c>
     </row>
     <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="444" t="s">
+      <c r="A105" s="420" t="s">
         <v>512</v>
       </c>
       <c r="B105" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C105" s="447"/>
+      <c r="C105" s="423"/>
       <c r="D105" s="266">
         <v>0</v>
       </c>
@@ -27611,11 +27611,11 @@
       </c>
     </row>
     <row r="106" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="445"/>
+      <c r="A106" s="421"/>
       <c r="B106" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C106" s="448"/>
+      <c r="C106" s="424"/>
       <c r="D106" s="266">
         <v>0</v>
       </c>
@@ -27624,13 +27624,13 @@
       </c>
     </row>
     <row r="107" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="444" t="s">
+      <c r="A107" s="420" t="s">
         <v>508</v>
       </c>
       <c r="B107" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C107" s="446" t="s">
+      <c r="C107" s="422" t="s">
         <v>515</v>
       </c>
       <c r="D107" s="266">
@@ -27641,11 +27641,11 @@
       </c>
     </row>
     <row r="108" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="445"/>
+      <c r="A108" s="421"/>
       <c r="B108" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C108" s="447"/>
+      <c r="C108" s="423"/>
       <c r="D108" s="266">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -27654,13 +27654,13 @@
       </c>
     </row>
     <row r="109" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="444" t="s">
+      <c r="A109" s="420" t="s">
         <v>512</v>
       </c>
       <c r="B109" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C109" s="447"/>
+      <c r="C109" s="423"/>
       <c r="D109" s="266">
         <v>0</v>
       </c>
@@ -27669,11 +27669,11 @@
       </c>
     </row>
     <row r="110" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="445"/>
+      <c r="A110" s="421"/>
       <c r="B110" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C110" s="448"/>
+      <c r="C110" s="424"/>
       <c r="D110" s="266">
         <v>0</v>
       </c>
@@ -29136,6 +29136,22 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="AC25:AE25"/>
+    <mergeCell ref="AC6:AE6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="W32:W34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="L36:L41"/>
+    <mergeCell ref="L42:L45"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="L32:L34"/>
+    <mergeCell ref="M32:M34"/>
+    <mergeCell ref="R32:R34"/>
+    <mergeCell ref="S32:S34"/>
+    <mergeCell ref="T32:T34"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="C107:C110"/>
     <mergeCell ref="A109:A110"/>
@@ -29146,22 +29162,6 @@
     <mergeCell ref="A103:A104"/>
     <mergeCell ref="C103:C106"/>
     <mergeCell ref="A105:A106"/>
-    <mergeCell ref="W32:W34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="L36:L41"/>
-    <mergeCell ref="L42:L45"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="L32:L34"/>
-    <mergeCell ref="M32:M34"/>
-    <mergeCell ref="R32:R34"/>
-    <mergeCell ref="S32:S34"/>
-    <mergeCell ref="T32:T34"/>
-    <mergeCell ref="AC25:AE25"/>
-    <mergeCell ref="AC6:AE6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29177,7 +29177,7 @@
   </sheetPr>
   <dimension ref="A1:BB96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -49994,18 +49994,18 @@
         <f>FORECAST(CR93,CP94:CQ94,CP93:CQ93)</f>
         <v>93</v>
       </c>
-      <c r="DL94" s="436" t="s">
+      <c r="DL94" s="432" t="s">
         <v>762</v>
       </c>
-      <c r="DM94" s="436"/>
-      <c r="DN94" s="436" t="s">
+      <c r="DM94" s="432"/>
+      <c r="DN94" s="432" t="s">
         <v>763</v>
       </c>
-      <c r="DO94" s="436"/>
-      <c r="DP94" s="436" t="s">
+      <c r="DO94" s="432"/>
+      <c r="DP94" s="432" t="s">
         <v>761</v>
       </c>
-      <c r="DQ94" s="436"/>
+      <c r="DQ94" s="432"/>
     </row>
     <row r="95" spans="1:121" x14ac:dyDescent="0.25">
       <c r="BK95" t="s">
@@ -55466,7 +55466,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="18">
         <f ca="1">NOW()</f>
-        <v>45215.654102546294</v>
+        <v>45217.994184490744</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -56290,7 +56290,7 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
         <f ca="1">NOW()</f>
-        <v>45215.654102546294</v>
+        <v>45217.994184490744</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -60426,12 +60426,12 @@
   </sheetPr>
   <dimension ref="A1:BF149"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <pane xSplit="5" ySplit="10" topLeftCell="F63" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A49" sqref="A49"/>
       <selection pane="topRight" activeCell="F49" sqref="F49"/>
       <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
-      <selection pane="bottomRight" activeCell="L73" sqref="L73"/>
+      <selection pane="bottomRight" activeCell="O73" sqref="O73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -65828,8 +65828,8 @@
       <c r="M72"/>
       <c r="N72"/>
       <c r="O72" s="82">
-        <f>K72*1.5</f>
-        <v>265.5</v>
+        <f>K72*2</f>
+        <v>354</v>
       </c>
       <c r="P72" s="82"/>
       <c r="Q72" s="82"/>

</xml_diff>

<commit_message>
Added CCS for Iron and Steel
Added CO2SPIIS to SUP definitions.
</commit_message>
<xml_diff>
--- a/VT_REGION1_SUP.xlsx
+++ b/VT_REGION1_SUP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEE6BA1-86DB-4F44-A75A-3982ED671E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD2AC2C-C94B-49F1-9610-9724F23CCFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="3420" windowWidth="28800" windowHeight="14985" firstSheet="3" activeTab="6" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="3" activeTab="5" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -1640,7 +1640,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2670" uniqueCount="1110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2676" uniqueCount="1112">
   <si>
     <t>Agriculture</t>
   </si>
@@ -5129,6 +5129,12 @@
   </si>
   <si>
     <t>CO2SCCEM</t>
+  </si>
+  <si>
+    <t>CO2SPIIS</t>
+  </si>
+  <si>
+    <t>Process Emissions Iron and Steel South Africa</t>
   </si>
 </sst>
 </file>
@@ -7434,57 +7440,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="42" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7522,6 +7477,57 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -25002,25 +25008,25 @@
       <c r="W6" s="175" t="s">
         <v>361</v>
       </c>
-      <c r="AC6" s="438" t="s">
+      <c r="AC6" s="421" t="s">
         <v>362</v>
       </c>
-      <c r="AD6" s="438"/>
-      <c r="AE6" s="438"/>
+      <c r="AD6" s="421"/>
+      <c r="AE6" s="421"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="439" t="s">
+      <c r="A7" s="422" t="s">
         <v>363</v>
       </c>
-      <c r="B7" s="441" t="s">
+      <c r="B7" s="424" t="s">
         <v>364</v>
       </c>
-      <c r="C7" s="443" t="s">
+      <c r="C7" s="426" t="s">
         <v>365</v>
       </c>
-      <c r="D7" s="444"/>
-      <c r="E7" s="445"/>
-      <c r="F7" s="448" t="s">
+      <c r="D7" s="427"/>
+      <c r="E7" s="428"/>
+      <c r="F7" s="431" t="s">
         <v>366</v>
       </c>
       <c r="G7" s="176"/>
@@ -25048,12 +25054,12 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="440"/>
-      <c r="B8" s="442"/>
-      <c r="C8" s="446"/>
-      <c r="D8" s="447"/>
-      <c r="E8" s="447"/>
-      <c r="F8" s="449"/>
+      <c r="A8" s="423"/>
+      <c r="B8" s="425"/>
+      <c r="C8" s="429"/>
+      <c r="D8" s="430"/>
+      <c r="E8" s="430"/>
+      <c r="F8" s="432"/>
       <c r="G8" s="176"/>
       <c r="H8" s="176"/>
       <c r="I8" s="176"/>
@@ -25919,11 +25925,11 @@
       <c r="I25" s="57"/>
       <c r="J25" s="57"/>
       <c r="V25" s="217"/>
-      <c r="AC25" s="437" t="s">
+      <c r="AC25" s="420" t="s">
         <v>432</v>
       </c>
-      <c r="AD25" s="437"/>
-      <c r="AE25" s="437"/>
+      <c r="AD25" s="420"/>
+      <c r="AE25" s="420"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C26" s="57"/>
@@ -26002,8 +26008,8 @@
       <c r="D30" s="57"/>
     </row>
     <row r="31" spans="1:31" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H31" s="433"/>
-      <c r="I31" s="433"/>
+      <c r="H31" s="440"/>
+      <c r="I31" s="440"/>
       <c r="R31" t="s">
         <v>370</v>
       </c>
@@ -26024,10 +26030,10 @@
       </c>
     </row>
     <row r="32" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L32" s="425" t="s">
+      <c r="L32" s="433" t="s">
         <v>436</v>
       </c>
-      <c r="M32" s="434" t="s">
+      <c r="M32" s="441" t="s">
         <v>437</v>
       </c>
       <c r="N32" s="220" t="s">
@@ -26042,22 +26048,22 @@
       <c r="Q32" s="223" t="s">
         <v>439</v>
       </c>
-      <c r="R32" s="425" t="s">
+      <c r="R32" s="433" t="s">
         <v>389</v>
       </c>
-      <c r="S32" s="425" t="s">
+      <c r="S32" s="433" t="s">
         <v>393</v>
       </c>
-      <c r="T32" s="425" t="s">
+      <c r="T32" s="433" t="s">
         <v>440</v>
       </c>
-      <c r="U32" s="425" t="s">
+      <c r="U32" s="433" t="s">
         <v>389</v>
       </c>
-      <c r="V32" s="425" t="s">
+      <c r="V32" s="433" t="s">
         <v>393</v>
       </c>
-      <c r="W32" s="425" t="s">
+      <c r="W32" s="433" t="s">
         <v>440</v>
       </c>
     </row>
@@ -26080,28 +26086,28 @@
       <c r="G33" s="142" t="s">
         <v>444</v>
       </c>
-      <c r="H33" s="432" t="s">
+      <c r="H33" s="436" t="s">
         <v>445</v>
       </c>
-      <c r="I33" s="432"/>
+      <c r="I33" s="436"/>
       <c r="J33" s="142" t="s">
         <v>443</v>
       </c>
       <c r="K33" t="s">
         <v>444</v>
       </c>
-      <c r="L33" s="426"/>
-      <c r="M33" s="435"/>
+      <c r="L33" s="434"/>
+      <c r="M33" s="442"/>
       <c r="N33" s="16"/>
       <c r="O33" s="73"/>
       <c r="P33" s="73"/>
       <c r="Q33" s="224"/>
-      <c r="R33" s="426"/>
-      <c r="S33" s="426"/>
-      <c r="T33" s="426"/>
-      <c r="U33" s="426"/>
-      <c r="V33" s="426"/>
-      <c r="W33" s="426"/>
+      <c r="R33" s="434"/>
+      <c r="S33" s="434"/>
+      <c r="T33" s="434"/>
+      <c r="U33" s="434"/>
+      <c r="V33" s="434"/>
+      <c r="W33" s="434"/>
     </row>
     <row r="34" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -26121,8 +26127,8 @@
       <c r="K34" t="s">
         <v>447</v>
       </c>
-      <c r="L34" s="427"/>
-      <c r="M34" s="436"/>
+      <c r="L34" s="435"/>
+      <c r="M34" s="443"/>
       <c r="N34" s="225" t="s">
         <v>449</v>
       </c>
@@ -26135,12 +26141,12 @@
       <c r="Q34" s="227" t="s">
         <v>449</v>
       </c>
-      <c r="R34" s="427"/>
-      <c r="S34" s="427"/>
-      <c r="T34" s="427"/>
-      <c r="U34" s="427"/>
-      <c r="V34" s="427"/>
-      <c r="W34" s="427"/>
+      <c r="R34" s="435"/>
+      <c r="S34" s="435"/>
+      <c r="T34" s="435"/>
+      <c r="U34" s="435"/>
+      <c r="V34" s="435"/>
+      <c r="W34" s="435"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="228" t="s">
@@ -26206,7 +26212,7 @@
         <v>2.9</v>
       </c>
       <c r="I36" s="237"/>
-      <c r="L36" s="428" t="str">
+      <c r="L36" s="437" t="str">
         <f>A36</f>
         <v>Well completion</v>
       </c>
@@ -26286,7 +26292,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="I37" s="237"/>
-      <c r="L37" s="429"/>
+      <c r="L37" s="438"/>
       <c r="M37" t="str">
         <f t="shared" ref="M37:M45" si="5">B37</f>
         <v>Jiang et al. (2011)</v>
@@ -26357,7 +26363,7 @@
         <v>7.8</v>
       </c>
       <c r="I38" s="237"/>
-      <c r="L38" s="429"/>
+      <c r="L38" s="438"/>
       <c r="M38" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26432,7 +26438,7 @@
       </c>
       <c r="I39" s="237"/>
       <c r="K39" s="237"/>
-      <c r="L39" s="429"/>
+      <c r="L39" s="438"/>
       <c r="M39" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26503,7 +26509,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="I40" s="237"/>
-      <c r="L40" s="429"/>
+      <c r="L40" s="438"/>
       <c r="M40" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26577,7 +26583,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="I41" s="237"/>
-      <c r="L41" s="430"/>
+      <c r="L41" s="439"/>
       <c r="M41" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Broderick et al. (2011)</v>
@@ -26651,7 +26657,7 @@
         <v>4.2</v>
       </c>
       <c r="I42" s="237"/>
-      <c r="L42" s="428" t="s">
+      <c r="L42" s="437" t="s">
         <v>413</v>
       </c>
       <c r="M42" s="222" t="str">
@@ -26724,7 +26730,7 @@
         <v>3.5</v>
       </c>
       <c r="I43" s="237"/>
-      <c r="L43" s="429"/>
+      <c r="L43" s="438"/>
       <c r="M43" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26800,7 +26806,7 @@
       </c>
       <c r="I44" s="237"/>
       <c r="K44" s="237"/>
-      <c r="L44" s="429"/>
+      <c r="L44" s="438"/>
       <c r="M44" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26872,7 +26878,7 @@
         <v>8.9</v>
       </c>
       <c r="I45" s="237"/>
-      <c r="L45" s="430"/>
+      <c r="L45" s="439"/>
       <c r="M45" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26941,7 +26947,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="237"/>
-      <c r="L46" s="428" t="str">
+      <c r="L46" s="437" t="str">
         <f>A47</f>
         <v>Transport, storage and distribution</v>
       </c>
@@ -27017,7 +27023,7 @@
         <v>1.9</v>
       </c>
       <c r="I47" s="237"/>
-      <c r="L47" s="429"/>
+      <c r="L47" s="438"/>
       <c r="M47" t="str">
         <f>B48</f>
         <v>Skone et al. (2011)</v>
@@ -27088,7 +27094,7 @@
         <v>2.7</v>
       </c>
       <c r="I48" s="237"/>
-      <c r="L48" s="430"/>
+      <c r="L48" s="439"/>
       <c r="M48" s="95" t="str">
         <f>B49</f>
         <v>Howarth et al. (2011)</v>
@@ -27457,10 +27463,10 @@
       <c r="C79" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="D79" s="431" t="s">
+      <c r="D79" s="449" t="s">
         <v>498</v>
       </c>
-      <c r="E79" s="431"/>
+      <c r="E79" s="449"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
@@ -27562,13 +27568,13 @@
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="420" t="s">
+      <c r="A103" s="444" t="s">
         <v>508</v>
       </c>
       <c r="B103" s="266" t="s">
         <v>509</v>
       </c>
-      <c r="C103" s="422" t="s">
+      <c r="C103" s="446" t="s">
         <v>510</v>
       </c>
       <c r="D103" s="266">
@@ -27579,11 +27585,11 @@
       </c>
     </row>
     <row r="104" spans="1:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="421"/>
+      <c r="A104" s="445"/>
       <c r="B104" s="266" t="s">
         <v>511</v>
       </c>
-      <c r="C104" s="423"/>
+      <c r="C104" s="447"/>
       <c r="D104" s="266">
         <v>0.18</v>
       </c>
@@ -27596,13 +27602,13 @@
       </c>
     </row>
     <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="420" t="s">
+      <c r="A105" s="444" t="s">
         <v>512</v>
       </c>
       <c r="B105" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C105" s="423"/>
+      <c r="C105" s="447"/>
       <c r="D105" s="266">
         <v>0</v>
       </c>
@@ -27611,11 +27617,11 @@
       </c>
     </row>
     <row r="106" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="421"/>
+      <c r="A106" s="445"/>
       <c r="B106" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C106" s="424"/>
+      <c r="C106" s="448"/>
       <c r="D106" s="266">
         <v>0</v>
       </c>
@@ -27624,13 +27630,13 @@
       </c>
     </row>
     <row r="107" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="420" t="s">
+      <c r="A107" s="444" t="s">
         <v>508</v>
       </c>
       <c r="B107" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C107" s="422" t="s">
+      <c r="C107" s="446" t="s">
         <v>515</v>
       </c>
       <c r="D107" s="266">
@@ -27641,11 +27647,11 @@
       </c>
     </row>
     <row r="108" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="421"/>
+      <c r="A108" s="445"/>
       <c r="B108" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C108" s="423"/>
+      <c r="C108" s="447"/>
       <c r="D108" s="266">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -27654,13 +27660,13 @@
       </c>
     </row>
     <row r="109" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="420" t="s">
+      <c r="A109" s="444" t="s">
         <v>512</v>
       </c>
       <c r="B109" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C109" s="423"/>
+      <c r="C109" s="447"/>
       <c r="D109" s="266">
         <v>0</v>
       </c>
@@ -27669,11 +27675,11 @@
       </c>
     </row>
     <row r="110" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="421"/>
+      <c r="A110" s="445"/>
       <c r="B110" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C110" s="424"/>
+      <c r="C110" s="448"/>
       <c r="D110" s="266">
         <v>0</v>
       </c>
@@ -29136,12 +29142,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AC25:AE25"/>
-    <mergeCell ref="AC6:AE6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="C107:C110"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="U32:U34"/>
+    <mergeCell ref="V32:V34"/>
+    <mergeCell ref="L46:L48"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="C103:C106"/>
+    <mergeCell ref="A105:A106"/>
     <mergeCell ref="W32:W34"/>
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="L36:L41"/>
@@ -29152,16 +29162,12 @@
     <mergeCell ref="R32:R34"/>
     <mergeCell ref="S32:S34"/>
     <mergeCell ref="T32:T34"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="C107:C110"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="U32:U34"/>
-    <mergeCell ref="V32:V34"/>
-    <mergeCell ref="L46:L48"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="C103:C106"/>
-    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="AC25:AE25"/>
+    <mergeCell ref="AC6:AE6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29178,7 +29184,7 @@
   <dimension ref="A1:BB96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29295,6 +29301,9 @@
       <c r="I10" t="s">
         <v>1109</v>
       </c>
+      <c r="J10" t="s">
+        <v>1110</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -29319,6 +29328,9 @@
         <v>1</v>
       </c>
       <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
         <v>1</v>
       </c>
     </row>
@@ -49994,18 +50006,18 @@
         <f>FORECAST(CR93,CP94:CQ94,CP93:CQ93)</f>
         <v>93</v>
       </c>
-      <c r="DL94" s="432" t="s">
+      <c r="DL94" s="436" t="s">
         <v>762</v>
       </c>
-      <c r="DM94" s="432"/>
-      <c r="DN94" s="432" t="s">
+      <c r="DM94" s="436"/>
+      <c r="DN94" s="436" t="s">
         <v>763</v>
       </c>
-      <c r="DO94" s="432"/>
-      <c r="DP94" s="432" t="s">
+      <c r="DO94" s="436"/>
+      <c r="DP94" s="436" t="s">
         <v>761</v>
       </c>
-      <c r="DQ94" s="432"/>
+      <c r="DQ94" s="436"/>
     </row>
     <row r="95" spans="1:121" x14ac:dyDescent="0.25">
       <c r="BK95" t="s">
@@ -55466,7 +55478,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="18">
         <f ca="1">NOW()</f>
-        <v>45217.994184490744</v>
+        <v>45310.469588194443</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -56290,7 +56302,7 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
         <f ca="1">NOW()</f>
-        <v>45217.994184490744</v>
+        <v>45310.469588194443</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -58975,10 +58987,10 @@
   <sheetPr codeName="Sheet6">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -60412,6 +60424,23 @@
         <v>357</v>
       </c>
     </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B71" s="380" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C71" s="380" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D71" s="381" t="s">
+        <v>980</v>
+      </c>
+      <c r="E71" s="381" t="s">
+        <v>979</v>
+      </c>
+      <c r="F71" s="380" t="s">
+        <v>357</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -60426,7 +60455,7 @@
   </sheetPr>
   <dimension ref="A1:BF149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <pane xSplit="5" ySplit="10" topLeftCell="F63" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A49" sqref="A49"/>
       <selection pane="topRight" activeCell="F49" sqref="F49"/>

</xml_diff>

<commit_message>
Fix on Elc Price calc and also on X-Techs InvCost
</commit_message>
<xml_diff>
--- a/VT_REGION1_SUP.xlsx
+++ b/VT_REGION1_SUP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD2AC2C-C94B-49F1-9610-9724F23CCFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C862BD9-4532-4A78-BE23-89CA12374CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="3" activeTab="5" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
+    <workbookView xWindow="270" yWindow="150" windowWidth="28350" windowHeight="15150" firstSheet="4" activeTab="11" xr2:uid="{E5F8B398-E078-41ED-B259-65DAD54952E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -7440,6 +7440,57 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7477,57 +7528,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -24534,9 +24534,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -24574,7 +24574,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -24680,7 +24680,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -24822,7 +24822,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -25008,25 +25008,25 @@
       <c r="W6" s="175" t="s">
         <v>361</v>
       </c>
-      <c r="AC6" s="421" t="s">
+      <c r="AC6" s="438" t="s">
         <v>362</v>
       </c>
-      <c r="AD6" s="421"/>
-      <c r="AE6" s="421"/>
+      <c r="AD6" s="438"/>
+      <c r="AE6" s="438"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="422" t="s">
+      <c r="A7" s="439" t="s">
         <v>363</v>
       </c>
-      <c r="B7" s="424" t="s">
+      <c r="B7" s="441" t="s">
         <v>364</v>
       </c>
-      <c r="C7" s="426" t="s">
+      <c r="C7" s="443" t="s">
         <v>365</v>
       </c>
-      <c r="D7" s="427"/>
-      <c r="E7" s="428"/>
-      <c r="F7" s="431" t="s">
+      <c r="D7" s="444"/>
+      <c r="E7" s="445"/>
+      <c r="F7" s="448" t="s">
         <v>366</v>
       </c>
       <c r="G7" s="176"/>
@@ -25054,12 +25054,12 @@
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="423"/>
-      <c r="B8" s="425"/>
-      <c r="C8" s="429"/>
-      <c r="D8" s="430"/>
-      <c r="E8" s="430"/>
-      <c r="F8" s="432"/>
+      <c r="A8" s="440"/>
+      <c r="B8" s="442"/>
+      <c r="C8" s="446"/>
+      <c r="D8" s="447"/>
+      <c r="E8" s="447"/>
+      <c r="F8" s="449"/>
       <c r="G8" s="176"/>
       <c r="H8" s="176"/>
       <c r="I8" s="176"/>
@@ -25925,11 +25925,11 @@
       <c r="I25" s="57"/>
       <c r="J25" s="57"/>
       <c r="V25" s="217"/>
-      <c r="AC25" s="420" t="s">
+      <c r="AC25" s="437" t="s">
         <v>432</v>
       </c>
-      <c r="AD25" s="420"/>
-      <c r="AE25" s="420"/>
+      <c r="AD25" s="437"/>
+      <c r="AE25" s="437"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C26" s="57"/>
@@ -26008,8 +26008,8 @@
       <c r="D30" s="57"/>
     </row>
     <row r="31" spans="1:31" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H31" s="440"/>
-      <c r="I31" s="440"/>
+      <c r="H31" s="433"/>
+      <c r="I31" s="433"/>
       <c r="R31" t="s">
         <v>370</v>
       </c>
@@ -26030,10 +26030,10 @@
       </c>
     </row>
     <row r="32" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L32" s="433" t="s">
+      <c r="L32" s="425" t="s">
         <v>436</v>
       </c>
-      <c r="M32" s="441" t="s">
+      <c r="M32" s="434" t="s">
         <v>437</v>
       </c>
       <c r="N32" s="220" t="s">
@@ -26048,22 +26048,22 @@
       <c r="Q32" s="223" t="s">
         <v>439</v>
       </c>
-      <c r="R32" s="433" t="s">
+      <c r="R32" s="425" t="s">
         <v>389</v>
       </c>
-      <c r="S32" s="433" t="s">
+      <c r="S32" s="425" t="s">
         <v>393</v>
       </c>
-      <c r="T32" s="433" t="s">
+      <c r="T32" s="425" t="s">
         <v>440</v>
       </c>
-      <c r="U32" s="433" t="s">
+      <c r="U32" s="425" t="s">
         <v>389</v>
       </c>
-      <c r="V32" s="433" t="s">
+      <c r="V32" s="425" t="s">
         <v>393</v>
       </c>
-      <c r="W32" s="433" t="s">
+      <c r="W32" s="425" t="s">
         <v>440</v>
       </c>
     </row>
@@ -26086,28 +26086,28 @@
       <c r="G33" s="142" t="s">
         <v>444</v>
       </c>
-      <c r="H33" s="436" t="s">
+      <c r="H33" s="432" t="s">
         <v>445</v>
       </c>
-      <c r="I33" s="436"/>
+      <c r="I33" s="432"/>
       <c r="J33" s="142" t="s">
         <v>443</v>
       </c>
       <c r="K33" t="s">
         <v>444</v>
       </c>
-      <c r="L33" s="434"/>
-      <c r="M33" s="442"/>
+      <c r="L33" s="426"/>
+      <c r="M33" s="435"/>
       <c r="N33" s="16"/>
       <c r="O33" s="73"/>
       <c r="P33" s="73"/>
       <c r="Q33" s="224"/>
-      <c r="R33" s="434"/>
-      <c r="S33" s="434"/>
-      <c r="T33" s="434"/>
-      <c r="U33" s="434"/>
-      <c r="V33" s="434"/>
-      <c r="W33" s="434"/>
+      <c r="R33" s="426"/>
+      <c r="S33" s="426"/>
+      <c r="T33" s="426"/>
+      <c r="U33" s="426"/>
+      <c r="V33" s="426"/>
+      <c r="W33" s="426"/>
     </row>
     <row r="34" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -26127,8 +26127,8 @@
       <c r="K34" t="s">
         <v>447</v>
       </c>
-      <c r="L34" s="435"/>
-      <c r="M34" s="443"/>
+      <c r="L34" s="427"/>
+      <c r="M34" s="436"/>
       <c r="N34" s="225" t="s">
         <v>449</v>
       </c>
@@ -26141,12 +26141,12 @@
       <c r="Q34" s="227" t="s">
         <v>449</v>
       </c>
-      <c r="R34" s="435"/>
-      <c r="S34" s="435"/>
-      <c r="T34" s="435"/>
-      <c r="U34" s="435"/>
-      <c r="V34" s="435"/>
-      <c r="W34" s="435"/>
+      <c r="R34" s="427"/>
+      <c r="S34" s="427"/>
+      <c r="T34" s="427"/>
+      <c r="U34" s="427"/>
+      <c r="V34" s="427"/>
+      <c r="W34" s="427"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="228" t="s">
@@ -26212,7 +26212,7 @@
         <v>2.9</v>
       </c>
       <c r="I36" s="237"/>
-      <c r="L36" s="437" t="str">
+      <c r="L36" s="428" t="str">
         <f>A36</f>
         <v>Well completion</v>
       </c>
@@ -26292,7 +26292,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="I37" s="237"/>
-      <c r="L37" s="438"/>
+      <c r="L37" s="429"/>
       <c r="M37" t="str">
         <f t="shared" ref="M37:M45" si="5">B37</f>
         <v>Jiang et al. (2011)</v>
@@ -26363,7 +26363,7 @@
         <v>7.8</v>
       </c>
       <c r="I38" s="237"/>
-      <c r="L38" s="438"/>
+      <c r="L38" s="429"/>
       <c r="M38" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26438,7 +26438,7 @@
       </c>
       <c r="I39" s="237"/>
       <c r="K39" s="237"/>
-      <c r="L39" s="438"/>
+      <c r="L39" s="429"/>
       <c r="M39" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26509,7 +26509,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="I40" s="237"/>
-      <c r="L40" s="438"/>
+      <c r="L40" s="429"/>
       <c r="M40" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26583,7 +26583,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="I41" s="237"/>
-      <c r="L41" s="439"/>
+      <c r="L41" s="430"/>
       <c r="M41" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Broderick et al. (2011)</v>
@@ -26657,7 +26657,7 @@
         <v>4.2</v>
       </c>
       <c r="I42" s="237"/>
-      <c r="L42" s="437" t="s">
+      <c r="L42" s="428" t="s">
         <v>413</v>
       </c>
       <c r="M42" s="222" t="str">
@@ -26730,7 +26730,7 @@
         <v>3.5</v>
       </c>
       <c r="I43" s="237"/>
-      <c r="L43" s="438"/>
+      <c r="L43" s="429"/>
       <c r="M43" t="str">
         <f t="shared" si="5"/>
         <v>Skone et al. (2011)</v>
@@ -26806,7 +26806,7 @@
       </c>
       <c r="I44" s="237"/>
       <c r="K44" s="237"/>
-      <c r="L44" s="438"/>
+      <c r="L44" s="429"/>
       <c r="M44" t="str">
         <f t="shared" si="5"/>
         <v>Howarth et al. (2011)</v>
@@ -26878,7 +26878,7 @@
         <v>8.9</v>
       </c>
       <c r="I45" s="237"/>
-      <c r="L45" s="439"/>
+      <c r="L45" s="430"/>
       <c r="M45" s="95" t="str">
         <f t="shared" si="5"/>
         <v>Lechtenbohmer et al. (2005)</v>
@@ -26947,7 +26947,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="237"/>
-      <c r="L46" s="437" t="str">
+      <c r="L46" s="428" t="str">
         <f>A47</f>
         <v>Transport, storage and distribution</v>
       </c>
@@ -27023,7 +27023,7 @@
         <v>1.9</v>
       </c>
       <c r="I47" s="237"/>
-      <c r="L47" s="438"/>
+      <c r="L47" s="429"/>
       <c r="M47" t="str">
         <f>B48</f>
         <v>Skone et al. (2011)</v>
@@ -27094,7 +27094,7 @@
         <v>2.7</v>
       </c>
       <c r="I48" s="237"/>
-      <c r="L48" s="439"/>
+      <c r="L48" s="430"/>
       <c r="M48" s="95" t="str">
         <f>B49</f>
         <v>Howarth et al. (2011)</v>
@@ -27463,10 +27463,10 @@
       <c r="C79" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="D79" s="449" t="s">
+      <c r="D79" s="431" t="s">
         <v>498</v>
       </c>
-      <c r="E79" s="449"/>
+      <c r="E79" s="431"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
@@ -27568,13 +27568,13 @@
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="444" t="s">
+      <c r="A103" s="420" t="s">
         <v>508</v>
       </c>
       <c r="B103" s="266" t="s">
         <v>509</v>
       </c>
-      <c r="C103" s="446" t="s">
+      <c r="C103" s="422" t="s">
         <v>510</v>
       </c>
       <c r="D103" s="266">
@@ -27585,11 +27585,11 @@
       </c>
     </row>
     <row r="104" spans="1:11" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="445"/>
+      <c r="A104" s="421"/>
       <c r="B104" s="266" t="s">
         <v>511</v>
       </c>
-      <c r="C104" s="447"/>
+      <c r="C104" s="423"/>
       <c r="D104" s="266">
         <v>0.18</v>
       </c>
@@ -27602,13 +27602,13 @@
       </c>
     </row>
     <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="444" t="s">
+      <c r="A105" s="420" t="s">
         <v>512</v>
       </c>
       <c r="B105" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C105" s="447"/>
+      <c r="C105" s="423"/>
       <c r="D105" s="266">
         <v>0</v>
       </c>
@@ -27617,11 +27617,11 @@
       </c>
     </row>
     <row r="106" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="445"/>
+      <c r="A106" s="421"/>
       <c r="B106" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C106" s="448"/>
+      <c r="C106" s="424"/>
       <c r="D106" s="266">
         <v>0</v>
       </c>
@@ -27630,13 +27630,13 @@
       </c>
     </row>
     <row r="107" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="444" t="s">
+      <c r="A107" s="420" t="s">
         <v>508</v>
       </c>
       <c r="B107" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C107" s="446" t="s">
+      <c r="C107" s="422" t="s">
         <v>515</v>
       </c>
       <c r="D107" s="266">
@@ -27647,11 +27647,11 @@
       </c>
     </row>
     <row r="108" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="445"/>
+      <c r="A108" s="421"/>
       <c r="B108" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C108" s="447"/>
+      <c r="C108" s="423"/>
       <c r="D108" s="266">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -27660,13 +27660,13 @@
       </c>
     </row>
     <row r="109" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="444" t="s">
+      <c r="A109" s="420" t="s">
         <v>512</v>
       </c>
       <c r="B109" s="266" t="s">
         <v>513</v>
       </c>
-      <c r="C109" s="447"/>
+      <c r="C109" s="423"/>
       <c r="D109" s="266">
         <v>0</v>
       </c>
@@ -27675,11 +27675,11 @@
       </c>
     </row>
     <row r="110" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="445"/>
+      <c r="A110" s="421"/>
       <c r="B110" s="266" t="s">
         <v>514</v>
       </c>
-      <c r="C110" s="448"/>
+      <c r="C110" s="424"/>
       <c r="D110" s="266">
         <v>0</v>
       </c>
@@ -29142,6 +29142,22 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="AC25:AE25"/>
+    <mergeCell ref="AC6:AE6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="W32:W34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="L36:L41"/>
+    <mergeCell ref="L42:L45"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="L32:L34"/>
+    <mergeCell ref="M32:M34"/>
+    <mergeCell ref="R32:R34"/>
+    <mergeCell ref="S32:S34"/>
+    <mergeCell ref="T32:T34"/>
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="C107:C110"/>
     <mergeCell ref="A109:A110"/>
@@ -29152,22 +29168,6 @@
     <mergeCell ref="A103:A104"/>
     <mergeCell ref="C103:C106"/>
     <mergeCell ref="A105:A106"/>
-    <mergeCell ref="W32:W34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="L36:L41"/>
-    <mergeCell ref="L42:L45"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="L32:L34"/>
-    <mergeCell ref="M32:M34"/>
-    <mergeCell ref="R32:R34"/>
-    <mergeCell ref="S32:S34"/>
-    <mergeCell ref="T32:T34"/>
-    <mergeCell ref="AC25:AE25"/>
-    <mergeCell ref="AC6:AE6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29930,8 +29930,8 @@
   </sheetPr>
   <dimension ref="A1:AE119"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y33" sqref="Y33:Y72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -30238,7 +30238,7 @@
       </c>
       <c r="X9"/>
       <c r="Y9">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z9">
         <v>1</v>
@@ -30309,7 +30309,7 @@
       </c>
       <c r="X10"/>
       <c r="Y10">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z10">
         <v>1</v>
@@ -30380,7 +30380,7 @@
       </c>
       <c r="X11"/>
       <c r="Y11">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z11">
         <v>1</v>
@@ -30451,7 +30451,7 @@
       </c>
       <c r="X12"/>
       <c r="Y12">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z12">
         <v>1</v>
@@ -30521,7 +30521,7 @@
       </c>
       <c r="X13"/>
       <c r="Y13">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z13">
         <v>1</v>
@@ -30591,7 +30591,7 @@
       </c>
       <c r="X14"/>
       <c r="Y14">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z14">
         <v>1</v>
@@ -30661,7 +30661,7 @@
       </c>
       <c r="X15"/>
       <c r="Y15">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z15">
         <v>1</v>
@@ -30731,7 +30731,7 @@
       </c>
       <c r="X16"/>
       <c r="Y16">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z16">
         <v>1</v>
@@ -30801,7 +30801,7 @@
       </c>
       <c r="X17"/>
       <c r="Y17">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z17">
         <v>1</v>
@@ -30871,7 +30871,7 @@
       </c>
       <c r="X18"/>
       <c r="Y18">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z18">
         <v>1</v>
@@ -30941,7 +30941,7 @@
       </c>
       <c r="X19"/>
       <c r="Y19">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z19">
         <v>1</v>
@@ -31010,7 +31010,7 @@
       </c>
       <c r="X20"/>
       <c r="Y20">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z20">
         <v>1</v>
@@ -31079,7 +31079,7 @@
       </c>
       <c r="X21"/>
       <c r="Y21">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z21">
         <v>1</v>
@@ -31149,7 +31149,7 @@
       </c>
       <c r="X22"/>
       <c r="Y22">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z22">
         <v>1</v>
@@ -31937,7 +31937,7 @@
       </c>
       <c r="X33"/>
       <c r="Y33">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z33">
         <v>1</v>
@@ -32007,7 +32007,7 @@
       </c>
       <c r="X34"/>
       <c r="Y34">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z34">
         <v>1</v>
@@ -32077,7 +32077,7 @@
       </c>
       <c r="X35"/>
       <c r="Y35">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z35">
         <v>1</v>
@@ -32147,7 +32147,7 @@
       </c>
       <c r="X36"/>
       <c r="Y36">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z36">
         <v>1</v>
@@ -32217,7 +32217,7 @@
       </c>
       <c r="X37"/>
       <c r="Y37">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z37">
         <v>1</v>
@@ -32287,7 +32287,7 @@
       </c>
       <c r="X38"/>
       <c r="Y38">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z38">
         <v>1</v>
@@ -32357,7 +32357,7 @@
       </c>
       <c r="X39"/>
       <c r="Y39">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z39">
         <v>1</v>
@@ -32427,7 +32427,7 @@
       </c>
       <c r="X40"/>
       <c r="Y40">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z40">
         <v>1</v>
@@ -32497,7 +32497,7 @@
       </c>
       <c r="X41"/>
       <c r="Y41">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z41">
         <v>1</v>
@@ -32567,7 +32567,7 @@
       </c>
       <c r="X42"/>
       <c r="Y42">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z42">
         <v>1</v>
@@ -32637,7 +32637,7 @@
       </c>
       <c r="X43"/>
       <c r="Y43">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z43">
         <v>1</v>
@@ -32707,7 +32707,7 @@
       </c>
       <c r="X44"/>
       <c r="Y44">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z44">
         <v>1</v>
@@ -32777,7 +32777,7 @@
       </c>
       <c r="X45"/>
       <c r="Y45">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z45">
         <v>1</v>
@@ -32847,7 +32847,7 @@
       </c>
       <c r="X46"/>
       <c r="Y46">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z46">
         <v>1</v>
@@ -32917,7 +32917,7 @@
       </c>
       <c r="X47"/>
       <c r="Y47">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z47">
         <v>1</v>
@@ -32987,7 +32987,7 @@
       </c>
       <c r="X48"/>
       <c r="Y48">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z48">
         <v>1</v>
@@ -33057,7 +33057,7 @@
       </c>
       <c r="X49"/>
       <c r="Y49">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z49">
         <v>1</v>
@@ -33128,7 +33128,7 @@
       </c>
       <c r="X50"/>
       <c r="Y50">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z50">
         <v>1</v>
@@ -33199,7 +33199,7 @@
       </c>
       <c r="X51"/>
       <c r="Y51">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z51">
         <v>1</v>
@@ -33269,7 +33269,7 @@
       </c>
       <c r="X52"/>
       <c r="Y52">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z52">
         <v>1</v>
@@ -33340,7 +33340,7 @@
       </c>
       <c r="X53"/>
       <c r="Y53">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z53">
         <v>1</v>
@@ -33411,7 +33411,7 @@
       </c>
       <c r="X54"/>
       <c r="Y54">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z54">
         <v>1</v>
@@ -33482,7 +33482,7 @@
       </c>
       <c r="X55"/>
       <c r="Y55">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z55">
         <v>1</v>
@@ -33553,7 +33553,7 @@
       </c>
       <c r="X56"/>
       <c r="Y56">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z56">
         <v>1</v>
@@ -33624,7 +33624,7 @@
       </c>
       <c r="X57"/>
       <c r="Y57">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z57">
         <v>1</v>
@@ -33695,7 +33695,7 @@
       </c>
       <c r="X58"/>
       <c r="Y58">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z58">
         <v>1</v>
@@ -33766,7 +33766,7 @@
       </c>
       <c r="X59"/>
       <c r="Y59">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z59">
         <v>1</v>
@@ -33837,7 +33837,7 @@
       </c>
       <c r="X60"/>
       <c r="Y60">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z60">
         <v>1</v>
@@ -33908,7 +33908,7 @@
       </c>
       <c r="X61"/>
       <c r="Y61">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z61">
         <v>1</v>
@@ -33979,7 +33979,7 @@
       </c>
       <c r="X62"/>
       <c r="Y62">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z62">
         <v>1</v>
@@ -34050,7 +34050,7 @@
       </c>
       <c r="X63"/>
       <c r="Y63">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z63">
         <v>1</v>
@@ -34121,7 +34121,7 @@
       </c>
       <c r="X64"/>
       <c r="Y64">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z64">
         <v>1</v>
@@ -34190,7 +34190,7 @@
       </c>
       <c r="X65"/>
       <c r="Y65">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z65">
         <v>1</v>
@@ -34260,7 +34260,7 @@
       </c>
       <c r="X66"/>
       <c r="Y66">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z66">
         <v>1</v>
@@ -34330,7 +34330,7 @@
       </c>
       <c r="X67"/>
       <c r="Y67">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z67">
         <v>1</v>
@@ -34400,7 +34400,7 @@
       </c>
       <c r="X68"/>
       <c r="Y68">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z68">
         <v>1</v>
@@ -34470,7 +34470,7 @@
       </c>
       <c r="X69"/>
       <c r="Y69">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z69">
         <v>1</v>
@@ -34540,7 +34540,7 @@
       </c>
       <c r="X70"/>
       <c r="Y70">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z70">
         <v>1</v>
@@ -34610,7 +34610,7 @@
       </c>
       <c r="X71"/>
       <c r="Y71">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z71">
         <v>1</v>
@@ -34680,7 +34680,7 @@
       </c>
       <c r="X72"/>
       <c r="Y72">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="Z72">
         <v>1</v>
@@ -50006,18 +50006,18 @@
         <f>FORECAST(CR93,CP94:CQ94,CP93:CQ93)</f>
         <v>93</v>
       </c>
-      <c r="DL94" s="436" t="s">
+      <c r="DL94" s="432" t="s">
         <v>762</v>
       </c>
-      <c r="DM94" s="436"/>
-      <c r="DN94" s="436" t="s">
+      <c r="DM94" s="432"/>
+      <c r="DN94" s="432" t="s">
         <v>763</v>
       </c>
-      <c r="DO94" s="436"/>
-      <c r="DP94" s="436" t="s">
+      <c r="DO94" s="432"/>
+      <c r="DP94" s="432" t="s">
         <v>761</v>
       </c>
-      <c r="DQ94" s="436"/>
+      <c r="DQ94" s="432"/>
     </row>
     <row r="95" spans="1:121" x14ac:dyDescent="0.25">
       <c r="BK95" t="s">
@@ -55478,7 +55478,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="18">
         <f ca="1">NOW()</f>
-        <v>45310.469588194443</v>
+        <v>45392.430493055559</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -56302,7 +56302,7 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
         <f ca="1">NOW()</f>
-        <v>45310.469588194443</v>
+        <v>45392.430493055559</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -58989,7 +58989,7 @@
   </sheetPr>
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>

</xml_diff>